<commit_message>
Starting  to input Philippines data
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="435" windowWidth="20370" windowHeight="7410" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
-  <si>
-    <t>program_prop_lowquality</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
   <si>
     <t>parameter</t>
   </si>
@@ -33,21 +27,6 @@
     <t>tb_n_contact</t>
   </si>
   <si>
-    <t>program_prop_vaccination</t>
-  </si>
-  <si>
-    <t>program_prop_detect</t>
-  </si>
-  <si>
-    <t>program_prop_algorithm_sensitivity</t>
-  </si>
-  <si>
-    <t>program_prop_firstline_dst</t>
-  </si>
-  <si>
-    <t>program_prop_secondline_dst</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -63,24 +42,6 @@
     <t>na</t>
   </si>
   <si>
-    <t>program_prop_treatment_success</t>
-  </si>
-  <si>
-    <t>program_prop_treatment_death</t>
-  </si>
-  <si>
-    <t>program_prop_treatment_success_mdr</t>
-  </si>
-  <si>
-    <t>program_prop_treatment_death_mdr</t>
-  </si>
-  <si>
-    <t>program_prop_treatment_success_xdr</t>
-  </si>
-  <si>
-    <t>program_prop_treatment_death_xdr</t>
-  </si>
-  <si>
     <t>scenario_1</t>
   </si>
   <si>
@@ -96,6 +57,12 @@
     <t>time_variant</t>
   </si>
   <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>susceptible_fully</t>
+  </si>
+  <si>
     <t>scenario_3</t>
   </si>
   <si>
@@ -114,7 +81,118 @@
     <t>scenario_8</t>
   </si>
   <si>
-    <t>program_prop_xpert</t>
+    <t>scenario_9</t>
+  </si>
+  <si>
+    <t>scipy</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>explicit</t>
+  </si>
+  <si>
+    <t>runge_kutta</t>
+  </si>
+  <si>
+    <t>scenario_10</t>
+  </si>
+  <si>
+    <t>scenario_11</t>
+  </si>
+  <si>
+    <t>age_unstratified</t>
+  </si>
+  <si>
+    <t>scenario_12</t>
+  </si>
+  <si>
+    <t>econ_cpi</t>
+  </si>
+  <si>
+    <t>without_diabetes</t>
+  </si>
+  <si>
+    <t>with_diabetes</t>
+  </si>
+  <si>
+    <t>program_perc_vaccination</t>
+  </si>
+  <si>
+    <t>program_perc_detect</t>
+  </si>
+  <si>
+    <t>program_perc_ipt</t>
+  </si>
+  <si>
+    <t>program_perc_ipt_age0to5</t>
+  </si>
+  <si>
+    <t>program_perc_ipt_age5to15</t>
+  </si>
+  <si>
+    <t>program_perc_algorithm_sensitivity</t>
+  </si>
+  <si>
+    <t>program_perc_lowquality</t>
+  </si>
+  <si>
+    <t>program_perc_firstline_dst</t>
+  </si>
+  <si>
+    <t>program_perc_secondline_dst</t>
+  </si>
+  <si>
+    <t>program_perc_xpert</t>
+  </si>
+  <si>
+    <t>program_perc_treatment_support</t>
+  </si>
+  <si>
+    <t>program_perc_smearacf</t>
+  </si>
+  <si>
+    <t>program_perc_xpertacf</t>
+  </si>
+  <si>
+    <t>program_perc_treatment_success</t>
+  </si>
+  <si>
+    <t>program_perc_treatment_death</t>
+  </si>
+  <si>
+    <t>program_perc_treatment_success_mdr</t>
+  </si>
+  <si>
+    <t>program_perc_treatment_death_mdr</t>
+  </si>
+  <si>
+    <t>program_perc_treatment_success_xdr</t>
+  </si>
+  <si>
+    <t>program_perc_treatment_death_xdr</t>
+  </si>
+  <si>
+    <t>epi_rr_diabetes</t>
+  </si>
+  <si>
+    <t>freeze_times</t>
+  </si>
+  <si>
+    <t>program_perc_decentralisation</t>
+  </si>
+  <si>
+    <t>scenario_13</t>
+  </si>
+  <si>
+    <t>scenario_14</t>
+  </si>
+  <si>
+    <t>comorb_perc_diabetes</t>
+  </si>
+  <si>
+    <t>age_breakpoints</t>
   </si>
 </sst>
 </file>
@@ -124,7 +202,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,8 +287,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +383,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,7 +496,9 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1062,7 +1168,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1099,19 +1205,41 @@
     <xf numFmtId="0" fontId="6" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="14" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="14" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="14" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -1785,25 +1913,11 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="country_constants"/>
-      <sheetName val="time_variants"/>
-      <sheetName val="dropdown_lists"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2096,56 +2210,141 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="29"/>
+    <col min="1" max="1" width="51.5703125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="37" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="29"/>
+    <col min="6" max="6" width="13.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="41"/>
+      <c r="B2" s="59">
+        <v>7.93</v>
+      </c>
+      <c r="F2" s="59">
+        <v>7.85</v>
+      </c>
+      <c r="G2" s="59">
+        <v>7.85</v>
+      </c>
+      <c r="H2">
+        <v>6.2</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="43">
-        <v>22</v>
-      </c>
-      <c r="C2" s="44"/>
+    <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="60">
+        <v>0.22</v>
+      </c>
+      <c r="F3" s="60">
+        <v>0.22</v>
+      </c>
+      <c r="G3" s="60">
+        <v>0.22</v>
+      </c>
+      <c r="H3">
+        <v>0.2</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="38">
-        <v>0.3</v>
-      </c>
-      <c r="C3" s="39"/>
+    <row r="4" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="61">
+        <v>1865</v>
+      </c>
+      <c r="F4" s="61">
+        <v>1865</v>
+      </c>
+      <c r="G4" s="61">
+        <v>1865</v>
+      </c>
+      <c r="H4">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="62">
+        <v>190000</v>
+      </c>
+      <c r="F5" s="62">
+        <v>190000</v>
+      </c>
+      <c r="G5" s="62">
+        <v>190000</v>
+      </c>
+      <c r="H5">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="37">
+        <v>5</v>
+      </c>
+      <c r="C6" s="29">
+        <v>15</v>
+      </c>
+      <c r="D6" s="29">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+  <dataValidations count="5">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 F4:G4">
+      <formula1>-10000</formula1>
+      <formula2>10000</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5 F5:G5">
+      <formula1>0</formula1>
+      <formula2>10000000000</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 F2:G2">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 F3:G3">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age unstratified" prompt="Some values you can replace the ones to the left with if you want a manual calibration for the model without age stratification." sqref="H1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2157,556 +2356,1480 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:CC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q9" sqref="Q9"/>
+      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56" style="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11" style="2" customWidth="1"/>
-    <col min="5" max="7" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.140625" style="1" customWidth="1"/>
-    <col min="15" max="17" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8" style="1" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="25" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="11" style="50" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="21" width="7.42578125" style="1" customWidth="1"/>
+    <col min="22" max="27" width="7.28515625" style="1" customWidth="1"/>
+    <col min="28" max="29" width="7.42578125" style="1" customWidth="1"/>
+    <col min="30" max="31" width="7.140625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="36" width="7.42578125" style="1" customWidth="1"/>
+    <col min="37" max="37" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="41" width="7.42578125" style="1" customWidth="1"/>
+    <col min="42" max="42" width="7.5703125" style="1" customWidth="1"/>
+    <col min="43" max="53" width="7" style="1" customWidth="1"/>
+    <col min="54" max="55" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="57" width="7.85546875" style="1" customWidth="1"/>
+    <col min="58" max="58" width="14" style="1" customWidth="1"/>
+    <col min="59" max="65" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="66" max="70" width="14.42578125" style="1" customWidth="1"/>
+    <col min="71" max="71" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="72" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:71" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="E1" s="5">
+        <v>1920</v>
+      </c>
+      <c r="F1" s="5">
         <v>1930</v>
       </c>
-      <c r="F1" s="5">
+      <c r="G1" s="5">
+        <v>1940</v>
+      </c>
+      <c r="H1" s="5">
         <v>1950</v>
       </c>
-      <c r="G1" s="5">
+      <c r="I1" s="5">
         <v>1955</v>
       </c>
-      <c r="H1" s="5">
+      <c r="J1" s="5">
         <v>1960</v>
       </c>
-      <c r="I1" s="5">
+      <c r="K1" s="5">
         <v>1965</v>
       </c>
-      <c r="J1" s="5">
+      <c r="L1" s="5">
+        <v>1970</v>
+      </c>
+      <c r="M1" s="5">
+        <v>1971</v>
+      </c>
+      <c r="N1" s="5">
+        <v>1972</v>
+      </c>
+      <c r="O1" s="5">
+        <v>1973</v>
+      </c>
+      <c r="P1" s="5">
+        <v>1974</v>
+      </c>
+      <c r="Q1" s="5">
         <v>1975</v>
       </c>
-      <c r="K1" s="5">
+      <c r="R1" s="5">
+        <v>1976</v>
+      </c>
+      <c r="S1" s="5">
+        <v>1977</v>
+      </c>
+      <c r="T1" s="5">
+        <v>1978</v>
+      </c>
+      <c r="U1" s="5">
+        <v>1979</v>
+      </c>
+      <c r="V1" s="5">
         <v>1980</v>
       </c>
-      <c r="L1" s="5">
+      <c r="W1" s="5">
+        <v>1981</v>
+      </c>
+      <c r="X1" s="5">
         <v>1982</v>
       </c>
-      <c r="M1" s="5">
+      <c r="Y1" s="5">
+        <v>1983</v>
+      </c>
+      <c r="Z1" s="5">
+        <v>1984</v>
+      </c>
+      <c r="AA1" s="5">
+        <v>1985</v>
+      </c>
+      <c r="AB1" s="5">
         <v>1986</v>
       </c>
-      <c r="N1" s="5">
+      <c r="AC1" s="5">
+        <v>1987</v>
+      </c>
+      <c r="AD1" s="5">
         <v>1988</v>
       </c>
-      <c r="O1" s="5">
+      <c r="AE1" s="5">
+        <v>1989</v>
+      </c>
+      <c r="AF1" s="5">
         <v>1990</v>
       </c>
-      <c r="P1" s="5">
+      <c r="AG1" s="5">
+        <v>1991</v>
+      </c>
+      <c r="AH1" s="5">
+        <v>1992</v>
+      </c>
+      <c r="AI1" s="5">
+        <v>1993</v>
+      </c>
+      <c r="AJ1" s="5">
+        <v>1994</v>
+      </c>
+      <c r="AK1" s="5">
         <v>1995</v>
       </c>
-      <c r="Q1" s="5">
+      <c r="AL1" s="5">
+        <v>1996</v>
+      </c>
+      <c r="AM1" s="5">
+        <v>1997</v>
+      </c>
+      <c r="AN1" s="5">
+        <v>1998</v>
+      </c>
+      <c r="AO1" s="5">
+        <v>1999</v>
+      </c>
+      <c r="AP1" s="5">
         <v>2000</v>
       </c>
-      <c r="R1" s="5">
+      <c r="AQ1" s="5">
         <v>2001</v>
       </c>
-      <c r="S1" s="5">
+      <c r="AR1" s="5">
+        <v>2002</v>
+      </c>
+      <c r="AS1" s="5">
+        <v>2003</v>
+      </c>
+      <c r="AT1" s="5">
+        <v>2004</v>
+      </c>
+      <c r="AU1" s="5">
+        <v>2005</v>
+      </c>
+      <c r="AV1" s="5">
+        <v>2006</v>
+      </c>
+      <c r="AW1" s="5">
+        <v>2007</v>
+      </c>
+      <c r="AX1" s="5">
+        <v>2008</v>
+      </c>
+      <c r="AY1" s="5">
+        <v>2009</v>
+      </c>
+      <c r="AZ1" s="5">
+        <v>2010</v>
+      </c>
+      <c r="BA1" s="5">
+        <v>2011</v>
+      </c>
+      <c r="BB1" s="5">
+        <v>2012</v>
+      </c>
+      <c r="BC1" s="5">
+        <v>2013</v>
+      </c>
+      <c r="BD1" s="5">
         <v>2014</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="BE1" s="5">
+        <v>2015</v>
+      </c>
+      <c r="BF1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="BG1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="BI1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="BJ1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="BK1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="BL1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="BM1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="BN1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="BO1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="BP1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="BQ1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="BR1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="BS1" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:71" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="43"/>
+      <c r="H2" s="7">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7">
         <v>25</v>
       </c>
-      <c r="W1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA1" s="5" t="s">
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="25"/>
+      <c r="AF2" s="25"/>
+      <c r="AG2" s="25"/>
+      <c r="AH2" s="25"/>
+      <c r="AI2" s="25"/>
+      <c r="AJ2" s="25"/>
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="25"/>
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="25"/>
+      <c r="AQ2" s="25"/>
+      <c r="AR2" s="25"/>
+      <c r="AS2" s="25"/>
+      <c r="AT2" s="25"/>
+      <c r="AU2" s="25"/>
+      <c r="AV2" s="25"/>
+      <c r="AW2" s="25"/>
+      <c r="AX2" s="25"/>
+      <c r="AY2" s="25"/>
+      <c r="AZ2" s="25"/>
+      <c r="BA2" s="25"/>
+      <c r="BB2" s="25"/>
+      <c r="BC2" s="25"/>
+      <c r="BD2" s="25"/>
+      <c r="BE2" s="25"/>
+      <c r="BK2" s="7">
+        <v>100</v>
+      </c>
+      <c r="BS2" s="7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:71" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="8">
+        <v>5</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="44"/>
+      <c r="F3" s="9">
+        <v>0</v>
+      </c>
+      <c r="K3" s="9">
+        <v>10</v>
+      </c>
+      <c r="AF3" s="26">
+        <v>40</v>
+      </c>
+      <c r="AG3" s="26">
+        <v>40</v>
+      </c>
+      <c r="AH3" s="26">
+        <v>40</v>
+      </c>
+      <c r="AI3" s="26">
+        <v>40</v>
+      </c>
+      <c r="AJ3" s="26">
+        <v>40</v>
+      </c>
+      <c r="AK3" s="26">
+        <v>40</v>
+      </c>
+      <c r="AL3" s="26">
+        <v>40</v>
+      </c>
+      <c r="AM3" s="26">
+        <v>40</v>
+      </c>
+      <c r="AN3" s="26">
+        <v>40</v>
+      </c>
+      <c r="AO3" s="26">
+        <v>40</v>
+      </c>
+      <c r="AP3" s="26">
+        <v>40</v>
+      </c>
+      <c r="AQ3" s="26">
+        <v>40</v>
+      </c>
+      <c r="AR3" s="26">
+        <v>40</v>
+      </c>
+      <c r="AS3" s="26">
+        <v>40</v>
+      </c>
+      <c r="AT3" s="26">
+        <v>40</v>
+      </c>
+      <c r="AU3" s="26">
+        <v>40</v>
+      </c>
+      <c r="AV3" s="26">
+        <v>10</v>
+      </c>
+      <c r="AW3" s="26">
+        <v>10</v>
+      </c>
+      <c r="AX3" s="26">
+        <v>10</v>
+      </c>
+      <c r="AY3" s="26"/>
+      <c r="AZ3" s="26">
         <v>30</v>
       </c>
+      <c r="BA3" s="26">
+        <v>30</v>
+      </c>
+      <c r="BB3" s="26"/>
+      <c r="BC3" s="26"/>
+      <c r="BD3" s="26">
+        <v>56</v>
+      </c>
+      <c r="BE3" s="26"/>
+      <c r="BH3" s="9">
+        <v>60</v>
+      </c>
+      <c r="BI3" s="9">
+        <v>75</v>
+      </c>
     </row>
-    <row r="2" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+    <row r="4" spans="1:71" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="44"/>
+      <c r="BD4" s="9">
+        <v>0</v>
+      </c>
+      <c r="BM4" s="9">
+        <v>50</v>
+      </c>
+      <c r="BS4" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:71" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="44"/>
+      <c r="BA5" s="9">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="9">
+        <v>7</v>
+      </c>
+      <c r="BD5" s="9">
+        <v>23.6</v>
+      </c>
+      <c r="BN5" s="9">
+        <v>75</v>
+      </c>
+      <c r="BS5" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:71" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="44"/>
+      <c r="BD6" s="9">
+        <v>0</v>
+      </c>
+      <c r="BN6" s="9">
+        <v>40</v>
+      </c>
+      <c r="BS6" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="7">
-        <v>0</v>
-      </c>
-      <c r="H2" s="7">
-        <v>25</v>
-      </c>
-      <c r="J2" s="7">
-        <v>40</v>
-      </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="Z2" s="7">
-        <v>100</v>
-      </c>
-      <c r="AA2" s="7">
-        <v>100</v>
+      <c r="C7" s="10">
+        <v>1</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="45"/>
+      <c r="F7" s="11">
+        <v>70</v>
+      </c>
+      <c r="J7" s="11">
+        <v>80</v>
+      </c>
+      <c r="AD7" s="11">
+        <v>82</v>
+      </c>
+      <c r="AQ7" s="11">
+        <v>84</v>
+      </c>
+      <c r="BC7" s="11">
+        <v>85</v>
+      </c>
+      <c r="BJ7" s="11">
+        <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="8">
-        <v>10</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="9">
-        <v>0</v>
-      </c>
-      <c r="I3" s="9">
-        <v>10</v>
-      </c>
-      <c r="L3" s="9">
+    <row r="8" spans="1:71" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="12">
+        <v>1</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="46"/>
+      <c r="H8" s="13">
         <v>30</v>
-      </c>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26">
-        <v>75</v>
-      </c>
-      <c r="V3" s="9">
-        <v>85</v>
-      </c>
-      <c r="W3" s="9">
-        <v>90</v>
-      </c>
-      <c r="AA3" s="9">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="10">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="11">
-        <v>70</v>
-      </c>
-      <c r="H4" s="11">
-        <v>80</v>
-      </c>
-      <c r="N4" s="11">
-        <v>82</v>
-      </c>
-      <c r="R4" s="11">
-        <v>84</v>
-      </c>
-      <c r="S4" s="11">
-        <v>85</v>
-      </c>
-      <c r="Y4" s="11">
-        <v>90</v>
-      </c>
-      <c r="AA4" s="11">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="12">
-        <v>1</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="13">
-        <v>30</v>
-      </c>
-      <c r="I5" s="13">
-        <v>35</v>
-      </c>
-      <c r="O5" s="13">
-        <v>40</v>
-      </c>
-      <c r="X5" s="13">
-        <v>20</v>
-      </c>
-      <c r="AA5" s="13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="14">
-        <v>1</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="K6" s="15">
-        <v>30</v>
-      </c>
-      <c r="O6" s="15">
-        <v>40</v>
-      </c>
-      <c r="Q6" s="15">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="14">
-        <v>1</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="15">
-        <v>7</v>
-      </c>
-      <c r="P7" s="15">
-        <v>50</v>
-      </c>
-      <c r="Q7" s="15">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="12">
-        <v>1</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="13">
-        <v>0</v>
       </c>
       <c r="K8" s="13">
         <v>40</v>
       </c>
-      <c r="M8" s="13">
+      <c r="AF8" s="13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="47"/>
+      <c r="V9" s="15">
+        <v>30</v>
+      </c>
+      <c r="AF9" s="15">
+        <v>40</v>
+      </c>
+      <c r="AP9" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="14">
+        <v>1</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="47"/>
+      <c r="I10" s="15">
+        <v>7</v>
+      </c>
+      <c r="AK10" s="15">
+        <v>50</v>
+      </c>
+      <c r="AP10" s="15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:71" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="12">
+        <v>1</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="46"/>
+      <c r="I11" s="13">
+        <v>0</v>
+      </c>
+      <c r="V11" s="13">
+        <v>40</v>
+      </c>
+      <c r="AB11" s="13">
         <v>65</v>
       </c>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
-      <c r="T8" s="13">
-        <v>91.1</v>
-      </c>
-      <c r="U8" s="13">
-        <v>96</v>
-      </c>
-      <c r="AA8" s="13">
-        <v>96</v>
+      <c r="AK11" s="27"/>
+      <c r="AL11" s="27"/>
+      <c r="AM11" s="27"/>
+      <c r="AN11" s="27"/>
+      <c r="AO11" s="27"/>
+      <c r="AP11" s="27"/>
+      <c r="AQ11" s="27"/>
+      <c r="AR11" s="27"/>
+      <c r="AS11" s="27"/>
+      <c r="AT11" s="27"/>
+      <c r="AU11" s="27"/>
+      <c r="AV11" s="27"/>
+      <c r="AW11" s="27"/>
+      <c r="AX11" s="27"/>
+      <c r="AY11" s="27"/>
+      <c r="AZ11" s="27"/>
+      <c r="BA11" s="27"/>
+      <c r="BB11" s="27">
+        <v>93</v>
+      </c>
+      <c r="BC11" s="27">
+        <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:27" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+    <row r="12" spans="1:71" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="12">
+        <v>3</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="46"/>
+      <c r="I12" s="13">
+        <v>0</v>
+      </c>
+      <c r="V12" s="13">
+        <v>10</v>
+      </c>
+      <c r="AB12" s="13">
+        <v>8</v>
+      </c>
+      <c r="AK12" s="27"/>
+      <c r="AL12" s="27"/>
+      <c r="AM12" s="27"/>
+      <c r="AN12" s="27"/>
+      <c r="AO12" s="27"/>
+      <c r="AP12" s="27"/>
+      <c r="AQ12" s="27"/>
+      <c r="AR12" s="27"/>
+      <c r="AS12" s="27"/>
+      <c r="AT12" s="27"/>
+      <c r="AU12" s="27"/>
+      <c r="AV12" s="27"/>
+      <c r="AW12" s="27"/>
+      <c r="AX12" s="27"/>
+      <c r="AY12" s="27"/>
+      <c r="AZ12" s="27"/>
+      <c r="BA12" s="27"/>
+      <c r="BB12" s="27"/>
+      <c r="BC12" s="27"/>
+      <c r="BD12" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:71" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="23">
+        <v>1</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="48"/>
+      <c r="I13" s="24">
+        <v>0</v>
+      </c>
+      <c r="V13" s="24">
         <v>15</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="12">
-        <v>1</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="13">
+      <c r="AB13" s="24">
+        <v>30</v>
+      </c>
+      <c r="AK13" s="28"/>
+      <c r="AL13" s="28"/>
+      <c r="AM13" s="28"/>
+      <c r="AN13" s="28"/>
+      <c r="AO13" s="28"/>
+      <c r="AP13" s="28"/>
+      <c r="AQ13" s="28"/>
+      <c r="AR13" s="28"/>
+      <c r="AS13" s="28"/>
+      <c r="AT13" s="28"/>
+      <c r="AU13" s="28"/>
+      <c r="AV13" s="28"/>
+      <c r="AW13" s="28"/>
+      <c r="AX13" s="28"/>
+      <c r="AY13" s="28"/>
+      <c r="AZ13" s="28"/>
+      <c r="BA13" s="28"/>
+      <c r="BB13" s="28"/>
+      <c r="BC13" s="28"/>
+      <c r="BD13" s="24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:71" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="23">
+        <v>1</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="48"/>
+      <c r="I14" s="24">
         <v>0</v>
       </c>
-      <c r="K9" s="13">
-        <v>12</v>
-      </c>
-      <c r="M9" s="13">
+      <c r="V14" s="24">
+        <v>55</v>
+      </c>
+      <c r="AB14" s="24">
+        <v>50</v>
+      </c>
+      <c r="AK14" s="28"/>
+      <c r="AL14" s="28"/>
+      <c r="AM14" s="28"/>
+      <c r="AN14" s="28"/>
+      <c r="AO14" s="28"/>
+      <c r="AP14" s="28"/>
+      <c r="AQ14" s="28"/>
+      <c r="AR14" s="28"/>
+      <c r="AS14" s="28"/>
+      <c r="AT14" s="28"/>
+      <c r="AU14" s="28"/>
+      <c r="AV14" s="28"/>
+      <c r="AW14" s="28"/>
+      <c r="AX14" s="28"/>
+      <c r="AY14" s="28"/>
+      <c r="AZ14" s="28"/>
+      <c r="BA14" s="28"/>
+      <c r="BB14" s="28"/>
+      <c r="BC14" s="28"/>
+      <c r="BD14" s="24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:71" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="44"/>
+      <c r="I15" s="9">
+        <v>0</v>
+      </c>
+      <c r="V15" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB15" s="9">
+        <v>15</v>
+      </c>
+      <c r="AK15" s="26"/>
+      <c r="AL15" s="26"/>
+      <c r="AM15" s="26"/>
+      <c r="AN15" s="26"/>
+      <c r="AO15" s="26"/>
+      <c r="AP15" s="26"/>
+      <c r="AQ15" s="26"/>
+      <c r="AR15" s="26"/>
+      <c r="AS15" s="26"/>
+      <c r="AT15" s="26"/>
+      <c r="AU15" s="26"/>
+      <c r="AV15" s="26"/>
+      <c r="AW15" s="26"/>
+      <c r="AX15" s="26"/>
+      <c r="AY15" s="26"/>
+      <c r="AZ15" s="26"/>
+      <c r="BA15" s="26"/>
+      <c r="BB15" s="26"/>
+      <c r="BC15" s="26"/>
+      <c r="BD15" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:71" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="44"/>
+      <c r="I16" s="9">
+        <v>0</v>
+      </c>
+      <c r="V16" s="9">
+        <v>65</v>
+      </c>
+      <c r="AB16" s="9">
+        <v>62</v>
+      </c>
+      <c r="AK16" s="26"/>
+      <c r="AL16" s="26"/>
+      <c r="AM16" s="26"/>
+      <c r="AN16" s="26"/>
+      <c r="AO16" s="26"/>
+      <c r="AP16" s="26"/>
+      <c r="AQ16" s="26"/>
+      <c r="AR16" s="26"/>
+      <c r="AS16" s="26"/>
+      <c r="AT16" s="26"/>
+      <c r="AU16" s="26"/>
+      <c r="AV16" s="26"/>
+      <c r="AW16" s="26"/>
+      <c r="AX16" s="26"/>
+      <c r="AY16" s="26"/>
+      <c r="AZ16" s="26"/>
+      <c r="BA16" s="26"/>
+      <c r="BB16" s="26"/>
+      <c r="BC16" s="26"/>
+      <c r="BD16" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:81" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="33">
+        <v>1</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="49"/>
+      <c r="AK17" s="35"/>
+      <c r="AL17" s="35"/>
+      <c r="AM17" s="35"/>
+      <c r="AN17" s="35"/>
+      <c r="AO17" s="35"/>
+      <c r="AP17" s="35"/>
+      <c r="AQ17" s="35"/>
+      <c r="AR17" s="35"/>
+      <c r="AS17" s="35"/>
+      <c r="AT17" s="35"/>
+      <c r="AU17" s="35"/>
+      <c r="AV17" s="35"/>
+      <c r="AW17" s="35"/>
+      <c r="AX17" s="35"/>
+      <c r="AY17" s="35"/>
+      <c r="AZ17" s="35"/>
+      <c r="BA17" s="35"/>
+      <c r="BB17" s="35"/>
+      <c r="BC17" s="35"/>
+      <c r="BD17" s="34">
+        <v>0</v>
+      </c>
+      <c r="BL17" s="34">
+        <v>100</v>
+      </c>
+      <c r="BS17" s="34">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:81" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="14">
+        <v>1</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="47"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="42"/>
+      <c r="R18" s="42"/>
+      <c r="S18" s="42"/>
+      <c r="T18" s="42"/>
+      <c r="U18" s="42"/>
+      <c r="V18" s="42"/>
+      <c r="W18" s="42"/>
+      <c r="X18" s="42"/>
+      <c r="Y18" s="42"/>
+      <c r="Z18" s="42"/>
+      <c r="AA18" s="42"/>
+      <c r="AB18" s="42"/>
+      <c r="AC18" s="42"/>
+      <c r="AD18" s="42"/>
+      <c r="AE18" s="42"/>
+      <c r="AF18" s="42"/>
+      <c r="AG18" s="42"/>
+      <c r="AH18" s="42"/>
+      <c r="AI18" s="42"/>
+      <c r="AJ18" s="42"/>
+      <c r="AK18" s="42"/>
+      <c r="AL18" s="42"/>
+      <c r="AM18" s="42"/>
+      <c r="AN18" s="42"/>
+      <c r="AO18" s="42"/>
+      <c r="AP18" s="42"/>
+      <c r="AQ18" s="42"/>
+      <c r="AR18" s="42"/>
+      <c r="AS18" s="42"/>
+      <c r="AT18" s="42"/>
+      <c r="AU18" s="42"/>
+      <c r="AV18" s="42"/>
+      <c r="AW18" s="42"/>
+      <c r="AX18" s="42"/>
+      <c r="AY18" s="42"/>
+      <c r="AZ18" s="42"/>
+      <c r="BA18" s="42"/>
+      <c r="BB18" s="42"/>
+      <c r="BC18" s="42"/>
+      <c r="BD18" s="42">
+        <v>0</v>
+      </c>
+      <c r="BE18" s="42"/>
+      <c r="BF18" s="42">
+        <v>100</v>
+      </c>
+      <c r="BG18" s="42"/>
+      <c r="BH18" s="42"/>
+      <c r="BI18" s="42"/>
+      <c r="BJ18" s="42"/>
+      <c r="BK18" s="42"/>
+      <c r="BL18" s="42"/>
+      <c r="BM18" s="42"/>
+      <c r="BN18" s="42"/>
+      <c r="BO18" s="42"/>
+      <c r="BP18" s="42"/>
+      <c r="BQ18" s="64"/>
+      <c r="BR18" s="64"/>
+      <c r="BS18" s="42"/>
+      <c r="BT18" s="42"/>
+      <c r="BU18" s="42"/>
+      <c r="BV18" s="42"/>
+      <c r="BW18" s="42"/>
+      <c r="BX18" s="42"/>
+      <c r="BY18" s="42"/>
+      <c r="BZ18" s="42"/>
+      <c r="CA18" s="42"/>
+      <c r="CB18" s="42"/>
+      <c r="CC18" s="42"/>
+    </row>
+    <row r="19" spans="1:81" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="14">
+        <v>1</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="47">
+        <v>0</v>
+      </c>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="42"/>
+      <c r="S19" s="42"/>
+      <c r="T19" s="42"/>
+      <c r="U19" s="42"/>
+      <c r="V19" s="42"/>
+      <c r="W19" s="42"/>
+      <c r="X19" s="42"/>
+      <c r="Y19" s="42"/>
+      <c r="Z19" s="42"/>
+      <c r="AA19" s="42"/>
+      <c r="AB19" s="42"/>
+      <c r="AC19" s="42"/>
+      <c r="AD19" s="42"/>
+      <c r="AE19" s="42"/>
+      <c r="AF19" s="42"/>
+      <c r="AG19" s="42"/>
+      <c r="AH19" s="42"/>
+      <c r="AI19" s="42"/>
+      <c r="AJ19" s="42"/>
+      <c r="AK19" s="42"/>
+      <c r="AL19" s="42"/>
+      <c r="AM19" s="42"/>
+      <c r="AN19" s="42"/>
+      <c r="AO19" s="42"/>
+      <c r="AP19" s="42"/>
+      <c r="AQ19" s="42"/>
+      <c r="AR19" s="42"/>
+      <c r="AS19" s="42"/>
+      <c r="AT19" s="42"/>
+      <c r="AU19" s="42"/>
+      <c r="AV19" s="42"/>
+      <c r="AW19" s="42"/>
+      <c r="AX19" s="42"/>
+      <c r="AY19" s="42"/>
+      <c r="AZ19" s="42"/>
+      <c r="BA19" s="42"/>
+      <c r="BB19" s="42"/>
+      <c r="BC19" s="42"/>
+      <c r="BD19" s="42">
+        <v>0</v>
+      </c>
+      <c r="BE19" s="42"/>
+      <c r="BF19" s="42"/>
+      <c r="BG19" s="42"/>
+      <c r="BH19" s="42"/>
+      <c r="BI19" s="42"/>
+      <c r="BJ19" s="42"/>
+      <c r="BK19" s="42"/>
+      <c r="BL19" s="42"/>
+      <c r="BM19" s="42"/>
+      <c r="BN19" s="42"/>
+      <c r="BO19" s="42"/>
+      <c r="BP19" s="42"/>
+      <c r="BQ19" s="64">
+        <v>50</v>
+      </c>
+      <c r="BR19" s="64">
+        <v>75</v>
+      </c>
+      <c r="BS19" s="42"/>
+      <c r="BT19" s="42"/>
+      <c r="BU19" s="42"/>
+      <c r="BV19" s="42"/>
+      <c r="BW19" s="42"/>
+      <c r="BX19" s="42"/>
+      <c r="BY19" s="42"/>
+      <c r="BZ19" s="42"/>
+      <c r="CA19" s="42"/>
+      <c r="CB19" s="42"/>
+      <c r="CC19" s="42"/>
+    </row>
+    <row r="20" spans="1:81" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="52">
+        <v>1</v>
+      </c>
+      <c r="D20" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="53"/>
+      <c r="BD20" s="54">
+        <v>0</v>
+      </c>
+      <c r="BO20" s="54">
+        <v>50</v>
+      </c>
+      <c r="BS20" s="54">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:81" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="52">
+        <v>1</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="53"/>
+      <c r="BD21" s="54">
+        <v>0</v>
+      </c>
+      <c r="BP21" s="54">
+        <v>50</v>
+      </c>
+      <c r="BS21" s="54">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:81" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="56">
+        <v>1</v>
+      </c>
+      <c r="D22" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="57">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="F22" s="58">
+        <v>4.84</v>
+      </c>
+      <c r="G22" s="58">
+        <v>5.44</v>
+      </c>
+      <c r="H22" s="58">
+        <v>6.11</v>
+      </c>
+      <c r="I22" s="58">
+        <v>6.86</v>
+      </c>
+      <c r="J22" s="58">
+        <v>7.7</v>
+      </c>
+      <c r="K22" s="58">
+        <v>8.68</v>
+      </c>
+      <c r="L22" s="58">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="M22" s="58">
+        <v>9.41</v>
+      </c>
+      <c r="N22" s="58">
+        <v>11.48</v>
+      </c>
+      <c r="O22" s="58">
+        <v>12.75</v>
+      </c>
+      <c r="P22" s="58">
+        <v>14.6</v>
+      </c>
+      <c r="Q22" s="58">
+        <v>16.5</v>
+      </c>
+      <c r="R22" s="58">
+        <v>18.38</v>
+      </c>
+      <c r="S22" s="58">
+        <v>19.670000000000002</v>
+      </c>
+      <c r="T22" s="58">
+        <v>20.87</v>
+      </c>
+      <c r="U22" s="58">
+        <v>22.5</v>
+      </c>
+      <c r="V22" s="58">
+        <v>25.9</v>
+      </c>
+      <c r="W22" s="58">
+        <v>28.8</v>
+      </c>
+      <c r="X22" s="58">
+        <v>30.8</v>
+      </c>
+      <c r="Y22" s="58">
+        <v>32.9</v>
+      </c>
+      <c r="Z22" s="58">
+        <v>34.6</v>
+      </c>
+      <c r="AA22" s="58">
+        <v>36.1</v>
+      </c>
+      <c r="AB22" s="58">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="AC22" s="58">
+        <v>38.9</v>
+      </c>
+      <c r="AD22" s="58">
+        <v>43.4</v>
+      </c>
+      <c r="AE22" s="58">
+        <v>46.1</v>
+      </c>
+      <c r="AF22" s="58">
+        <v>49.9</v>
+      </c>
+      <c r="AG22" s="58">
+        <v>53.1</v>
+      </c>
+      <c r="AH22" s="58">
+        <v>55.7</v>
+      </c>
+      <c r="AI22" s="58">
+        <v>58.6</v>
+      </c>
+      <c r="AJ22" s="58">
+        <v>59.1</v>
+      </c>
+      <c r="AK22" s="58">
+        <v>60.4</v>
+      </c>
+      <c r="AL22" s="58">
+        <v>62.2</v>
+      </c>
+      <c r="AM22" s="58">
+        <v>64.3</v>
+      </c>
+      <c r="AN22" s="58">
+        <v>68</v>
+      </c>
+      <c r="AO22" s="58">
+        <v>69.3</v>
+      </c>
+      <c r="AP22" s="58">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="AQ22" s="58">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="AR22" s="58">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="AS22" s="58">
+        <v>76.7</v>
+      </c>
+      <c r="AT22" s="58">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="AU22" s="58">
+        <v>80.8</v>
+      </c>
+      <c r="AV22" s="58">
+        <v>82.8</v>
+      </c>
+      <c r="AW22" s="58">
+        <v>86.7</v>
+      </c>
+      <c r="AX22" s="58">
+        <v>93.4</v>
+      </c>
+      <c r="AY22" s="58">
+        <v>96.5</v>
+      </c>
+      <c r="AZ22" s="58">
+        <v>100</v>
+      </c>
+      <c r="BA22" s="58">
+        <v>107.3</v>
+      </c>
+      <c r="BB22" s="58">
+        <v>110.9</v>
+      </c>
+      <c r="BC22" s="58">
+        <v>114.2</v>
+      </c>
+      <c r="BD22" s="58">
+        <v>114.8</v>
+      </c>
+      <c r="BE22" s="58">
+        <v>116.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:81" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="14">
+        <v>1</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="47">
+        <v>1</v>
+      </c>
+      <c r="F23" s="15">
+        <v>1</v>
+      </c>
+      <c r="G23" s="15">
+        <v>1</v>
+      </c>
+      <c r="H23" s="15">
+        <v>1</v>
+      </c>
+      <c r="I23" s="15">
+        <v>1</v>
+      </c>
+      <c r="J23" s="15">
+        <v>1</v>
+      </c>
+      <c r="K23" s="15">
+        <v>1</v>
+      </c>
+      <c r="L23" s="15">
+        <v>1</v>
+      </c>
+      <c r="M23" s="15">
+        <v>1</v>
+      </c>
+      <c r="N23" s="15">
+        <v>1</v>
+      </c>
+      <c r="O23" s="15">
+        <v>1</v>
+      </c>
+      <c r="P23" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="15">
+        <v>1</v>
+      </c>
+      <c r="R23" s="15">
+        <v>1</v>
+      </c>
+      <c r="S23" s="15">
+        <v>1</v>
+      </c>
+      <c r="T23" s="15">
+        <v>1</v>
+      </c>
+      <c r="U23" s="15">
+        <v>1</v>
+      </c>
+      <c r="V23" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="BA23" s="15">
+        <v>3.11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:81" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="63"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="49"/>
+      <c r="BG24" s="34">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="25" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="50">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="1">
         <v>10</v>
       </c>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
-      <c r="T9" s="13">
-        <v>1.6</v>
-      </c>
-      <c r="U9" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="AA9" s="13">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="23">
-        <v>1</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="24">
-        <v>0</v>
-      </c>
-      <c r="K10" s="24">
-        <v>15</v>
-      </c>
-      <c r="M10" s="24">
-        <v>30</v>
-      </c>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="24">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="23">
-        <v>1</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="24">
-        <v>0</v>
-      </c>
-      <c r="K11" s="24">
-        <v>55</v>
-      </c>
-      <c r="M11" s="24">
-        <v>50</v>
-      </c>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="24">
+      <c r="AT25" s="1">
         <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="8">
-        <v>1</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="9">
-        <v>0</v>
-      </c>
-      <c r="K12" s="9">
-        <v>5</v>
-      </c>
-      <c r="M12" s="9">
-        <v>15</v>
-      </c>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="9">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="8">
-        <v>1</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="9">
-        <v>0</v>
-      </c>
-      <c r="K13" s="9">
-        <v>65</v>
-      </c>
-      <c r="M13" s="9">
-        <v>62</v>
-      </c>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="26"/>
-      <c r="S13" s="9">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="33">
-        <v>1</v>
-      </c>
-      <c r="D14" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="34">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations xWindow="343" yWindow="238" count="4">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T14:U14">
+  <dataValidations xWindow="382" yWindow="552" count="5">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF17:BG17 F4:BG6">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:D1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:BG16 F17:BE17 F2:BG3">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E14:S14 E2:U13">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C23 C25:C1048576">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B24:D24"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="343" yWindow="238" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B13</xm:sqref>
+          <xm:sqref>B2:B17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D15:D1048576 D2:D13</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]dropdown_lists!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B14</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
-          <x14:formula1>
-            <xm:f>[1]dropdown_lists!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D14</xm:sqref>
+          <xm:sqref>D2:D23 D25:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2719,27 +3842,45 @@
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>
-  <dimension ref="A2:A4"/>
+  <dimension ref="A2:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Philippines-specific constant parameters
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
   <si>
     <t>parameter</t>
   </si>
@@ -193,6 +198,15 @@
   </si>
   <si>
     <t>age_breakpoints</t>
+  </si>
+  <si>
+    <t>demo_household_size</t>
+  </si>
+  <si>
+    <t>comorb_startage_diabetes</t>
+  </si>
+  <si>
+    <t>Philippines average houshold size in 2010 https://psa.gov.ph/content/household-population-philippines-reaches-921-million</t>
   </si>
 </sst>
 </file>
@@ -1168,7 +1182,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1240,6 +1254,8 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -1963,7 +1979,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1998,7 +2014,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2210,10 +2226,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,7 +2316,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="62">
-        <v>190000</v>
+        <v>7000000</v>
       </c>
       <c r="F5" s="62">
         <v>190000</v>
@@ -2323,7 +2339,26 @@
         <v>15</v>
       </c>
       <c r="D6" s="29">
-        <v>25</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="66">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="37">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2358,11 +2393,11 @@
   </sheetPr>
   <dimension ref="A1:CC25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2693,75 +2728,31 @@
       <c r="K3" s="9">
         <v>10</v>
       </c>
-      <c r="AF3" s="26">
-        <v>40</v>
-      </c>
-      <c r="AG3" s="26">
-        <v>40</v>
-      </c>
-      <c r="AH3" s="26">
-        <v>40</v>
-      </c>
-      <c r="AI3" s="26">
-        <v>40</v>
-      </c>
-      <c r="AJ3" s="26">
-        <v>40</v>
-      </c>
-      <c r="AK3" s="26">
-        <v>40</v>
-      </c>
-      <c r="AL3" s="26">
-        <v>40</v>
-      </c>
-      <c r="AM3" s="26">
-        <v>40</v>
-      </c>
-      <c r="AN3" s="26">
-        <v>40</v>
-      </c>
-      <c r="AO3" s="26">
-        <v>40</v>
-      </c>
-      <c r="AP3" s="26">
-        <v>40</v>
-      </c>
-      <c r="AQ3" s="26">
-        <v>40</v>
-      </c>
-      <c r="AR3" s="26">
-        <v>40</v>
-      </c>
-      <c r="AS3" s="26">
-        <v>40</v>
-      </c>
-      <c r="AT3" s="26">
-        <v>40</v>
-      </c>
-      <c r="AU3" s="26">
-        <v>40</v>
-      </c>
-      <c r="AV3" s="26">
-        <v>10</v>
-      </c>
-      <c r="AW3" s="26">
-        <v>10</v>
-      </c>
-      <c r="AX3" s="26">
-        <v>10</v>
-      </c>
+      <c r="AF3" s="26"/>
+      <c r="AG3" s="26"/>
+      <c r="AH3" s="26"/>
+      <c r="AI3" s="26"/>
+      <c r="AJ3" s="26"/>
+      <c r="AK3" s="26"/>
+      <c r="AL3" s="26"/>
+      <c r="AM3" s="26"/>
+      <c r="AN3" s="26"/>
+      <c r="AO3" s="26"/>
+      <c r="AP3" s="26"/>
+      <c r="AQ3" s="26"/>
+      <c r="AR3" s="26"/>
+      <c r="AS3" s="26"/>
+      <c r="AT3" s="26"/>
+      <c r="AU3" s="26"/>
+      <c r="AV3" s="26"/>
+      <c r="AW3" s="26"/>
+      <c r="AX3" s="26"/>
       <c r="AY3" s="26"/>
-      <c r="AZ3" s="26">
-        <v>30</v>
-      </c>
-      <c r="BA3" s="26">
-        <v>30</v>
-      </c>
+      <c r="AZ3" s="26"/>
+      <c r="BA3" s="26"/>
       <c r="BB3" s="26"/>
       <c r="BC3" s="26"/>
-      <c r="BD3" s="26">
-        <v>56</v>
-      </c>
+      <c r="BD3" s="26"/>
       <c r="BE3" s="26"/>
       <c r="BH3" s="9">
         <v>60</v>

</xml_diff>

<commit_message>
Philippines-specific time-variant diabetes and HIV data
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="63">
   <si>
     <t>parameter</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Philippines average houshold size in 2010 https://psa.gov.ph/content/household-population-philippines-reaches-921-million</t>
+  </si>
+  <si>
+    <t>comorb_perc_hiv</t>
   </si>
 </sst>
 </file>
@@ -2230,7 +2233,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2392,13 +2395,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:CC25"/>
+  <dimension ref="A1:CC26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="BF26" sqref="BF26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3845,7 +3848,7 @@
         <v>57</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C25" s="2">
         <v>1</v>
@@ -3856,14 +3859,70 @@
       <c r="E25" s="50">
         <v>0</v>
       </c>
-      <c r="Y25" s="1">
+      <c r="M25" s="1">
         <v>0</v>
       </c>
-      <c r="AF25" s="1">
-        <v>10</v>
-      </c>
-      <c r="AT25" s="1">
-        <v>20</v>
+      <c r="U25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN25" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="AS25" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AX25" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="BC25" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="BD25" s="1">
+        <v>5.9</v>
+      </c>
+      <c r="BE25" s="1">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="W26" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AH26" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AP26" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AY26" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="BE26" s="1">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
JT Philippines manual calibration
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="6660" tabRatio="807" activeTab="1"/>
   </bookViews>
@@ -20,12 +15,12 @@
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>parameter</t>
   </si>
@@ -111,21 +106,9 @@
     <t>scenario_11</t>
   </si>
   <si>
-    <t>age_unstratified</t>
-  </si>
-  <si>
-    <t>scenario_12</t>
-  </si>
-  <si>
     <t>econ_cpi</t>
   </si>
   <si>
-    <t>without_diabetes</t>
-  </si>
-  <si>
-    <t>with_diabetes</t>
-  </si>
-  <si>
     <t>program_perc_vaccination</t>
   </si>
   <si>
@@ -138,12 +121,6 @@
     <t>program_perc_lowquality</t>
   </si>
   <si>
-    <t>program_perc_firstline_dst</t>
-  </si>
-  <si>
-    <t>program_perc_secondline_dst</t>
-  </si>
-  <si>
     <t>program_perc_xpert</t>
   </si>
   <si>
@@ -162,18 +139,6 @@
     <t>program_perc_treatment_death</t>
   </si>
   <si>
-    <t>program_perc_treatment_success_mdr</t>
-  </si>
-  <si>
-    <t>program_perc_treatment_death_mdr</t>
-  </si>
-  <si>
-    <t>program_perc_treatment_success_xdr</t>
-  </si>
-  <si>
-    <t>program_perc_treatment_death_xdr</t>
-  </si>
-  <si>
     <t>epi_rr_diabetes</t>
   </si>
   <si>
@@ -183,37 +148,40 @@
     <t>program_perc_decentralisation</t>
   </si>
   <si>
-    <t>scenario_13</t>
-  </si>
-  <si>
-    <t>scenario_14</t>
-  </si>
-  <si>
     <t>comorb_perc_diabetes</t>
   </si>
   <si>
+    <t>demo_household_size</t>
+  </si>
+  <si>
+    <t>comorb_startage_diabetes</t>
+  </si>
+  <si>
+    <t>Philippines average houshold size in 2010 https://psa.gov.ph/content/household-population-philippines-reaches-921-million</t>
+  </si>
+  <si>
+    <t>comorb_perc_hiv</t>
+  </si>
+  <si>
+    <t>tb_prop_early_progression_age5to15</t>
+  </si>
+  <si>
+    <t>tb_prop_early_progression_age15up</t>
+  </si>
+  <si>
+    <t>program_perc_ipt_age0to5</t>
+  </si>
+  <si>
+    <t>plot_end_time</t>
+  </si>
+  <si>
+    <t>transmission_modifier</t>
+  </si>
+  <si>
     <t>age_breakpoints</t>
   </si>
   <si>
-    <t>demo_household_size</t>
-  </si>
-  <si>
-    <t>comorb_startage_diabetes</t>
-  </si>
-  <si>
-    <t>Philippines average houshold size in 2010 https://psa.gov.ph/content/household-population-philippines-reaches-921-million</t>
-  </si>
-  <si>
-    <t>comorb_perc_hiv</t>
-  </si>
-  <si>
-    <t>tb_prop_early_progression_age5to15</t>
-  </si>
-  <si>
-    <t>tb_prop_early_progression_age15up</t>
-  </si>
-  <si>
-    <t>program_perc_ipt_age0to5</t>
+    <t>program_perc_novel_vaccination</t>
   </si>
 </sst>
 </file>
@@ -1197,9 +1165,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1227,6 +1192,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="665">
     <cellStyle name="Comma" xfId="664" builtinId="3"/>
@@ -1985,7 +1951,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2020,7 +1986,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2232,7 +2198,7 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -2249,153 +2215,122 @@
     <col min="9" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="21">
-        <v>19</v>
-      </c>
-      <c r="F2" s="21">
-        <v>7.85</v>
-      </c>
-      <c r="G2" s="21">
-        <v>7.85</v>
-      </c>
-      <c r="H2">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="22">
         <v>0.45</v>
       </c>
-      <c r="F3" s="22">
-        <v>0.22</v>
-      </c>
-      <c r="G3" s="22">
-        <v>0.22</v>
-      </c>
-      <c r="H3">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="23">
         <v>1865</v>
       </c>
-      <c r="F4" s="23">
-        <v>1865</v>
-      </c>
-      <c r="G4" s="23">
-        <v>1865</v>
-      </c>
-      <c r="H4">
-        <v>1915</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="44">
-        <v>11500000</v>
-      </c>
-      <c r="F5" s="24">
-        <v>190000</v>
-      </c>
-      <c r="G5" s="24">
-        <v>190000</v>
-      </c>
-      <c r="H5">
-        <v>280000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="14">
+      <c r="B5" s="43">
+        <v>19000000</v>
+      </c>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+    </row>
+    <row r="6" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="43">
         <v>5</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6">
         <v>15</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B7" s="27">
         <v>4.5999999999999996</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B8" s="14">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="45">
+        <v>47</v>
+      </c>
+      <c r="B9" s="44">
         <v>0.26</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="45">
+        <v>48</v>
+      </c>
+      <c r="B10" s="44">
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="45"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="44">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
-      <c r="B12" s="45"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="44"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
-      <c r="B13" s="45"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="44"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="27"/>
     </row>
@@ -2405,7 +2340,7 @@
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5 F5:G5">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B6 F5:G6">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
@@ -2429,13 +2364,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:CC24"/>
+  <dimension ref="A1:BZ20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AW2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="BC2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BF3" sqref="BF3"/>
+      <selection pane="bottomRight" activeCell="BR10" sqref="BR10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2463,12 +2398,11 @@
     <col min="56" max="57" width="7.85546875" style="1" customWidth="1"/>
     <col min="58" max="58" width="14" style="1" customWidth="1"/>
     <col min="59" max="65" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="66" max="70" width="14.42578125" style="1" customWidth="1"/>
-    <col min="71" max="71" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="72" max="16384" width="9.140625" style="1"/>
+    <col min="66" max="68" width="14.42578125" style="1" customWidth="1"/>
+    <col min="69" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:78" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -2673,311 +2607,147 @@
       <c r="BP1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="BQ1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:78" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="BR1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="BS1" s="5" t="s">
+      <c r="B2" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="40">
+        <v>0.1</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="41"/>
+      <c r="F2" s="42">
+        <v>0</v>
+      </c>
+      <c r="J2" s="42">
+        <v>25</v>
+      </c>
+      <c r="BF2" s="50">
+        <v>99</v>
+      </c>
+      <c r="BP2" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:78" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:81" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="41" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="41"/>
+      <c r="BF3" s="50"/>
+      <c r="BK3" s="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:78" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="41">
+      <c r="C4" s="40">
+        <v>5</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="41"/>
+      <c r="I4" s="42">
+        <v>0</v>
+      </c>
+      <c r="BD4" s="42">
+        <v>82</v>
+      </c>
+      <c r="BO4" s="42">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:78" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="47">
         <v>1</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D5" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="H2" s="43">
+      <c r="E5" s="48"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49">
         <v>0</v>
       </c>
-      <c r="J2" s="43">
-        <v>25</v>
-      </c>
-      <c r="BF2" s="51">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:81" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="41">
-        <v>5</v>
-      </c>
-      <c r="D3" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="43">
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49"/>
+      <c r="U5" s="49"/>
+      <c r="V5" s="49"/>
+      <c r="W5" s="49"/>
+      <c r="X5" s="49"/>
+      <c r="Y5" s="49"/>
+      <c r="Z5" s="49"/>
+      <c r="AA5" s="49"/>
+      <c r="AB5" s="49"/>
+      <c r="AC5" s="49"/>
+      <c r="AD5" s="49"/>
+      <c r="AE5" s="49"/>
+      <c r="AF5" s="49"/>
+      <c r="AG5" s="49"/>
+      <c r="AH5" s="49"/>
+      <c r="AI5" s="49"/>
+      <c r="AJ5" s="49"/>
+      <c r="AK5" s="49"/>
+      <c r="AL5" s="49"/>
+      <c r="AM5" s="49"/>
+      <c r="AN5" s="49"/>
+      <c r="AO5" s="49"/>
+      <c r="AP5" s="49"/>
+      <c r="AQ5" s="49"/>
+      <c r="AR5" s="49"/>
+      <c r="AS5" s="49"/>
+      <c r="AT5" s="49"/>
+      <c r="AU5" s="49"/>
+      <c r="AV5" s="49"/>
+      <c r="AW5" s="49"/>
+      <c r="AX5" s="49"/>
+      <c r="AY5" s="49"/>
+      <c r="AZ5" s="49"/>
+      <c r="BA5" s="49"/>
+      <c r="BB5" s="49"/>
+      <c r="BC5" s="49"/>
+      <c r="BD5" s="49">
         <v>0</v>
       </c>
-      <c r="K3" s="43">
-        <v>57</v>
-      </c>
-      <c r="L3" s="43">
-        <v>57</v>
-      </c>
-      <c r="M3" s="43">
-        <v>57</v>
-      </c>
-      <c r="N3" s="43">
-        <v>57</v>
-      </c>
-      <c r="O3" s="43">
-        <v>57</v>
-      </c>
-      <c r="P3" s="43">
-        <v>57</v>
-      </c>
-      <c r="Q3" s="43">
-        <v>57</v>
-      </c>
-      <c r="R3" s="43">
-        <v>57</v>
-      </c>
-      <c r="S3" s="43">
-        <v>57</v>
-      </c>
-      <c r="T3" s="43">
-        <v>57</v>
-      </c>
-      <c r="U3" s="43">
-        <v>57</v>
-      </c>
-      <c r="V3" s="43">
-        <v>57</v>
-      </c>
-      <c r="W3" s="43">
-        <v>57</v>
-      </c>
-      <c r="X3" s="43">
-        <v>57</v>
-      </c>
-      <c r="Y3" s="43">
-        <v>57</v>
-      </c>
-      <c r="Z3" s="43">
-        <v>57</v>
-      </c>
-      <c r="AA3" s="43">
-        <v>57</v>
-      </c>
-      <c r="AB3" s="43">
-        <v>57</v>
-      </c>
-      <c r="AC3" s="43">
-        <v>57</v>
-      </c>
-      <c r="AD3" s="43">
-        <v>57</v>
-      </c>
-      <c r="AE3" s="43">
-        <v>60</v>
-      </c>
-      <c r="AF3" s="43">
-        <v>100</v>
-      </c>
-      <c r="AG3" s="43">
-        <v>80</v>
-      </c>
-      <c r="AH3" s="43">
-        <v>70</v>
-      </c>
-      <c r="AI3" s="43">
-        <v>60</v>
-      </c>
-      <c r="AJ3" s="43">
-        <v>60</v>
-      </c>
-      <c r="AK3" s="43">
-        <v>60</v>
-      </c>
-      <c r="AL3" s="43">
-        <v>60</v>
-      </c>
-      <c r="AM3" s="43">
-        <v>60</v>
-      </c>
-      <c r="AN3" s="43">
-        <v>60</v>
-      </c>
-      <c r="AO3" s="43">
-        <v>50</v>
-      </c>
-      <c r="AP3" s="43">
-        <v>40</v>
-      </c>
-      <c r="AQ3" s="43">
-        <v>55</v>
-      </c>
-      <c r="AR3" s="43">
-        <v>55</v>
-      </c>
-      <c r="AS3" s="43">
-        <v>60</v>
-      </c>
-      <c r="AT3" s="43">
-        <v>60</v>
-      </c>
-      <c r="AU3" s="43">
-        <v>60</v>
-      </c>
-      <c r="AV3" s="43">
-        <v>60</v>
-      </c>
-      <c r="AW3" s="43">
-        <v>60</v>
-      </c>
-      <c r="AX3" s="43">
-        <v>60</v>
-      </c>
-      <c r="AY3" s="43">
-        <v>60</v>
-      </c>
-      <c r="AZ3" s="43">
-        <v>60</v>
-      </c>
-      <c r="BA3" s="43">
-        <v>60</v>
-      </c>
-      <c r="BB3" s="43">
-        <v>60</v>
-      </c>
-      <c r="BC3" s="43">
-        <v>60</v>
-      </c>
-      <c r="BD3" s="43">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:81" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="48">
-        <v>1</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="49"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50">
-        <v>0</v>
-      </c>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="50"/>
-      <c r="R4" s="50"/>
-      <c r="S4" s="50"/>
-      <c r="T4" s="50"/>
-      <c r="U4" s="50"/>
-      <c r="V4" s="50"/>
-      <c r="W4" s="50"/>
-      <c r="X4" s="50"/>
-      <c r="Y4" s="50"/>
-      <c r="Z4" s="50"/>
-      <c r="AA4" s="50">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="50"/>
-      <c r="AC4" s="50"/>
-      <c r="AD4" s="50"/>
-      <c r="AE4" s="50"/>
-      <c r="AF4" s="50"/>
-      <c r="AG4" s="50"/>
-      <c r="AH4" s="50"/>
-      <c r="AI4" s="50"/>
-      <c r="AJ4" s="50"/>
-      <c r="AK4" s="50"/>
-      <c r="AL4" s="50"/>
-      <c r="AM4" s="50"/>
-      <c r="AN4" s="50"/>
-      <c r="AO4" s="50"/>
-      <c r="AP4" s="50"/>
-      <c r="AQ4" s="50"/>
-      <c r="AR4" s="50"/>
-      <c r="AS4" s="50"/>
-      <c r="AT4" s="50"/>
-      <c r="AU4" s="50"/>
-      <c r="AV4" s="50"/>
-      <c r="AW4" s="50"/>
-      <c r="AX4" s="50"/>
-      <c r="AY4" s="50"/>
-      <c r="AZ4" s="50"/>
-      <c r="BA4" s="50">
-        <v>0</v>
-      </c>
-      <c r="BB4" s="50">
-        <v>0</v>
-      </c>
-      <c r="BC4" s="50"/>
-      <c r="BD4" s="50">
-        <v>0</v>
-      </c>
-      <c r="BE4" s="43">
-        <v>0</v>
-      </c>
-      <c r="BH4" s="51">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:81" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="29">
-        <v>1</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="31">
-        <v>70</v>
-      </c>
-      <c r="J5" s="31">
-        <v>80</v>
-      </c>
-      <c r="AD5" s="31">
-        <v>82</v>
-      </c>
-      <c r="AQ5" s="31">
-        <v>84</v>
-      </c>
-      <c r="BC5" s="31">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:81" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BH5" s="50">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:78" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>4</v>
@@ -2989,19 +2759,19 @@
         <v>3</v>
       </c>
       <c r="E6" s="30"/>
-      <c r="H6" s="31">
-        <v>30</v>
-      </c>
-      <c r="K6" s="31">
-        <v>40</v>
-      </c>
-      <c r="AF6" s="31">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:81" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="31">
+        <v>70</v>
+      </c>
+      <c r="V6" s="31">
+        <v>80</v>
+      </c>
+      <c r="BC6" s="31">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:78" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>4</v>
@@ -3013,138 +2783,127 @@
         <v>3</v>
       </c>
       <c r="E7" s="30"/>
-      <c r="V7" s="31">
+      <c r="H7" s="31">
         <v>30</v>
       </c>
-      <c r="AF7" s="31">
+      <c r="K7" s="31">
         <v>40</v>
       </c>
-      <c r="AP7" s="31">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:81" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:78" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="29">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="30"/>
       <c r="I8" s="31">
-        <v>7</v>
-      </c>
-      <c r="AK8" s="31">
-        <v>50</v>
-      </c>
-      <c r="AP8" s="31">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:81" s="31" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="V8" s="31">
+        <v>40</v>
+      </c>
+      <c r="AK8" s="32"/>
+      <c r="AL8" s="32"/>
+      <c r="AM8" s="32"/>
+      <c r="AN8" s="32"/>
+      <c r="AO8" s="32"/>
+      <c r="AP8" s="32"/>
+      <c r="AQ8" s="32"/>
+      <c r="AR8" s="32"/>
+      <c r="AS8" s="32"/>
+      <c r="AT8" s="32"/>
+      <c r="AU8" s="32"/>
+      <c r="AV8" s="32"/>
+      <c r="AW8" s="32"/>
+      <c r="AX8" s="32"/>
+      <c r="AY8" s="32"/>
+      <c r="AZ8" s="32"/>
+      <c r="BA8" s="32"/>
+      <c r="BB8" s="32">
+        <v>93</v>
+      </c>
+      <c r="BC8" s="32">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:78" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="29">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="30"/>
-      <c r="I9" s="31">
-        <v>0</v>
-      </c>
       <c r="V9" s="31">
-        <v>40</v>
-      </c>
-      <c r="AB9" s="31">
-        <v>65</v>
-      </c>
-      <c r="AK9" s="32"/>
+        <v>10</v>
+      </c>
+      <c r="AK9" s="45"/>
       <c r="AL9" s="32"/>
       <c r="AM9" s="32"/>
       <c r="AN9" s="32"/>
       <c r="AO9" s="32"/>
-      <c r="AP9" s="32"/>
+      <c r="AP9" s="45"/>
       <c r="AQ9" s="32"/>
       <c r="AR9" s="32"/>
       <c r="AS9" s="32"/>
       <c r="AT9" s="32"/>
-      <c r="AU9" s="32"/>
+      <c r="AU9" s="45"/>
       <c r="AV9" s="32"/>
       <c r="AW9" s="32"/>
       <c r="AX9" s="32"/>
       <c r="AY9" s="32"/>
-      <c r="AZ9" s="32"/>
+      <c r="AZ9" s="45"/>
       <c r="BA9" s="32"/>
-      <c r="BB9" s="32">
-        <v>93</v>
-      </c>
-      <c r="BC9" s="32">
-        <v>85</v>
-      </c>
-      <c r="BD9" s="31">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:81" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="29" t="s">
+      <c r="BB9" s="32"/>
+      <c r="BC9" s="32"/>
+    </row>
+    <row r="10" spans="1:78" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="40">
+        <v>1</v>
+      </c>
+      <c r="D10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="30"/>
-      <c r="V10" s="31">
-        <v>2</v>
-      </c>
-      <c r="AK10" s="46">
-        <v>1</v>
-      </c>
-      <c r="AL10" s="32"/>
-      <c r="AM10" s="32"/>
-      <c r="AN10" s="32"/>
-      <c r="AO10" s="32"/>
-      <c r="AP10" s="46"/>
-      <c r="AQ10" s="32"/>
-      <c r="AR10" s="32"/>
-      <c r="AS10" s="32"/>
-      <c r="AT10" s="32"/>
-      <c r="AU10" s="46"/>
-      <c r="AV10" s="32"/>
-      <c r="AW10" s="32"/>
-      <c r="AX10" s="32"/>
-      <c r="AY10" s="32"/>
-      <c r="AZ10" s="46"/>
-      <c r="BA10" s="32"/>
-      <c r="BB10" s="32"/>
-      <c r="BC10" s="32"/>
-      <c r="BD10" s="31">
+      <c r="E10" s="41"/>
+      <c r="AZ10" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:81" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BB10" s="42">
+        <v>2.8</v>
+      </c>
+      <c r="BD10" s="42">
+        <v>2.8</v>
+      </c>
+      <c r="BG10" s="50">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:78" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" s="29">
         <v>1</v>
@@ -3153,41 +2912,87 @@
         <v>3</v>
       </c>
       <c r="E11" s="30"/>
-      <c r="I11" s="31">
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="33"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="33"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="33"/>
+      <c r="X11" s="33"/>
+      <c r="Y11" s="33"/>
+      <c r="Z11" s="33"/>
+      <c r="AA11" s="33"/>
+      <c r="AB11" s="33"/>
+      <c r="AC11" s="33"/>
+      <c r="AD11" s="33"/>
+      <c r="AE11" s="33"/>
+      <c r="AF11" s="33"/>
+      <c r="AG11" s="33"/>
+      <c r="AH11" s="33"/>
+      <c r="AI11" s="33"/>
+      <c r="AJ11" s="33"/>
+      <c r="AK11" s="33"/>
+      <c r="AL11" s="33"/>
+      <c r="AM11" s="33"/>
+      <c r="AN11" s="33"/>
+      <c r="AO11" s="33"/>
+      <c r="AP11" s="33"/>
+      <c r="AQ11" s="33"/>
+      <c r="AR11" s="33"/>
+      <c r="AS11" s="33"/>
+      <c r="AT11" s="33"/>
+      <c r="AU11" s="33"/>
+      <c r="AV11" s="33"/>
+      <c r="AW11" s="33"/>
+      <c r="AX11" s="33"/>
+      <c r="AY11" s="33"/>
+      <c r="AZ11" s="33"/>
+      <c r="BA11" s="33"/>
+      <c r="BB11" s="33"/>
+      <c r="BC11" s="33"/>
+      <c r="BD11" s="33">
         <v>0</v>
       </c>
-      <c r="V11" s="31">
-        <v>15</v>
-      </c>
-      <c r="AB11" s="31">
-        <v>30</v>
-      </c>
-      <c r="AK11" s="32"/>
-      <c r="AL11" s="32"/>
-      <c r="AM11" s="32"/>
-      <c r="AN11" s="32"/>
-      <c r="AO11" s="32"/>
-      <c r="AP11" s="32"/>
-      <c r="AQ11" s="32"/>
-      <c r="AR11" s="32"/>
-      <c r="AS11" s="32"/>
-      <c r="AT11" s="32"/>
-      <c r="AU11" s="32"/>
-      <c r="AV11" s="32"/>
-      <c r="AW11" s="32"/>
-      <c r="AX11" s="32"/>
-      <c r="AY11" s="32"/>
-      <c r="AZ11" s="32"/>
-      <c r="BA11" s="32"/>
-      <c r="BB11" s="32"/>
-      <c r="BC11" s="32"/>
-      <c r="BD11" s="31">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:81" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BE11" s="33"/>
+      <c r="BF11" s="33"/>
+      <c r="BG11" s="33"/>
+      <c r="BH11" s="33"/>
+      <c r="BI11" s="33"/>
+      <c r="BJ11" s="33"/>
+      <c r="BK11" s="33"/>
+      <c r="BL11" s="33"/>
+      <c r="BM11" s="33">
+        <v>75</v>
+      </c>
+      <c r="BN11" s="33"/>
+      <c r="BO11" s="33"/>
+      <c r="BP11" s="33"/>
+      <c r="BQ11" s="33"/>
+      <c r="BR11" s="33"/>
+      <c r="BS11" s="33"/>
+      <c r="BT11" s="33"/>
+      <c r="BU11" s="33"/>
+      <c r="BV11" s="33"/>
+      <c r="BW11" s="33"/>
+      <c r="BX11" s="33"/>
+      <c r="BY11" s="33"/>
+      <c r="BZ11" s="33"/>
+    </row>
+    <row r="12" spans="1:78" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B12" s="29" t="s">
         <v>3</v>
@@ -3199,823 +3004,441 @@
         <v>3</v>
       </c>
       <c r="E12" s="30"/>
-      <c r="I12" s="31">
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="33"/>
+      <c r="T12" s="33"/>
+      <c r="U12" s="33"/>
+      <c r="V12" s="33"/>
+      <c r="W12" s="33"/>
+      <c r="X12" s="33"/>
+      <c r="Y12" s="33"/>
+      <c r="Z12" s="33"/>
+      <c r="AA12" s="33"/>
+      <c r="AB12" s="33"/>
+      <c r="AC12" s="33"/>
+      <c r="AD12" s="33"/>
+      <c r="AE12" s="33"/>
+      <c r="AF12" s="33"/>
+      <c r="AG12" s="33"/>
+      <c r="AH12" s="33"/>
+      <c r="AI12" s="33"/>
+      <c r="AJ12" s="33"/>
+      <c r="AK12" s="33"/>
+      <c r="AL12" s="33"/>
+      <c r="AM12" s="33"/>
+      <c r="AN12" s="33"/>
+      <c r="AO12" s="33"/>
+      <c r="AP12" s="33"/>
+      <c r="AQ12" s="33"/>
+      <c r="AR12" s="33"/>
+      <c r="AS12" s="33"/>
+      <c r="AT12" s="33"/>
+      <c r="AU12" s="33"/>
+      <c r="AV12" s="33"/>
+      <c r="AW12" s="33"/>
+      <c r="AX12" s="33"/>
+      <c r="AY12" s="33"/>
+      <c r="AZ12" s="33"/>
+      <c r="BA12" s="33"/>
+      <c r="BB12" s="33"/>
+      <c r="BC12" s="33"/>
+      <c r="BD12" s="33">
         <v>0</v>
       </c>
-      <c r="V12" s="31">
-        <v>55</v>
-      </c>
-      <c r="AB12" s="31">
+      <c r="BE12" s="33"/>
+      <c r="BF12" s="33"/>
+      <c r="BG12" s="33"/>
+      <c r="BH12" s="33"/>
+      <c r="BI12" s="33"/>
+      <c r="BJ12" s="33"/>
+      <c r="BK12" s="33"/>
+      <c r="BL12" s="33">
+        <v>75</v>
+      </c>
+      <c r="BM12" s="33"/>
+      <c r="BN12" s="33"/>
+      <c r="BO12" s="33"/>
+      <c r="BP12" s="33"/>
+      <c r="BQ12" s="33"/>
+      <c r="BR12" s="33"/>
+      <c r="BS12" s="33"/>
+      <c r="BT12" s="33"/>
+      <c r="BU12" s="33"/>
+      <c r="BV12" s="33"/>
+      <c r="BW12" s="33"/>
+      <c r="BX12" s="33"/>
+      <c r="BY12" s="33"/>
+      <c r="BZ12" s="33"/>
+    </row>
+    <row r="13" spans="1:78" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="35">
+        <v>1</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="36"/>
+      <c r="BD13" s="37">
+        <v>0</v>
+      </c>
+      <c r="BI13" s="51">
         <v>50</v>
       </c>
-      <c r="AK12" s="32"/>
-      <c r="AL12" s="32"/>
-      <c r="AM12" s="32"/>
-      <c r="AN12" s="32"/>
-      <c r="AO12" s="32"/>
-      <c r="AP12" s="32"/>
-      <c r="AQ12" s="32"/>
-      <c r="AR12" s="32"/>
-      <c r="AS12" s="32"/>
-      <c r="AT12" s="32"/>
-      <c r="AU12" s="32"/>
-      <c r="AV12" s="32"/>
-      <c r="AW12" s="32"/>
-      <c r="AX12" s="32"/>
-      <c r="AY12" s="32"/>
-      <c r="AZ12" s="32"/>
-      <c r="BA12" s="32"/>
-      <c r="BB12" s="32"/>
-      <c r="BC12" s="32"/>
-      <c r="BD12" s="31">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:81" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="29" t="s">
+      <c r="BJ13" s="52"/>
+    </row>
+    <row r="14" spans="1:78" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C14" s="35">
         <v>1</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D14" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="I13" s="31">
+      <c r="E14" s="36"/>
+      <c r="BD14" s="37">
         <v>0</v>
       </c>
-      <c r="V13" s="31">
-        <v>5</v>
-      </c>
-      <c r="AB13" s="31">
-        <v>15</v>
-      </c>
-      <c r="AK13" s="32"/>
-      <c r="AL13" s="32"/>
-      <c r="AM13" s="32"/>
-      <c r="AN13" s="32"/>
-      <c r="AO13" s="32"/>
-      <c r="AP13" s="32"/>
-      <c r="AQ13" s="32"/>
-      <c r="AR13" s="32"/>
-      <c r="AS13" s="32"/>
-      <c r="AT13" s="32"/>
-      <c r="AU13" s="32"/>
-      <c r="AV13" s="32"/>
-      <c r="AW13" s="32"/>
-      <c r="AX13" s="32"/>
-      <c r="AY13" s="32"/>
-      <c r="AZ13" s="32"/>
-      <c r="BA13" s="32"/>
-      <c r="BB13" s="32"/>
-      <c r="BC13" s="32"/>
-      <c r="BD13" s="31">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:81" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="29" t="s">
+      <c r="BI14" s="52"/>
+      <c r="BJ14" s="51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:78" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C15" s="35">
         <v>1</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D15" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="I14" s="31">
+      <c r="E15" s="36">
+        <v>1</v>
+      </c>
+      <c r="H15" s="38">
+        <v>1</v>
+      </c>
+      <c r="J15" s="38">
+        <v>1.1289570744394</v>
+      </c>
+      <c r="K15" s="38">
+        <v>1.42215881727406</v>
+      </c>
+      <c r="L15" s="38">
+        <v>1.90118931222233</v>
+      </c>
+      <c r="M15" s="38">
+        <v>2.3081073919986701</v>
+      </c>
+      <c r="N15" s="38">
+        <v>2.4974653103104298</v>
+      </c>
+      <c r="O15" s="38">
+        <v>2.9115458645382701</v>
+      </c>
+      <c r="P15" s="38">
+        <v>3.90623450399154</v>
+      </c>
+      <c r="Q15" s="38">
+        <v>4.1703507493909102</v>
+      </c>
+      <c r="R15" s="38">
+        <v>4.55399078719985</v>
+      </c>
+      <c r="S15" s="38">
+        <v>5.0047790229916798</v>
+      </c>
+      <c r="T15" s="38">
+        <v>5.3718558386314896</v>
+      </c>
+      <c r="U15" s="38">
+        <v>6.3137212289735496</v>
+      </c>
+      <c r="V15" s="38">
+        <v>7.4628507238053698</v>
+      </c>
+      <c r="W15" s="38">
+        <v>8.4391855224587609</v>
+      </c>
+      <c r="X15" s="38">
+        <v>9.3018160392078606</v>
+      </c>
+      <c r="Y15" s="38">
+        <v>10.2347283365258</v>
+      </c>
+      <c r="Z15" s="38">
+        <v>15.386785740408699</v>
+      </c>
+      <c r="AA15" s="38">
+        <v>18.9416113416321</v>
+      </c>
+      <c r="AB15" s="38">
+        <v>19.1590871369295</v>
+      </c>
+      <c r="AC15" s="38">
+        <v>19.938817427385899</v>
+      </c>
+      <c r="AD15" s="38">
+        <v>22.702351313969601</v>
+      </c>
+      <c r="AE15" s="38">
+        <v>25.481798063623799</v>
+      </c>
+      <c r="AF15" s="38">
+        <v>28.584806362378998</v>
+      </c>
+      <c r="AG15" s="38">
+        <v>34.090656984785603</v>
+      </c>
+      <c r="AH15" s="38">
+        <v>37.0398409405256</v>
+      </c>
+      <c r="AI15" s="38">
+        <v>39.527551867219898</v>
+      </c>
+      <c r="AJ15" s="38">
+        <v>43.633070539419101</v>
+      </c>
+      <c r="AK15" s="38">
+        <v>46.6140802213001</v>
+      </c>
+      <c r="AL15" s="38">
+        <v>50.0989972337483</v>
+      </c>
+      <c r="AM15" s="38">
+        <v>52.899661134163203</v>
+      </c>
+      <c r="AN15" s="38">
+        <v>57.784910096818798</v>
+      </c>
+      <c r="AO15" s="38">
+        <v>61.2167842323652</v>
+      </c>
+      <c r="AP15" s="38">
+        <v>63.651452282157699</v>
+      </c>
+      <c r="AQ15" s="38">
+        <v>67.053941908713696</v>
+      </c>
+      <c r="AR15" s="38">
+        <v>68.8796680497925</v>
+      </c>
+      <c r="AS15" s="38">
+        <v>70.456431535269701</v>
+      </c>
+      <c r="AT15" s="38">
+        <v>73.858921161825705</v>
+      </c>
+      <c r="AU15" s="38">
+        <v>78.6721991701245</v>
+      </c>
+      <c r="AV15" s="38">
+        <v>82.987551867219906</v>
+      </c>
+      <c r="AW15" s="38">
+        <v>85.394190871369304</v>
+      </c>
+      <c r="AX15" s="38">
+        <v>92.448132780083</v>
+      </c>
+      <c r="AY15" s="38">
+        <v>96.348547717842294</v>
+      </c>
+      <c r="AZ15" s="38">
+        <v>100</v>
+      </c>
+      <c r="BA15" s="38">
+        <v>104.647302904564</v>
+      </c>
+      <c r="BB15" s="38">
+        <v>107.966804979253</v>
+      </c>
+      <c r="BC15" s="38">
+        <v>111.203319502075</v>
+      </c>
+      <c r="BD15" s="38">
+        <v>115.767634854772</v>
+      </c>
+      <c r="BE15" s="38">
+        <v>117.42738589211601</v>
+      </c>
+    </row>
+    <row r="16" spans="1:78" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="35">
+        <v>1</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="36">
+        <v>1</v>
+      </c>
+      <c r="AE16" s="37">
+        <v>1</v>
+      </c>
+      <c r="AF16" s="37">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="BA16" s="37">
+        <v>3.11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:66" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="19"/>
+      <c r="BG17" s="12">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="18" spans="1:66" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="35">
+        <v>1</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="36"/>
+      <c r="AE18" s="37">
         <v>0</v>
       </c>
-      <c r="V14" s="31">
-        <v>65</v>
-      </c>
-      <c r="AB14" s="31">
-        <v>62</v>
-      </c>
-      <c r="AK14" s="32"/>
-      <c r="AL14" s="32"/>
-      <c r="AM14" s="32"/>
-      <c r="AN14" s="32"/>
-      <c r="AO14" s="32"/>
-      <c r="AP14" s="32"/>
-      <c r="AQ14" s="32"/>
-      <c r="AR14" s="32"/>
-      <c r="AS14" s="32"/>
-      <c r="AT14" s="32"/>
-      <c r="AU14" s="32"/>
-      <c r="AV14" s="32"/>
-      <c r="AW14" s="32"/>
-      <c r="AX14" s="32"/>
-      <c r="AY14" s="32"/>
-      <c r="AZ14" s="32"/>
-      <c r="BA14" s="32"/>
-      <c r="BB14" s="32"/>
-      <c r="BC14" s="32"/>
-      <c r="BD14" s="31">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:81" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="41" t="s">
+      <c r="AN18" s="37">
+        <v>3.1</v>
+      </c>
+      <c r="AS18" s="37">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AX18" s="37">
+        <v>5.2</v>
+      </c>
+      <c r="BC18" s="37">
+        <v>5.4</v>
+      </c>
+      <c r="BD18" s="37">
+        <v>5.9</v>
+      </c>
+      <c r="BE18" s="37">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:66" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="41">
+      <c r="C19" s="35">
         <v>1</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D19" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="42">
-        <v>0</v>
-      </c>
-      <c r="I15" s="43">
-        <v>0</v>
-      </c>
-      <c r="L15" s="43">
-        <v>0</v>
-      </c>
-      <c r="V15" s="43">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="43">
-        <v>0</v>
-      </c>
-      <c r="AP15" s="43">
-        <v>0</v>
-      </c>
-      <c r="AZ15" s="43">
-        <v>0</v>
-      </c>
-      <c r="BB15" s="43">
-        <v>2.8</v>
-      </c>
-      <c r="BC15" s="43">
-        <v>2.8</v>
-      </c>
-      <c r="BD15" s="43">
-        <v>2.8</v>
-      </c>
-      <c r="BG15" s="51">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:81" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="29" t="s">
+      <c r="E19" s="36"/>
+      <c r="W19" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="AH19" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="AP19" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="AY19" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="BE19" s="37">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C20" s="2">
         <v>1</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="33"/>
-      <c r="R16" s="33"/>
-      <c r="S16" s="33"/>
-      <c r="T16" s="33"/>
-      <c r="U16" s="33"/>
-      <c r="V16" s="33"/>
-      <c r="W16" s="33"/>
-      <c r="X16" s="33"/>
-      <c r="Y16" s="33"/>
-      <c r="Z16" s="33"/>
-      <c r="AA16" s="33"/>
-      <c r="AB16" s="33"/>
-      <c r="AC16" s="33"/>
-      <c r="AD16" s="33"/>
-      <c r="AE16" s="33"/>
-      <c r="AF16" s="33"/>
-      <c r="AG16" s="33"/>
-      <c r="AH16" s="33"/>
-      <c r="AI16" s="33"/>
-      <c r="AJ16" s="33"/>
-      <c r="AK16" s="33"/>
-      <c r="AL16" s="33"/>
-      <c r="AM16" s="33"/>
-      <c r="AN16" s="33"/>
-      <c r="AO16" s="33"/>
-      <c r="AP16" s="33"/>
-      <c r="AQ16" s="33"/>
-      <c r="AR16" s="33"/>
-      <c r="AS16" s="33"/>
-      <c r="AT16" s="33"/>
-      <c r="AU16" s="33"/>
-      <c r="AV16" s="33"/>
-      <c r="AW16" s="33"/>
-      <c r="AX16" s="33"/>
-      <c r="AY16" s="33"/>
-      <c r="AZ16" s="33"/>
-      <c r="BA16" s="33"/>
-      <c r="BB16" s="33"/>
-      <c r="BC16" s="33"/>
-      <c r="BD16" s="33">
-        <v>0</v>
-      </c>
-      <c r="BE16" s="33"/>
-      <c r="BF16" s="33"/>
-      <c r="BG16" s="33"/>
-      <c r="BH16" s="33"/>
-      <c r="BI16" s="33"/>
-      <c r="BJ16" s="33"/>
-      <c r="BK16" s="33"/>
-      <c r="BL16" s="33"/>
-      <c r="BM16" s="33"/>
-      <c r="BN16" s="33"/>
-      <c r="BO16" s="33"/>
-      <c r="BP16" s="33"/>
-      <c r="BQ16" s="34"/>
-      <c r="BR16" s="34"/>
-      <c r="BS16" s="33"/>
-      <c r="BT16" s="33"/>
-      <c r="BU16" s="33"/>
-      <c r="BV16" s="33"/>
-      <c r="BW16" s="33"/>
-      <c r="BX16" s="33"/>
-      <c r="BY16" s="33"/>
-      <c r="BZ16" s="33"/>
-      <c r="CA16" s="33"/>
-      <c r="CB16" s="33"/>
-      <c r="CC16" s="33"/>
-    </row>
-    <row r="17" spans="1:81" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="29">
+      <c r="E20" s="20">
         <v>1</v>
       </c>
-      <c r="D17" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="30">
-        <v>0</v>
-      </c>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="33"/>
-      <c r="Q17" s="33"/>
-      <c r="R17" s="33"/>
-      <c r="S17" s="33"/>
-      <c r="T17" s="33"/>
-      <c r="U17" s="33"/>
-      <c r="V17" s="33"/>
-      <c r="W17" s="33"/>
-      <c r="X17" s="33"/>
-      <c r="Y17" s="33"/>
-      <c r="Z17" s="33"/>
-      <c r="AA17" s="33"/>
-      <c r="AB17" s="33"/>
-      <c r="AC17" s="33"/>
-      <c r="AD17" s="33"/>
-      <c r="AE17" s="33"/>
-      <c r="AF17" s="33"/>
-      <c r="AG17" s="33"/>
-      <c r="AH17" s="33"/>
-      <c r="AI17" s="33"/>
-      <c r="AJ17" s="33"/>
-      <c r="AK17" s="33"/>
-      <c r="AL17" s="33"/>
-      <c r="AM17" s="33"/>
-      <c r="AN17" s="33"/>
-      <c r="AO17" s="33"/>
-      <c r="AP17" s="33"/>
-      <c r="AQ17" s="33"/>
-      <c r="AR17" s="33"/>
-      <c r="AS17" s="33"/>
-      <c r="AT17" s="33"/>
-      <c r="AU17" s="33"/>
-      <c r="AV17" s="33"/>
-      <c r="AW17" s="33"/>
-      <c r="AX17" s="33"/>
-      <c r="AY17" s="33"/>
-      <c r="AZ17" s="33"/>
-      <c r="BA17" s="33"/>
-      <c r="BB17" s="33"/>
-      <c r="BC17" s="33"/>
-      <c r="BD17" s="33">
-        <v>0</v>
-      </c>
-      <c r="BE17" s="33"/>
-      <c r="BF17" s="33"/>
-      <c r="BG17" s="33"/>
-      <c r="BH17" s="33"/>
-      <c r="BI17" s="33"/>
-      <c r="BJ17" s="33"/>
-      <c r="BK17" s="33"/>
-      <c r="BL17" s="33"/>
-      <c r="BM17" s="33"/>
-      <c r="BN17" s="33"/>
-      <c r="BO17" s="33"/>
-      <c r="BP17" s="33"/>
-      <c r="BQ17" s="34">
-        <v>50</v>
-      </c>
-      <c r="BR17" s="34">
-        <v>75</v>
-      </c>
-      <c r="BS17" s="33"/>
-      <c r="BT17" s="33"/>
-      <c r="BU17" s="33"/>
-      <c r="BV17" s="33"/>
-      <c r="BW17" s="33"/>
-      <c r="BX17" s="33"/>
-      <c r="BY17" s="33"/>
-      <c r="BZ17" s="33"/>
-      <c r="CA17" s="33"/>
-      <c r="CB17" s="33"/>
-      <c r="CC17" s="33"/>
-    </row>
-    <row r="18" spans="1:81" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="36">
+      <c r="AK20" s="1">
         <v>1</v>
       </c>
-      <c r="D18" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="37">
-        <v>0</v>
-      </c>
-      <c r="L18" s="38">
-        <v>0</v>
-      </c>
-      <c r="V18" s="38">
-        <v>0</v>
-      </c>
-      <c r="AF18" s="38">
-        <v>0</v>
-      </c>
-      <c r="AP18" s="38">
-        <v>0</v>
-      </c>
-      <c r="AZ18" s="38">
-        <v>0</v>
-      </c>
-      <c r="BD18" s="38">
-        <v>0</v>
-      </c>
-      <c r="BI18" s="52">
-        <v>50</v>
-      </c>
-      <c r="BJ18" s="53"/>
-    </row>
-    <row r="19" spans="1:81" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="36">
-        <v>1</v>
-      </c>
-      <c r="D19" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="37">
-        <v>0</v>
-      </c>
-      <c r="L19" s="38">
-        <v>0</v>
-      </c>
-      <c r="V19" s="38">
-        <v>0</v>
-      </c>
-      <c r="AF19" s="38">
-        <v>0</v>
-      </c>
-      <c r="AP19" s="38">
-        <v>0</v>
-      </c>
-      <c r="AZ19" s="38">
-        <v>0</v>
-      </c>
-      <c r="BD19" s="38">
-        <v>0</v>
-      </c>
-      <c r="BI19" s="53"/>
-      <c r="BJ19" s="52">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:81" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="36">
-        <v>1</v>
-      </c>
-      <c r="D20" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="37">
-        <v>1</v>
-      </c>
-      <c r="F20" s="38">
-        <v>1</v>
-      </c>
-      <c r="G20" s="38">
-        <v>1</v>
-      </c>
-      <c r="H20" s="39">
-        <v>1</v>
-      </c>
-      <c r="J20" s="39">
-        <v>1.1289570744394</v>
-      </c>
-      <c r="K20" s="39">
-        <v>1.42215881727406</v>
-      </c>
-      <c r="L20" s="39">
-        <v>1.90118931222233</v>
-      </c>
-      <c r="M20" s="39">
-        <v>2.3081073919986701</v>
-      </c>
-      <c r="N20" s="39">
-        <v>2.4974653103104298</v>
-      </c>
-      <c r="O20" s="39">
-        <v>2.9115458645382701</v>
-      </c>
-      <c r="P20" s="39">
-        <v>3.90623450399154</v>
-      </c>
-      <c r="Q20" s="39">
-        <v>4.1703507493909102</v>
-      </c>
-      <c r="R20" s="39">
-        <v>4.55399078719985</v>
-      </c>
-      <c r="S20" s="39">
-        <v>5.0047790229916798</v>
-      </c>
-      <c r="T20" s="39">
-        <v>5.3718558386314896</v>
-      </c>
-      <c r="U20" s="39">
-        <v>6.3137212289735496</v>
-      </c>
-      <c r="V20" s="39">
-        <v>7.4628507238053698</v>
-      </c>
-      <c r="W20" s="39">
-        <v>8.4391855224587609</v>
-      </c>
-      <c r="X20" s="39">
-        <v>9.3018160392078606</v>
-      </c>
-      <c r="Y20" s="39">
-        <v>10.2347283365258</v>
-      </c>
-      <c r="Z20" s="39">
-        <v>15.386785740408699</v>
-      </c>
-      <c r="AA20" s="39">
-        <v>18.9416113416321</v>
-      </c>
-      <c r="AB20" s="39">
-        <v>19.1590871369295</v>
-      </c>
-      <c r="AC20" s="39">
-        <v>19.938817427385899</v>
-      </c>
-      <c r="AD20" s="39">
-        <v>22.702351313969601</v>
-      </c>
-      <c r="AE20" s="39">
-        <v>25.481798063623799</v>
-      </c>
-      <c r="AF20" s="39">
-        <v>28.584806362378998</v>
-      </c>
-      <c r="AG20" s="39">
-        <v>34.090656984785603</v>
-      </c>
-      <c r="AH20" s="39">
-        <v>37.0398409405256</v>
-      </c>
-      <c r="AI20" s="39">
-        <v>39.527551867219898</v>
-      </c>
-      <c r="AJ20" s="39">
-        <v>43.633070539419101</v>
-      </c>
-      <c r="AK20" s="39">
-        <v>46.6140802213001</v>
-      </c>
-      <c r="AL20" s="39">
-        <v>50.0989972337483</v>
-      </c>
-      <c r="AM20" s="39">
-        <v>52.899661134163203</v>
-      </c>
-      <c r="AN20" s="39">
-        <v>57.784910096818798</v>
-      </c>
-      <c r="AO20" s="39">
-        <v>61.2167842323652</v>
-      </c>
-      <c r="AP20" s="39">
-        <v>63.651452282157699</v>
-      </c>
-      <c r="AQ20" s="39">
-        <v>67.053941908713696</v>
-      </c>
-      <c r="AR20" s="39">
-        <v>68.8796680497925</v>
-      </c>
-      <c r="AS20" s="39">
-        <v>70.456431535269701</v>
-      </c>
-      <c r="AT20" s="39">
-        <v>73.858921161825705</v>
-      </c>
-      <c r="AU20" s="39">
-        <v>78.6721991701245</v>
-      </c>
-      <c r="AV20" s="39">
-        <v>82.987551867219906</v>
-      </c>
-      <c r="AW20" s="39">
-        <v>85.394190871369304</v>
-      </c>
-      <c r="AX20" s="39">
-        <v>92.448132780083</v>
-      </c>
-      <c r="AY20" s="39">
-        <v>96.348547717842294</v>
-      </c>
-      <c r="AZ20" s="39">
-        <v>100</v>
-      </c>
-      <c r="BA20" s="39">
-        <v>104.647302904564</v>
-      </c>
-      <c r="BB20" s="39">
-        <v>107.966804979253</v>
-      </c>
-      <c r="BC20" s="39">
-        <v>111.203319502075</v>
-      </c>
-      <c r="BD20" s="39">
-        <v>115.767634854772</v>
-      </c>
-      <c r="BE20" s="39">
-        <v>117.42738589211601</v>
-      </c>
-    </row>
-    <row r="21" spans="1:81" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="36">
-        <v>1</v>
-      </c>
-      <c r="D21" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="37">
-        <v>1</v>
-      </c>
-      <c r="F21" s="38">
-        <v>1</v>
-      </c>
-      <c r="G21" s="38">
-        <v>1</v>
-      </c>
-      <c r="H21" s="38">
-        <v>1</v>
-      </c>
-      <c r="I21" s="38">
-        <v>1</v>
-      </c>
-      <c r="J21" s="38">
-        <v>1</v>
-      </c>
-      <c r="K21" s="38">
-        <v>1</v>
-      </c>
-      <c r="L21" s="38">
-        <v>1</v>
-      </c>
-      <c r="M21" s="38">
-        <v>1</v>
-      </c>
-      <c r="N21" s="38">
-        <v>1</v>
-      </c>
-      <c r="O21" s="38">
-        <v>1</v>
-      </c>
-      <c r="P21" s="38">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="38">
-        <v>1</v>
-      </c>
-      <c r="R21" s="38">
-        <v>1</v>
-      </c>
-      <c r="S21" s="38">
-        <v>1</v>
-      </c>
-      <c r="T21" s="38">
-        <v>1</v>
-      </c>
-      <c r="U21" s="38">
-        <v>1</v>
-      </c>
-      <c r="V21" s="38">
-        <v>1</v>
-      </c>
-      <c r="W21" s="38">
-        <v>1</v>
-      </c>
-      <c r="X21" s="38">
-        <v>1</v>
-      </c>
-      <c r="Y21" s="38">
-        <v>1</v>
-      </c>
-      <c r="Z21" s="38">
-        <v>1</v>
-      </c>
-      <c r="AA21" s="38">
-        <v>1</v>
-      </c>
-      <c r="AB21" s="38">
-        <v>1</v>
-      </c>
-      <c r="AC21" s="38">
-        <v>1</v>
-      </c>
-      <c r="AD21" s="38">
-        <v>1</v>
-      </c>
-      <c r="AE21" s="38">
-        <v>1</v>
-      </c>
-      <c r="AF21" s="38">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="BA21" s="38">
-        <v>3.11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:81" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="19"/>
-      <c r="BG22" s="12">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="23" spans="1:81" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="36">
-        <v>1</v>
-      </c>
-      <c r="D23" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="37">
-        <v>0</v>
-      </c>
-      <c r="M23" s="38">
-        <v>0</v>
-      </c>
-      <c r="U23" s="38">
-        <v>0</v>
-      </c>
-      <c r="AC23" s="38">
-        <v>0</v>
-      </c>
-      <c r="AE23" s="38">
-        <v>0</v>
-      </c>
-      <c r="AN23" s="38">
-        <v>3.1</v>
-      </c>
-      <c r="AS23" s="38">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="AX23" s="38">
-        <v>5.2</v>
-      </c>
-      <c r="BC23" s="38">
-        <v>5.4</v>
-      </c>
-      <c r="BD23" s="38">
-        <v>5.9</v>
-      </c>
-      <c r="BE23" s="38">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:81" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="36">
-        <v>1</v>
-      </c>
-      <c r="D24" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="37"/>
-      <c r="W24" s="38">
-        <v>0.1</v>
-      </c>
-      <c r="AH24" s="38">
-        <v>0.1</v>
-      </c>
-      <c r="AP24" s="38">
-        <v>0.1</v>
-      </c>
-      <c r="AY24" s="38">
-        <v>0.1</v>
-      </c>
-      <c r="BE24" s="38">
-        <v>0.1</v>
+      <c r="AP20" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="AU20" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="BN20" s="1">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="5">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF15:BG15 F4:BD4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF10:BG10 F5:BD5">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:D1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F15:BE15 F2:AF2 BE2:BG14 AG2:BD3 F3:AE3 F5:BD14">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:BE10 F2:AF3 AG2:BD4 F4:AE4 BE2:BG9 F6:BD9">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C23:C1048576 C2:C21">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C18:C1048576 C2:C16">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B22:D22"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B17:D17"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4026,37 +3449,37 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D23:D1048576 D2 D5:D21</xm:sqref>
+          <xm:sqref>D18:D1048576 D2:D3 D6:D16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2 B5:B15</xm:sqref>
+          <xm:sqref>B2:B3 B6:B10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
           <x14:formula1>
             <xm:f>[1]dropdown_lists!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>D3</xm:sqref>
+          <xm:sqref>D4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>[1]dropdown_lists!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>B3</xm:sqref>
+          <xm:sqref>B4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
           <x14:formula1>
             <xm:f>[2]dropdown_lists!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>D4</xm:sqref>
+          <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>[2]dropdown_lists!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>B4</xm:sqref>
+          <xm:sqref>B5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Remove over-writing of fundamental parameters
Disease-specific parameters being over-written removed from Philippines
spreadsheet.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="53">
   <si>
     <t>parameter</t>
   </si>
@@ -161,12 +161,6 @@
   </si>
   <si>
     <t>comorb_perc_hiv</t>
-  </si>
-  <si>
-    <t>tb_prop_early_progression_age5to15</t>
-  </si>
-  <si>
-    <t>tb_prop_early_progression_age15up</t>
   </si>
   <si>
     <t>program_perc_ipt_age0to5</t>
@@ -2207,10 +2201,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2254,7 +2248,7 @@
     </row>
     <row r="4" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="54" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="22">
         <v>1</v>
@@ -2284,7 +2278,7 @@
     </row>
     <row r="7" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="53" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" s="43">
         <v>5</v>
@@ -2319,39 +2313,23 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B10" s="44">
-        <v>0.26</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="44">
-        <v>0.03</v>
-      </c>
+      <c r="A11" s="55"/>
+      <c r="B11" s="21"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="44">
-        <v>2035</v>
-      </c>
+      <c r="A12" s="55"/>
+      <c r="B12" s="21"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="55"/>
-      <c r="B13" s="21"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
-      <c r="B14" s="21"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="56"/>
-      <c r="B15" s="57"/>
+      <c r="A13" s="56"/>
+      <c r="B13" s="57"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -2656,7 +2634,7 @@
     </row>
     <row r="3" spans="1:78" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -2693,7 +2671,7 @@
     </row>
     <row r="5" spans="1:78" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" s="47" t="s">
         <v>3</v>
@@ -3412,7 +3390,7 @@
     </row>
     <row r="20" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Xpert increase in smear-negative detection
Relatively complicated code to implement increase in smear-negative
detection.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -2364,7 +2364,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="BB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BQ13" sqref="BQ13"/>
+      <selection pane="bottomRight" activeCell="BG17" sqref="BG17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3302,9 +3302,6 @@
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="19"/>
-      <c r="BG16" s="12">
-        <v>2010</v>
-      </c>
     </row>
     <row r="17" spans="1:66" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">

</xml_diff>

<commit_message>
Implement prison risk group
Implemented for Philippines. Pretty simple stuff and no modifications in
the simulation for this population as yet.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
   <si>
     <t>parameter</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>program_perc_shortcourse_mdr</t>
+  </si>
+  <si>
+    <t>comorb_perc_prison</t>
   </si>
 </sst>
 </file>
@@ -1903,8 +1906,8 @@
       <sheetName val="dropdown_lists"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
@@ -2361,13 +2364,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BZ20"/>
+  <dimension ref="A1:BZ21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AQ5" sqref="AQ5"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3334,7 +3337,7 @@
         <v>42</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C18" s="35">
         <v>1</v>
@@ -3395,32 +3398,52 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:66" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="35">
+        <v>1</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="36">
+        <v>1</v>
+      </c>
+      <c r="BD20" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C21" s="2">
         <v>1</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E21" s="20">
         <v>1</v>
       </c>
-      <c r="AK20" s="1">
+      <c r="AK21" s="1">
         <v>1</v>
       </c>
-      <c r="AP20" s="1">
+      <c r="AP21" s="1">
         <v>0.75</v>
       </c>
-      <c r="AU20" s="1">
+      <c r="AU21" s="1">
         <v>0.62</v>
       </c>
-      <c r="BN20" s="1">
+      <c r="BN21" s="1">
         <v>0.01</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement ACF for at-risk groups
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
   <si>
     <t>parameter</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>comorb_perc_prison</t>
+  </si>
+  <si>
+    <t>program_perc_smearacf_prison</t>
   </si>
 </sst>
 </file>
@@ -2364,13 +2367,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BZ21"/>
+  <dimension ref="A1:BZ22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="BC2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="BM15" sqref="BM15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3112,7 +3115,7 @@
     </row>
     <row r="14" spans="1:78" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B14" s="35" t="s">
         <v>4</v>
@@ -3129,16 +3132,13 @@
       </c>
       <c r="BI14" s="52"/>
       <c r="BJ14" s="51"/>
-      <c r="BK14" s="37">
-        <v>50</v>
-      </c>
     </row>
     <row r="15" spans="1:78" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15" s="35">
         <v>1</v>
@@ -3146,160 +3146,19 @@
       <c r="D15" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="36">
-        <v>1</v>
-      </c>
-      <c r="H15" s="38">
-        <v>1</v>
-      </c>
-      <c r="J15" s="38">
-        <v>1.1289570744394</v>
-      </c>
-      <c r="K15" s="38">
-        <v>1.42215881727406</v>
-      </c>
-      <c r="L15" s="38">
-        <v>1.90118931222233</v>
-      </c>
-      <c r="M15" s="38">
-        <v>2.3081073919986701</v>
-      </c>
-      <c r="N15" s="38">
-        <v>2.4974653103104298</v>
-      </c>
-      <c r="O15" s="38">
-        <v>2.9115458645382701</v>
-      </c>
-      <c r="P15" s="38">
-        <v>3.90623450399154</v>
-      </c>
-      <c r="Q15" s="38">
-        <v>4.1703507493909102</v>
-      </c>
-      <c r="R15" s="38">
-        <v>4.55399078719985</v>
-      </c>
-      <c r="S15" s="38">
-        <v>5.0047790229916798</v>
-      </c>
-      <c r="T15" s="38">
-        <v>5.3718558386314896</v>
-      </c>
-      <c r="U15" s="38">
-        <v>6.3137212289735496</v>
-      </c>
-      <c r="V15" s="38">
-        <v>7.4628507238053698</v>
-      </c>
-      <c r="W15" s="38">
-        <v>8.4391855224587609</v>
-      </c>
-      <c r="X15" s="38">
-        <v>9.3018160392078606</v>
-      </c>
-      <c r="Y15" s="38">
-        <v>10.2347283365258</v>
-      </c>
-      <c r="Z15" s="38">
-        <v>15.386785740408699</v>
-      </c>
-      <c r="AA15" s="38">
-        <v>18.9416113416321</v>
-      </c>
-      <c r="AB15" s="38">
-        <v>19.1590871369295</v>
-      </c>
-      <c r="AC15" s="38">
-        <v>19.938817427385899</v>
-      </c>
-      <c r="AD15" s="38">
-        <v>22.702351313969601</v>
-      </c>
-      <c r="AE15" s="38">
-        <v>25.481798063623799</v>
-      </c>
-      <c r="AF15" s="38">
-        <v>28.584806362378998</v>
-      </c>
-      <c r="AG15" s="38">
-        <v>34.090656984785603</v>
-      </c>
-      <c r="AH15" s="38">
-        <v>37.0398409405256</v>
-      </c>
-      <c r="AI15" s="38">
-        <v>39.527551867219898</v>
-      </c>
-      <c r="AJ15" s="38">
-        <v>43.633070539419101</v>
-      </c>
-      <c r="AK15" s="38">
-        <v>46.6140802213001</v>
-      </c>
-      <c r="AL15" s="38">
-        <v>50.0989972337483</v>
-      </c>
-      <c r="AM15" s="38">
-        <v>52.899661134163203</v>
-      </c>
-      <c r="AN15" s="38">
-        <v>57.784910096818798</v>
-      </c>
-      <c r="AO15" s="38">
-        <v>61.2167842323652</v>
-      </c>
-      <c r="AP15" s="38">
-        <v>63.651452282157699</v>
-      </c>
-      <c r="AQ15" s="38">
-        <v>67.053941908713696</v>
-      </c>
-      <c r="AR15" s="38">
-        <v>68.8796680497925</v>
-      </c>
-      <c r="AS15" s="38">
-        <v>70.456431535269701</v>
-      </c>
-      <c r="AT15" s="38">
-        <v>73.858921161825705</v>
-      </c>
-      <c r="AU15" s="38">
-        <v>78.6721991701245</v>
-      </c>
-      <c r="AV15" s="38">
-        <v>82.987551867219906</v>
-      </c>
-      <c r="AW15" s="38">
-        <v>85.394190871369304</v>
-      </c>
-      <c r="AX15" s="38">
-        <v>92.448132780083</v>
-      </c>
-      <c r="AY15" s="38">
-        <v>96.348547717842294</v>
-      </c>
-      <c r="AZ15" s="38">
-        <v>100</v>
-      </c>
-      <c r="BA15" s="38">
-        <v>104.647302904564</v>
-      </c>
-      <c r="BB15" s="38">
-        <v>107.966804979253</v>
-      </c>
-      <c r="BC15" s="38">
-        <v>111.203319502075</v>
-      </c>
-      <c r="BD15" s="38">
-        <v>115.767634854772</v>
-      </c>
-      <c r="BE15" s="38">
-        <v>117.42738589211601</v>
+      <c r="E15" s="36"/>
+      <c r="BD15" s="37">
+        <v>0</v>
+      </c>
+      <c r="BI15" s="52"/>
+      <c r="BJ15" s="51"/>
+      <c r="BK15" s="37">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:78" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B16" s="35" t="s">
         <v>3</v>
@@ -3313,67 +3172,195 @@
       <c r="E16" s="36">
         <v>1</v>
       </c>
-      <c r="AE16" s="37">
+      <c r="H16" s="38">
         <v>1</v>
       </c>
-      <c r="AF16" s="37">
+      <c r="J16" s="38">
+        <v>1.1289570744394</v>
+      </c>
+      <c r="K16" s="38">
+        <v>1.42215881727406</v>
+      </c>
+      <c r="L16" s="38">
+        <v>1.90118931222233</v>
+      </c>
+      <c r="M16" s="38">
+        <v>2.3081073919986701</v>
+      </c>
+      <c r="N16" s="38">
+        <v>2.4974653103104298</v>
+      </c>
+      <c r="O16" s="38">
+        <v>2.9115458645382701</v>
+      </c>
+      <c r="P16" s="38">
+        <v>3.90623450399154</v>
+      </c>
+      <c r="Q16" s="38">
+        <v>4.1703507493909102</v>
+      </c>
+      <c r="R16" s="38">
+        <v>4.55399078719985</v>
+      </c>
+      <c r="S16" s="38">
+        <v>5.0047790229916798</v>
+      </c>
+      <c r="T16" s="38">
+        <v>5.3718558386314896</v>
+      </c>
+      <c r="U16" s="38">
+        <v>6.3137212289735496</v>
+      </c>
+      <c r="V16" s="38">
+        <v>7.4628507238053698</v>
+      </c>
+      <c r="W16" s="38">
+        <v>8.4391855224587609</v>
+      </c>
+      <c r="X16" s="38">
+        <v>9.3018160392078606</v>
+      </c>
+      <c r="Y16" s="38">
+        <v>10.2347283365258</v>
+      </c>
+      <c r="Z16" s="38">
+        <v>15.386785740408699</v>
+      </c>
+      <c r="AA16" s="38">
+        <v>18.9416113416321</v>
+      </c>
+      <c r="AB16" s="38">
+        <v>19.1590871369295</v>
+      </c>
+      <c r="AC16" s="38">
+        <v>19.938817427385899</v>
+      </c>
+      <c r="AD16" s="38">
+        <v>22.702351313969601</v>
+      </c>
+      <c r="AE16" s="38">
+        <v>25.481798063623799</v>
+      </c>
+      <c r="AF16" s="38">
+        <v>28.584806362378998</v>
+      </c>
+      <c r="AG16" s="38">
+        <v>34.090656984785603</v>
+      </c>
+      <c r="AH16" s="38">
+        <v>37.0398409405256</v>
+      </c>
+      <c r="AI16" s="38">
+        <v>39.527551867219898</v>
+      </c>
+      <c r="AJ16" s="38">
+        <v>43.633070539419101</v>
+      </c>
+      <c r="AK16" s="38">
+        <v>46.6140802213001</v>
+      </c>
+      <c r="AL16" s="38">
+        <v>50.0989972337483</v>
+      </c>
+      <c r="AM16" s="38">
+        <v>52.899661134163203</v>
+      </c>
+      <c r="AN16" s="38">
+        <v>57.784910096818798</v>
+      </c>
+      <c r="AO16" s="38">
+        <v>61.2167842323652</v>
+      </c>
+      <c r="AP16" s="38">
+        <v>63.651452282157699</v>
+      </c>
+      <c r="AQ16" s="38">
+        <v>67.053941908713696</v>
+      </c>
+      <c r="AR16" s="38">
+        <v>68.8796680497925</v>
+      </c>
+      <c r="AS16" s="38">
+        <v>70.456431535269701</v>
+      </c>
+      <c r="AT16" s="38">
+        <v>73.858921161825705</v>
+      </c>
+      <c r="AU16" s="38">
+        <v>78.6721991701245</v>
+      </c>
+      <c r="AV16" s="38">
+        <v>82.987551867219906</v>
+      </c>
+      <c r="AW16" s="38">
+        <v>85.394190871369304</v>
+      </c>
+      <c r="AX16" s="38">
+        <v>92.448132780083</v>
+      </c>
+      <c r="AY16" s="38">
+        <v>96.348547717842294</v>
+      </c>
+      <c r="AZ16" s="38">
+        <v>100</v>
+      </c>
+      <c r="BA16" s="38">
+        <v>104.647302904564</v>
+      </c>
+      <c r="BB16" s="38">
+        <v>107.966804979253</v>
+      </c>
+      <c r="BC16" s="38">
+        <v>111.203319502075</v>
+      </c>
+      <c r="BD16" s="38">
+        <v>115.767634854772</v>
+      </c>
+      <c r="BE16" s="38">
+        <v>117.42738589211601</v>
+      </c>
+    </row>
+    <row r="17" spans="1:66" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="35">
+        <v>1</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="36">
+        <v>1</v>
+      </c>
+      <c r="AE17" s="37">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="37">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BA16" s="37">
+      <c r="BA17" s="37">
         <v>3.11</v>
       </c>
     </row>
-    <row r="17" spans="1:66" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+    <row r="18" spans="1:66" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="19"/>
-    </row>
-    <row r="18" spans="1:66" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="35">
-        <v>1</v>
-      </c>
-      <c r="D18" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="36"/>
-      <c r="AE18" s="37">
-        <v>0</v>
-      </c>
-      <c r="AN18" s="37">
-        <v>3.1</v>
-      </c>
-      <c r="AS18" s="37">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="AX18" s="37">
-        <v>5.2</v>
-      </c>
-      <c r="BC18" s="37">
-        <v>5.4</v>
-      </c>
-      <c r="BD18" s="37">
-        <v>5.9</v>
-      </c>
-      <c r="BE18" s="37">
-        <v>5.9</v>
-      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:66" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C19" s="35">
         <v>1</v>
@@ -3382,28 +3369,34 @@
         <v>3</v>
       </c>
       <c r="E19" s="36"/>
-      <c r="W19" s="37">
-        <v>0.1</v>
-      </c>
-      <c r="AH19" s="37">
-        <v>0.1</v>
-      </c>
-      <c r="AP19" s="37">
-        <v>0.1</v>
-      </c>
-      <c r="AY19" s="37">
-        <v>0.1</v>
+      <c r="AE19" s="37">
+        <v>0</v>
+      </c>
+      <c r="AN19" s="37">
+        <v>3.1</v>
+      </c>
+      <c r="AS19" s="37">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AX19" s="37">
+        <v>5.2</v>
+      </c>
+      <c r="BC19" s="37">
+        <v>5.4</v>
+      </c>
+      <c r="BD19" s="37">
+        <v>5.9</v>
       </c>
       <c r="BE19" s="37">
-        <v>0.1</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="20" spans="1:66" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" s="35">
         <v>1</v>
@@ -3411,39 +3404,69 @@
       <c r="D20" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="36">
+      <c r="E20" s="36"/>
+      <c r="W20" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="AH20" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="AP20" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="AY20" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="BE20" s="37">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:66" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="35">
         <v>1</v>
       </c>
-      <c r="BD20" s="37">
+      <c r="D21" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="36">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="BD21" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C22" s="2">
         <v>1</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E22" s="20">
         <v>1</v>
       </c>
-      <c r="AK21" s="1">
+      <c r="AK22" s="1">
         <v>1</v>
       </c>
-      <c r="AP21" s="1">
+      <c r="AP22" s="1">
         <v>0.75</v>
       </c>
-      <c r="AU21" s="1">
+      <c r="AU22" s="1">
         <v>0.62</v>
       </c>
-      <c r="BN21" s="1">
+      <c r="BN22" s="1">
         <v>0.01</v>
       </c>
     </row>
@@ -3458,11 +3481,11 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C18:C1048576 C2:C16">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C19:C1048576 C2:C17">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B17:D17"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B18:D18"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3473,7 +3496,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D18:D1048576 D2 D5:D16</xm:sqref>
+          <xm:sqref>D19:D1048576 D2 D5:D17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Apply paediatric under-reporting to notifications
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="555" windowWidth="20370" windowHeight="6600" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="555" windowWidth="20370" windowHeight="6600" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2102,7 +2102,7 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -2130,7 +2130,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="8">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -2150,7 +2150,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="9">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -2170,7 +2170,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="18">
-        <v>22000000</v>
+        <v>44000000</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -2251,7 +2251,7 @@
   </sheetPr>
   <dimension ref="A1:BO18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Finished cost inputs for BCG and IPT
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="555" windowWidth="20370" windowHeight="6600" tabRatio="807" activeTab="1"/>
   </bookViews>
@@ -14,12 +19,12 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
   <si>
     <t>parameter</t>
   </si>
@@ -151,6 +156,27 @@
   </si>
   <si>
     <t>program_perc_smearacf_indigenous</t>
+  </si>
+  <si>
+    <t>scenario_8</t>
+  </si>
+  <si>
+    <t>scenario_9</t>
+  </si>
+  <si>
+    <t>econ_unitcost_ipt</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_ipt</t>
+  </si>
+  <si>
+    <t>econ_startupcost_ipt</t>
+  </si>
+  <si>
+    <t>econ_startupduration_ipt</t>
+  </si>
+  <si>
+    <t>econ_saturation_ipt</t>
   </si>
 </sst>
 </file>
@@ -240,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +282,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB9DAED"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1018,7 +1056,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1052,6 +1090,14 @@
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="665">
     <cellStyle name="Comma" xfId="664" builtinId="3"/>
@@ -1742,8 +1788,8 @@
       <sheetName val="dropdown_lists"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
@@ -1793,7 +1839,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1828,7 +1874,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2040,10 +2086,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2134,8 +2180,59 @@
       <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
+      <c r="A9" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="26">
+        <v>26.22</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="26">
+        <v>0</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="26">
+        <v>265450</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="26">
+        <v>3</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="26">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -2163,13 +2260,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BI18"/>
+  <dimension ref="A1:BK18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AW2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BA26" sqref="BA26"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2194,11 +2291,12 @@
     <col min="51" max="52" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="53" max="54" width="7.85546875" style="7" customWidth="1"/>
     <col min="55" max="55" width="14" style="7" customWidth="1"/>
-    <col min="56" max="61" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="62" max="16384" width="9.140625" style="7"/>
+    <col min="56" max="62" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="14.28515625" style="7" customWidth="1"/>
+    <col min="64" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
@@ -2382,8 +2480,14 @@
       <c r="BI1" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:61" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BJ1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:63" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>24</v>
       </c>
@@ -2398,8 +2502,11 @@
       </c>
       <c r="E2" s="1"/>
       <c r="BC2" s="13"/>
-    </row>
-    <row r="3" spans="1:61" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BJ2" s="25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:63" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
@@ -2440,7 +2547,9 @@
       <c r="AB3" s="7"/>
       <c r="AC3" s="7"/>
       <c r="AD3" s="7"/>
-      <c r="AE3" s="7"/>
+      <c r="AE3" s="7">
+        <v>0</v>
+      </c>
       <c r="AF3" s="7"/>
       <c r="AG3" s="7"/>
       <c r="AH3" s="7"/>
@@ -2456,18 +2565,23 @@
       <c r="AR3" s="7"/>
       <c r="AS3" s="7"/>
       <c r="AT3" s="7"/>
-      <c r="AU3" s="7"/>
+      <c r="AU3" s="7">
+        <v>0</v>
+      </c>
       <c r="AV3" s="7"/>
       <c r="AW3" s="7"/>
       <c r="AX3" s="7"/>
       <c r="AY3" s="7"/>
       <c r="AZ3" s="7"/>
       <c r="BA3" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BE3" s="13"/>
-    </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="BK3" s="25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
@@ -2496,7 +2610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
@@ -2533,7 +2647,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
@@ -2566,7 +2680,7 @@
       <c r="AY6" s="8"/>
       <c r="AZ6" s="8"/>
     </row>
-    <row r="7" spans="1:61" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>26</v>
       </c>
@@ -2590,7 +2704,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -2612,7 +2726,7 @@
       <c r="BF8" s="14"/>
       <c r="BG8" s="14"/>
     </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
@@ -2633,7 +2747,7 @@
       </c>
       <c r="BG9" s="14"/>
     </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>41</v>
       </c>
@@ -2654,7 +2768,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
@@ -2676,7 +2790,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>39</v>
       </c>
@@ -2698,7 +2812,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -2862,7 +2976,7 @@
         <v>117.42738589211601</v>
       </c>
     </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
@@ -2894,7 +3008,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>34</v>
       </c>
@@ -2911,7 +3025,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Finsh cost input for short course MDR
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
   <si>
     <t>parameter</t>
   </si>
@@ -207,6 +207,39 @@
   </si>
   <si>
     <t>econ_unitcost_xpert</t>
+  </si>
+  <si>
+    <t>econ_unitcost_xpertacf_prison</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_xpertacf_prison</t>
+  </si>
+  <si>
+    <t>econ_startupcost_xpertacf_prison</t>
+  </si>
+  <si>
+    <t>econ_startupduration_xpertacf_prison</t>
+  </si>
+  <si>
+    <t>econ_saturation_xpertacf_prison</t>
+  </si>
+  <si>
+    <t>program_perc_xpertacf_prison</t>
+  </si>
+  <si>
+    <t>econ_unitcost_shortcourse_mdr</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_shortcourse_mdr</t>
+  </si>
+  <si>
+    <t>econ_startupcost_shortcourse_mdr</t>
+  </si>
+  <si>
+    <t>econ_startupduration_shortcourse_mdr</t>
+  </si>
+  <si>
+    <t>econ_saturation_shortcourse_mdr</t>
   </si>
 </sst>
 </file>
@@ -296,7 +329,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,12 +361,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -347,6 +374,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1110,7 +1155,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1152,17 +1197,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="6" borderId="0" xfId="664" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="7" borderId="0" xfId="664" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="7"/>
     </xf>
   </cellXfs>
   <cellStyles count="665">
@@ -2152,10 +2206,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2301,10 +2355,10 @@
       <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="32">
+      <c r="B14" s="31">
         <v>16</v>
       </c>
       <c r="C14" s="28"/>
@@ -2312,75 +2366,155 @@
       <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="31">
+      <c r="B15" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="33">
+      <c r="B16" s="32">
         <v>11575186.195826644</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="30">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="31">
+      <c r="B18" s="30">
         <v>1.0009999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="35">
+      <c r="B19" s="34">
         <v>30.42</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="35">
+      <c r="B20" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="35">
+      <c r="B21" s="34">
         <v>140500</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="35">
+      <c r="B22" s="34">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="35">
+      <c r="B23" s="34">
         <v>0.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="35">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="41">
+        <v>3837.6979926791319</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="40">
+        <v>1144060.9951845906</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="38">
+        <v>0.90010000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2409,13 +2543,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BK18"/>
+  <dimension ref="A1:BK19"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AJ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O9" sqref="O9"/>
+      <selection pane="bottomRight" activeCell="BH13" sqref="BH13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2650,8 +2784,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="BC2" s="13"/>
-      <c r="BJ2" s="25">
+      <c r="BC2" s="25">
         <v>100</v>
       </c>
     </row>
@@ -2725,10 +2858,10 @@
       <c r="BA3" s="7">
         <v>5</v>
       </c>
+      <c r="BD3" s="25">
+        <v>90</v>
+      </c>
       <c r="BE3" s="13"/>
-      <c r="BK3" s="25">
-        <v>90</v>
-      </c>
     </row>
     <row r="4" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -2754,9 +2887,6 @@
       </c>
       <c r="AW4" s="7">
         <v>30</v>
-      </c>
-      <c r="BC4" s="7">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:63" x14ac:dyDescent="0.25">
@@ -2849,7 +2979,7 @@
       <c r="AY7" s="9">
         <v>2.8</v>
       </c>
-      <c r="BD7" s="29">
+      <c r="BE7" s="36">
         <v>100</v>
       </c>
     </row>
@@ -2869,14 +2999,11 @@
       <c r="BA8" s="7">
         <v>0</v>
       </c>
-      <c r="BE8" s="7">
-        <v>50</v>
-      </c>
       <c r="BF8" s="14"/>
       <c r="BG8" s="14"/>
     </row>
     <row r="9" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="33" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -2897,17 +3024,17 @@
       <c r="BA9" s="7">
         <v>0</v>
       </c>
-      <c r="BF9" s="36">
+      <c r="BF9" s="37">
         <v>80</v>
       </c>
       <c r="BG9" s="14"/>
     </row>
     <row r="10" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>40</v>
+      <c r="A10" s="33" t="s">
+        <v>66</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -2915,17 +3042,23 @@
       <c r="D10" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="7">
+        <v>0</v>
+      </c>
       <c r="BA10" s="7">
         <v>0</v>
       </c>
       <c r="BF10" s="14"/>
-      <c r="BG10" s="14">
-        <v>75</v>
+      <c r="BG10" s="37">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>4</v>
@@ -2941,13 +3074,10 @@
       </c>
       <c r="BF11" s="14"/>
       <c r="BG11" s="14"/>
-      <c r="BH11" s="7">
-        <v>75</v>
-      </c>
     </row>
     <row r="12" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
@@ -2963,16 +3093,13 @@
       </c>
       <c r="BF12" s="14"/>
       <c r="BG12" s="14"/>
-      <c r="BI12" s="7">
-        <v>75</v>
-      </c>
     </row>
     <row r="13" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
@@ -2980,163 +3107,21 @@
       <c r="D13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="6">
-        <v>1</v>
-      </c>
-      <c r="F13" s="15">
-        <v>1</v>
-      </c>
-      <c r="G13" s="15">
-        <v>1.1289570744394</v>
-      </c>
-      <c r="H13" s="15">
-        <v>1.42215881727406</v>
-      </c>
-      <c r="I13" s="15">
-        <v>1.90118931222233</v>
-      </c>
-      <c r="J13" s="15">
-        <v>2.3081073919986701</v>
-      </c>
-      <c r="K13" s="15">
-        <v>2.4974653103104298</v>
-      </c>
-      <c r="L13" s="15">
-        <v>2.9115458645382701</v>
-      </c>
-      <c r="M13" s="15">
-        <v>3.90623450399154</v>
-      </c>
-      <c r="N13" s="15">
-        <v>4.1703507493909102</v>
-      </c>
-      <c r="O13" s="15">
-        <v>4.55399078719985</v>
-      </c>
-      <c r="P13" s="15">
-        <v>5.0047790229916798</v>
-      </c>
-      <c r="Q13" s="15">
-        <v>5.3718558386314896</v>
-      </c>
-      <c r="R13" s="15">
-        <v>6.3137212289735496</v>
-      </c>
-      <c r="S13" s="15">
-        <v>7.4628507238053698</v>
-      </c>
-      <c r="T13" s="15">
-        <v>8.4391855224587609</v>
-      </c>
-      <c r="U13" s="15">
-        <v>9.3018160392078606</v>
-      </c>
-      <c r="V13" s="15">
-        <v>10.2347283365258</v>
-      </c>
-      <c r="W13" s="15">
-        <v>15.386785740408699</v>
-      </c>
-      <c r="X13" s="15">
-        <v>18.9416113416321</v>
-      </c>
-      <c r="Y13" s="15">
-        <v>19.1590871369295</v>
-      </c>
-      <c r="Z13" s="15">
-        <v>19.938817427385899</v>
-      </c>
-      <c r="AA13" s="15">
-        <v>22.702351313969601</v>
-      </c>
-      <c r="AB13" s="15">
-        <v>25.481798063623799</v>
-      </c>
-      <c r="AC13" s="15">
-        <v>28.584806362378998</v>
-      </c>
-      <c r="AD13" s="15">
-        <v>34.090656984785603</v>
-      </c>
-      <c r="AE13" s="15">
-        <v>37.0398409405256</v>
-      </c>
-      <c r="AF13" s="15">
-        <v>39.527551867219898</v>
-      </c>
-      <c r="AG13" s="15">
-        <v>43.633070539419101</v>
-      </c>
-      <c r="AH13" s="15">
-        <v>46.6140802213001</v>
-      </c>
-      <c r="AI13" s="15">
-        <v>50.0989972337483</v>
-      </c>
-      <c r="AJ13" s="15">
-        <v>52.899661134163203</v>
-      </c>
-      <c r="AK13" s="15">
-        <v>57.784910096818798</v>
-      </c>
-      <c r="AL13" s="15">
-        <v>61.2167842323652</v>
-      </c>
-      <c r="AM13" s="15">
-        <v>63.651452282157699</v>
-      </c>
-      <c r="AN13" s="15">
-        <v>67.053941908713696</v>
-      </c>
-      <c r="AO13" s="15">
-        <v>68.8796680497925</v>
-      </c>
-      <c r="AP13" s="15">
-        <v>70.456431535269701</v>
-      </c>
-      <c r="AQ13" s="15">
-        <v>73.858921161825705</v>
-      </c>
-      <c r="AR13" s="15">
-        <v>78.6721991701245</v>
-      </c>
-      <c r="AS13" s="15">
-        <v>82.987551867219906</v>
-      </c>
-      <c r="AT13" s="15">
-        <v>85.394190871369304</v>
-      </c>
-      <c r="AU13" s="15">
-        <v>92.448132780083</v>
-      </c>
-      <c r="AV13" s="15">
-        <v>96.348547717842294</v>
-      </c>
-      <c r="AW13" s="15">
-        <v>100</v>
-      </c>
-      <c r="AX13" s="15">
-        <v>104.647302904564</v>
-      </c>
-      <c r="AY13" s="15">
-        <v>107.966804979253</v>
-      </c>
-      <c r="AZ13" s="15">
-        <v>111.203319502075</v>
-      </c>
-      <c r="BA13" s="15">
-        <v>115.767634854772</v>
-      </c>
-      <c r="BB13" s="15">
-        <v>117.42738589211601</v>
+      <c r="BA13" s="7">
+        <v>0</v>
+      </c>
+      <c r="BF13" s="14"/>
+      <c r="BG13" s="14"/>
+      <c r="BH13" s="39">
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
@@ -3144,31 +3129,163 @@
       <c r="D14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB14" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK14" s="7">
-        <v>3.1</v>
-      </c>
-      <c r="AP14" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="AU14" s="7">
-        <v>5.2</v>
-      </c>
-      <c r="AZ14" s="7">
-        <v>5.4</v>
-      </c>
-      <c r="BB14" s="7">
-        <v>5.9</v>
+      <c r="E14" s="6">
+        <v>1</v>
+      </c>
+      <c r="F14" s="15">
+        <v>1</v>
+      </c>
+      <c r="G14" s="15">
+        <v>1.1289570744394</v>
+      </c>
+      <c r="H14" s="15">
+        <v>1.42215881727406</v>
+      </c>
+      <c r="I14" s="15">
+        <v>1.90118931222233</v>
+      </c>
+      <c r="J14" s="15">
+        <v>2.3081073919986701</v>
+      </c>
+      <c r="K14" s="15">
+        <v>2.4974653103104298</v>
+      </c>
+      <c r="L14" s="15">
+        <v>2.9115458645382701</v>
+      </c>
+      <c r="M14" s="15">
+        <v>3.90623450399154</v>
+      </c>
+      <c r="N14" s="15">
+        <v>4.1703507493909102</v>
+      </c>
+      <c r="O14" s="15">
+        <v>4.55399078719985</v>
+      </c>
+      <c r="P14" s="15">
+        <v>5.0047790229916798</v>
+      </c>
+      <c r="Q14" s="15">
+        <v>5.3718558386314896</v>
+      </c>
+      <c r="R14" s="15">
+        <v>6.3137212289735496</v>
+      </c>
+      <c r="S14" s="15">
+        <v>7.4628507238053698</v>
+      </c>
+      <c r="T14" s="15">
+        <v>8.4391855224587609</v>
+      </c>
+      <c r="U14" s="15">
+        <v>9.3018160392078606</v>
+      </c>
+      <c r="V14" s="15">
+        <v>10.2347283365258</v>
+      </c>
+      <c r="W14" s="15">
+        <v>15.386785740408699</v>
+      </c>
+      <c r="X14" s="15">
+        <v>18.9416113416321</v>
+      </c>
+      <c r="Y14" s="15">
+        <v>19.1590871369295</v>
+      </c>
+      <c r="Z14" s="15">
+        <v>19.938817427385899</v>
+      </c>
+      <c r="AA14" s="15">
+        <v>22.702351313969601</v>
+      </c>
+      <c r="AB14" s="15">
+        <v>25.481798063623799</v>
+      </c>
+      <c r="AC14" s="15">
+        <v>28.584806362378998</v>
+      </c>
+      <c r="AD14" s="15">
+        <v>34.090656984785603</v>
+      </c>
+      <c r="AE14" s="15">
+        <v>37.0398409405256</v>
+      </c>
+      <c r="AF14" s="15">
+        <v>39.527551867219898</v>
+      </c>
+      <c r="AG14" s="15">
+        <v>43.633070539419101</v>
+      </c>
+      <c r="AH14" s="15">
+        <v>46.6140802213001</v>
+      </c>
+      <c r="AI14" s="15">
+        <v>50.0989972337483</v>
+      </c>
+      <c r="AJ14" s="15">
+        <v>52.899661134163203</v>
+      </c>
+      <c r="AK14" s="15">
+        <v>57.784910096818798</v>
+      </c>
+      <c r="AL14" s="15">
+        <v>61.2167842323652</v>
+      </c>
+      <c r="AM14" s="15">
+        <v>63.651452282157699</v>
+      </c>
+      <c r="AN14" s="15">
+        <v>67.053941908713696</v>
+      </c>
+      <c r="AO14" s="15">
+        <v>68.8796680497925</v>
+      </c>
+      <c r="AP14" s="15">
+        <v>70.456431535269701</v>
+      </c>
+      <c r="AQ14" s="15">
+        <v>73.858921161825705</v>
+      </c>
+      <c r="AR14" s="15">
+        <v>78.6721991701245</v>
+      </c>
+      <c r="AS14" s="15">
+        <v>82.987551867219906</v>
+      </c>
+      <c r="AT14" s="15">
+        <v>85.394190871369304</v>
+      </c>
+      <c r="AU14" s="15">
+        <v>92.448132780083</v>
+      </c>
+      <c r="AV14" s="15">
+        <v>96.348547717842294</v>
+      </c>
+      <c r="AW14" s="15">
+        <v>100</v>
+      </c>
+      <c r="AX14" s="15">
+        <v>104.647302904564</v>
+      </c>
+      <c r="AY14" s="15">
+        <v>107.966804979253</v>
+      </c>
+      <c r="AZ14" s="15">
+        <v>111.203319502075</v>
+      </c>
+      <c r="BA14" s="15">
+        <v>115.767634854772</v>
+      </c>
+      <c r="BB14" s="15">
+        <v>117.42738589211601</v>
       </c>
     </row>
     <row r="15" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15" s="5">
         <v>1</v>
@@ -3176,16 +3293,31 @@
       <c r="D15" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="AB15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="AP15" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AU15" s="7">
+        <v>5.2</v>
+      </c>
+      <c r="AZ15" s="7">
+        <v>5.4</v>
+      </c>
       <c r="BB15" s="7">
-        <v>0.1</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="16" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
@@ -3193,16 +3325,13 @@
       <c r="D16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AW16" s="7">
-        <v>0.112</v>
-      </c>
       <c r="BB16" s="7">
-        <v>0.153</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>4</v>
@@ -3213,45 +3342,65 @@
       <c r="D17" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="AW17" s="7">
+        <v>0.112</v>
+      </c>
       <c r="BB17" s="7">
+        <v>0.153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BB18" s="7">
         <f xml:space="preserve"> 7/98*100</f>
         <v>7.1428571428571423</v>
       </c>
     </row>
-    <row r="18" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="19" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C19" s="5">
         <v>1</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E19" s="6">
         <v>1</v>
       </c>
-      <c r="AH18" s="7">
+      <c r="AH19" s="7">
         <v>1</v>
       </c>
-      <c r="AM18" s="7">
+      <c r="AM19" s="7">
         <v>0.75</v>
       </c>
-      <c r="AR18" s="7">
+      <c r="AR19" s="7">
         <v>0.62</v>
       </c>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="4">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BC7:BD7 F3:BA3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:BA3 BE7 BC7">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:D1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB2:BD6 F2:BA2 F7:BB7 F4:BA6">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:BA6 F2:BA2 F7:BB7 BB2:BB6 BC3:BC6 BD2 BD4:BD6">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
"Turn on" load data for population groups
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="555" windowWidth="20370" windowHeight="6600" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="555" windowWidth="20370" windowHeight="6600" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2212,8 +2212,8 @@
   </sheetPr>
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2549,11 +2549,11 @@
   </sheetPr>
   <dimension ref="A1:BK19"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AJ2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BH13" sqref="BH13"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3103,7 +3103,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
@@ -3289,7 +3289,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15" s="5">
         <v>1</v>
@@ -3338,7 +3338,7 @@
         <v>39</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
@@ -3358,7 +3358,7 @@
         <v>41</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
Some update to cost data
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="555" windowWidth="20370" windowHeight="6600" tabRatio="807" activeTab="1"/>
   </bookViews>
@@ -1919,7 +1924,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1954,7 +1959,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2169,7 +2174,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2315,7 +2320,7 @@
         <v>56</v>
       </c>
       <c r="B13" s="30">
-        <v>16</v>
+        <v>30.26</v>
       </c>
       <c r="C13" s="27"/>
       <c r="D13" s="27"/>
@@ -2342,7 +2347,7 @@
         <v>48</v>
       </c>
       <c r="B16" s="29">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2358,7 +2363,7 @@
         <v>51</v>
       </c>
       <c r="B18" s="33">
-        <v>30.42</v>
+        <v>473</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2374,7 +2379,7 @@
         <v>53</v>
       </c>
       <c r="B20" s="33">
-        <v>140500</v>
+        <v>142024</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2398,7 +2403,7 @@
         <v>57</v>
       </c>
       <c r="B23" s="34">
-        <v>20</v>
+        <v>30.26</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2414,7 +2419,7 @@
         <v>59</v>
       </c>
       <c r="B25" s="34">
-        <v>0</v>
+        <v>662</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2502,10 +2507,10 @@
   <dimension ref="A1:BH18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AV2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BE1" sqref="BE1"/>
+      <selection pane="bottomRight" activeCell="BB17" sqref="BB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2970,7 +2975,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -3156,7 +3161,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
@@ -3205,7 +3210,7 @@
         <v>37</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
@@ -3225,7 +3230,7 @@
         <v>39</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
@@ -3234,7 +3239,7 @@
         <v>3</v>
       </c>
       <c r="BB17" s="7">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:54" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Convert low quality improvement to intervention
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="555" windowWidth="20370" windowHeight="6600" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="555" windowWidth="20370" windowHeight="6600" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
   <si>
     <t>parameter</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>age_breakpoints</t>
+  </si>
+  <si>
+    <t>program_perc_engage_lowquality</t>
+  </si>
+  <si>
+    <t>scenario_7</t>
   </si>
 </sst>
 </file>
@@ -2063,7 +2069,7 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -2329,13 +2335,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BH16"/>
+  <dimension ref="A1:BI17"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AV2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BE7" sqref="BE7"/>
+      <selection pane="bottomRight" activeCell="BI2" sqref="BI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2359,12 +2365,12 @@
     <col min="40" max="50" width="7" style="7" customWidth="1"/>
     <col min="51" max="52" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="53" max="54" width="7.85546875" style="7" customWidth="1"/>
-    <col min="55" max="55" width="14" style="7" customWidth="1"/>
-    <col min="56" max="60" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="61" max="16384" width="9.140625" style="7"/>
+    <col min="55" max="56" width="14" style="7" customWidth="1"/>
+    <col min="57" max="61" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="62" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
@@ -2545,8 +2551,11 @@
       <c r="BH1" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:60" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BI1" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:61" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -2563,8 +2572,9 @@
       <c r="BC2" s="27">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="BD2" s="27"/>
+    </row>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -2590,46 +2600,29 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="5">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AH4" s="8"/>
-      <c r="AI4" s="8"/>
-      <c r="AJ4" s="8"/>
-      <c r="AK4" s="8"/>
-      <c r="AL4" s="8"/>
-      <c r="AM4" s="8"/>
-      <c r="AN4" s="8"/>
-      <c r="AO4" s="8"/>
-      <c r="AP4" s="8"/>
-      <c r="AQ4" s="8"/>
-      <c r="AR4" s="8"/>
-      <c r="AS4" s="8"/>
-      <c r="AT4" s="8"/>
-      <c r="AU4" s="8"/>
-      <c r="AV4" s="8"/>
-      <c r="AW4" s="8"/>
-      <c r="AX4" s="8"/>
-      <c r="AY4" s="8">
-        <v>93</v>
-      </c>
-      <c r="AZ4" s="8">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="BB4" s="7">
+        <v>0</v>
+      </c>
+      <c r="BD4" s="7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>3</v>
@@ -2640,82 +2633,91 @@
       <c r="D5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AH5" s="9"/>
+      <c r="AH5" s="8"/>
       <c r="AI5" s="8"/>
       <c r="AJ5" s="8"/>
       <c r="AK5" s="8"/>
       <c r="AL5" s="8"/>
-      <c r="AM5" s="9"/>
+      <c r="AM5" s="8"/>
       <c r="AN5" s="8"/>
       <c r="AO5" s="8"/>
       <c r="AP5" s="8"/>
       <c r="AQ5" s="8"/>
-      <c r="AR5" s="9"/>
+      <c r="AR5" s="8"/>
       <c r="AS5" s="8"/>
       <c r="AT5" s="8"/>
       <c r="AU5" s="8"/>
       <c r="AV5" s="8"/>
-      <c r="AW5" s="9"/>
+      <c r="AW5" s="8"/>
       <c r="AX5" s="8"/>
-      <c r="AY5" s="8"/>
-      <c r="AZ5" s="8"/>
-    </row>
-    <row r="6" spans="1:60" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AY5" s="8">
+        <v>93</v>
+      </c>
+      <c r="AZ5" s="8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="8"/>
+      <c r="AJ6" s="8"/>
+      <c r="AK6" s="8"/>
+      <c r="AL6" s="8"/>
+      <c r="AM6" s="9"/>
+      <c r="AN6" s="8"/>
+      <c r="AO6" s="8"/>
+      <c r="AP6" s="8"/>
+      <c r="AQ6" s="8"/>
+      <c r="AR6" s="9"/>
+      <c r="AS6" s="8"/>
+      <c r="AT6" s="8"/>
+      <c r="AU6" s="8"/>
+      <c r="AV6" s="8"/>
+      <c r="AW6" s="9"/>
+      <c r="AX6" s="8"/>
+      <c r="AY6" s="8"/>
+      <c r="AZ6" s="8"/>
+    </row>
+    <row r="7" spans="1:61" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C7" s="12">
         <v>1</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="AW6" s="9">
+      <c r="E7" s="1"/>
+      <c r="AW7" s="9">
         <v>0</v>
       </c>
-      <c r="AY6" s="9">
+      <c r="AY7" s="9">
         <v>2.8</v>
       </c>
-      <c r="BD6" s="9">
+      <c r="BE7" s="9">
         <v>100</v>
       </c>
-      <c r="BE6" s="27"/>
-    </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="BF7" s="27"/>
+    </row>
+    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="7">
-        <v>0</v>
-      </c>
-      <c r="BB7" s="7">
-        <v>0</v>
-      </c>
-      <c r="BE7" s="7">
-        <v>80</v>
-      </c>
-      <c r="BF7" s="13"/>
-      <c r="BG7" s="13"/>
-    </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>3</v>
@@ -2735,17 +2737,18 @@
       <c r="BB8" s="7">
         <v>0</v>
       </c>
-      <c r="BF8" s="13">
+      <c r="BF8" s="7">
         <v>80</v>
       </c>
       <c r="BG8" s="13"/>
-    </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="BH8" s="13"/>
+    </row>
+    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -2753,20 +2756,26 @@
       <c r="D9" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="7">
+        <v>0</v>
+      </c>
       <c r="BB9" s="7">
         <v>0</v>
       </c>
-      <c r="BF9" s="13"/>
       <c r="BG9" s="13">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="BH9" s="13"/>
+    </row>
+    <row r="10" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -2777,15 +2786,14 @@
       <c r="BB10" s="7">
         <v>0</v>
       </c>
-      <c r="BF10" s="13"/>
       <c r="BG10" s="13"/>
       <c r="BH10" s="13">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>3</v>
@@ -2796,160 +2804,18 @@
       <c r="D11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="6">
-        <v>1</v>
-      </c>
-      <c r="F11" s="14">
-        <v>1</v>
-      </c>
-      <c r="G11" s="14">
-        <v>1.1289570744394</v>
-      </c>
-      <c r="H11" s="14">
-        <v>1.42215881727406</v>
-      </c>
-      <c r="I11" s="14">
-        <v>1.90118931222233</v>
-      </c>
-      <c r="J11" s="14">
-        <v>2.3081073919986701</v>
-      </c>
-      <c r="K11" s="14">
-        <v>2.4974653103104298</v>
-      </c>
-      <c r="L11" s="14">
-        <v>2.9115458645382701</v>
-      </c>
-      <c r="M11" s="14">
-        <v>3.90623450399154</v>
-      </c>
-      <c r="N11" s="14">
-        <v>4.1703507493909102</v>
-      </c>
-      <c r="O11" s="14">
-        <v>4.55399078719985</v>
-      </c>
-      <c r="P11" s="14">
-        <v>5.0047790229916798</v>
-      </c>
-      <c r="Q11" s="14">
-        <v>5.3718558386314896</v>
-      </c>
-      <c r="R11" s="14">
-        <v>6.3137212289735496</v>
-      </c>
-      <c r="S11" s="14">
-        <v>7.4628507238053698</v>
-      </c>
-      <c r="T11" s="14">
-        <v>8.4391855224587609</v>
-      </c>
-      <c r="U11" s="14">
-        <v>9.3018160392078606</v>
-      </c>
-      <c r="V11" s="14">
-        <v>10.2347283365258</v>
-      </c>
-      <c r="W11" s="14">
-        <v>15.386785740408699</v>
-      </c>
-      <c r="X11" s="14">
-        <v>18.9416113416321</v>
-      </c>
-      <c r="Y11" s="14">
-        <v>19.1590871369295</v>
-      </c>
-      <c r="Z11" s="14">
-        <v>19.938817427385899</v>
-      </c>
-      <c r="AA11" s="14">
-        <v>22.702351313969601</v>
-      </c>
-      <c r="AB11" s="14">
-        <v>25.481798063623799</v>
-      </c>
-      <c r="AC11" s="14">
-        <v>28.584806362378998</v>
-      </c>
-      <c r="AD11" s="14">
-        <v>34.090656984785603</v>
-      </c>
-      <c r="AE11" s="14">
-        <v>37.0398409405256</v>
-      </c>
-      <c r="AF11" s="14">
-        <v>39.527551867219898</v>
-      </c>
-      <c r="AG11" s="14">
-        <v>43.633070539419101</v>
-      </c>
-      <c r="AH11" s="14">
-        <v>46.6140802213001</v>
-      </c>
-      <c r="AI11" s="14">
-        <v>50.0989972337483</v>
-      </c>
-      <c r="AJ11" s="14">
-        <v>52.899661134163203</v>
-      </c>
-      <c r="AK11" s="14">
-        <v>57.784910096818798</v>
-      </c>
-      <c r="AL11" s="14">
-        <v>61.2167842323652</v>
-      </c>
-      <c r="AM11" s="14">
-        <v>63.651452282157699</v>
-      </c>
-      <c r="AN11" s="14">
-        <v>67.053941908713696</v>
-      </c>
-      <c r="AO11" s="14">
-        <v>68.8796680497925</v>
-      </c>
-      <c r="AP11" s="14">
-        <v>70.456431535269701</v>
-      </c>
-      <c r="AQ11" s="14">
-        <v>73.858921161825705</v>
-      </c>
-      <c r="AR11" s="14">
-        <v>78.6721991701245</v>
-      </c>
-      <c r="AS11" s="14">
-        <v>82.987551867219906</v>
-      </c>
-      <c r="AT11" s="14">
-        <v>85.394190871369304</v>
-      </c>
-      <c r="AU11" s="14">
-        <v>92.448132780083</v>
-      </c>
-      <c r="AV11" s="14">
-        <v>96.348547717842294</v>
-      </c>
-      <c r="AW11" s="14">
-        <v>100</v>
-      </c>
-      <c r="AX11" s="14">
-        <v>104.647302904564</v>
-      </c>
-      <c r="AY11" s="14">
-        <v>107.966804979253</v>
-      </c>
-      <c r="AZ11" s="14">
-        <v>111.203319502075</v>
-      </c>
-      <c r="BA11" s="14">
-        <v>115.767634854772</v>
-      </c>
-      <c r="BB11" s="14">
-        <v>117.42738589211601</v>
-      </c>
-    </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="BB11" s="7">
+        <v>0</v>
+      </c>
+      <c r="BG11" s="13"/>
+      <c r="BH11" s="13"/>
+      <c r="BI11" s="13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>3</v>
@@ -2960,28 +2826,160 @@
       <c r="D12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB12" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK12" s="7">
-        <v>3.1</v>
-      </c>
-      <c r="AP12" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="AU12" s="7">
-        <v>5.2</v>
-      </c>
-      <c r="AZ12" s="7">
-        <v>5.4</v>
-      </c>
-      <c r="BB12" s="7">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="E12" s="6">
+        <v>1</v>
+      </c>
+      <c r="F12" s="14">
+        <v>1</v>
+      </c>
+      <c r="G12" s="14">
+        <v>1.1289570744394</v>
+      </c>
+      <c r="H12" s="14">
+        <v>1.42215881727406</v>
+      </c>
+      <c r="I12" s="14">
+        <v>1.90118931222233</v>
+      </c>
+      <c r="J12" s="14">
+        <v>2.3081073919986701</v>
+      </c>
+      <c r="K12" s="14">
+        <v>2.4974653103104298</v>
+      </c>
+      <c r="L12" s="14">
+        <v>2.9115458645382701</v>
+      </c>
+      <c r="M12" s="14">
+        <v>3.90623450399154</v>
+      </c>
+      <c r="N12" s="14">
+        <v>4.1703507493909102</v>
+      </c>
+      <c r="O12" s="14">
+        <v>4.55399078719985</v>
+      </c>
+      <c r="P12" s="14">
+        <v>5.0047790229916798</v>
+      </c>
+      <c r="Q12" s="14">
+        <v>5.3718558386314896</v>
+      </c>
+      <c r="R12" s="14">
+        <v>6.3137212289735496</v>
+      </c>
+      <c r="S12" s="14">
+        <v>7.4628507238053698</v>
+      </c>
+      <c r="T12" s="14">
+        <v>8.4391855224587609</v>
+      </c>
+      <c r="U12" s="14">
+        <v>9.3018160392078606</v>
+      </c>
+      <c r="V12" s="14">
+        <v>10.2347283365258</v>
+      </c>
+      <c r="W12" s="14">
+        <v>15.386785740408699</v>
+      </c>
+      <c r="X12" s="14">
+        <v>18.9416113416321</v>
+      </c>
+      <c r="Y12" s="14">
+        <v>19.1590871369295</v>
+      </c>
+      <c r="Z12" s="14">
+        <v>19.938817427385899</v>
+      </c>
+      <c r="AA12" s="14">
+        <v>22.702351313969601</v>
+      </c>
+      <c r="AB12" s="14">
+        <v>25.481798063623799</v>
+      </c>
+      <c r="AC12" s="14">
+        <v>28.584806362378998</v>
+      </c>
+      <c r="AD12" s="14">
+        <v>34.090656984785603</v>
+      </c>
+      <c r="AE12" s="14">
+        <v>37.0398409405256</v>
+      </c>
+      <c r="AF12" s="14">
+        <v>39.527551867219898</v>
+      </c>
+      <c r="AG12" s="14">
+        <v>43.633070539419101</v>
+      </c>
+      <c r="AH12" s="14">
+        <v>46.6140802213001</v>
+      </c>
+      <c r="AI12" s="14">
+        <v>50.0989972337483</v>
+      </c>
+      <c r="AJ12" s="14">
+        <v>52.899661134163203</v>
+      </c>
+      <c r="AK12" s="14">
+        <v>57.784910096818798</v>
+      </c>
+      <c r="AL12" s="14">
+        <v>61.2167842323652</v>
+      </c>
+      <c r="AM12" s="14">
+        <v>63.651452282157699</v>
+      </c>
+      <c r="AN12" s="14">
+        <v>67.053941908713696</v>
+      </c>
+      <c r="AO12" s="14">
+        <v>68.8796680497925</v>
+      </c>
+      <c r="AP12" s="14">
+        <v>70.456431535269701</v>
+      </c>
+      <c r="AQ12" s="14">
+        <v>73.858921161825705</v>
+      </c>
+      <c r="AR12" s="14">
+        <v>78.6721991701245</v>
+      </c>
+      <c r="AS12" s="14">
+        <v>82.987551867219906</v>
+      </c>
+      <c r="AT12" s="14">
+        <v>85.394190871369304</v>
+      </c>
+      <c r="AU12" s="14">
+        <v>92.448132780083</v>
+      </c>
+      <c r="AV12" s="14">
+        <v>96.348547717842294</v>
+      </c>
+      <c r="AW12" s="14">
+        <v>100</v>
+      </c>
+      <c r="AX12" s="14">
+        <v>104.647302904564</v>
+      </c>
+      <c r="AY12" s="14">
+        <v>107.966804979253</v>
+      </c>
+      <c r="AZ12" s="14">
+        <v>111.203319502075</v>
+      </c>
+      <c r="BA12" s="14">
+        <v>115.767634854772</v>
+      </c>
+      <c r="BB12" s="14">
+        <v>117.42738589211601</v>
+      </c>
+    </row>
+    <row r="13" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>3</v>
@@ -2992,13 +2990,28 @@
       <c r="D13" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="AB13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="AP13" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AU13" s="7">
+        <v>5.2</v>
+      </c>
+      <c r="AZ13" s="7">
+        <v>5.4</v>
+      </c>
       <c r="BB13" s="7">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:60" x14ac:dyDescent="0.25">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>3</v>
@@ -3009,16 +3022,13 @@
       <c r="D14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AW14" s="7">
-        <v>0.112</v>
-      </c>
       <c r="BB14" s="7">
-        <v>0.153</v>
-      </c>
-    </row>
-    <row r="15" spans="1:60" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>3</v>
@@ -3029,16 +3039,19 @@
       <c r="D15" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="AW15" s="7">
+        <v>0.112</v>
+      </c>
       <c r="BB15" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:60" x14ac:dyDescent="0.25">
+        <v>0.153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
@@ -3046,27 +3059,44 @@
       <c r="D16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="6">
+      <c r="BB16" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5">
         <v>1</v>
       </c>
-      <c r="AH16" s="7">
+      <c r="D17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="6">
         <v>1</v>
       </c>
-      <c r="AM16" s="7">
+      <c r="AH17" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM17" s="7">
         <v>0.75</v>
       </c>
-      <c r="AR16" s="7">
+      <c r="AR17" s="7">
         <v>0.62</v>
       </c>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="4">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BE6 BC6">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF7 BC7:BD7">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:D1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BD2 BC3:BD5 F2:BB6">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BE2 BC3:BE6 F2:BB7">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3084,7 +3114,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B6</xm:sqref>
+          <xm:sqref>B2:B7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
           <x14:formula1>

</xml_diff>

<commit_message>
Re-set GUI to base run for the Philippines
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="555" windowWidth="20370" windowHeight="6600" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="555" windowWidth="20370" windowHeight="6600" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2102,8 +2102,8 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,7 +2130,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="16">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
@@ -2140,7 +2140,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="19">
-        <v>0.35</v>
+        <v>0.25</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
@@ -2378,7 +2378,7 @@
   </sheetPr>
   <dimension ref="A1:BL21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="BB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
changed program_number_tests_per_tb_presentation back to 2.5
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="555" windowWidth="16275" windowHeight="6360" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="555" windowWidth="16275" windowHeight="6360" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2092,8 +2092,8 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,7 +2184,7 @@
         <v>63</v>
       </c>
       <c r="B8" s="19">
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2368,7 +2368,7 @@
   </sheetPr>
   <dimension ref="A1:BJ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="BB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Change beta range for Philippines to debug
Point estimate of transmission parameter for the Philippines was outside
of the uncertainty range considered - fix to get uncertainty running
again for the Philippines.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="555" windowWidth="16275" windowHeight="6360" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="555" windowWidth="16275" windowHeight="6360" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2087,8 +2087,8 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2116,6 +2116,12 @@
       </c>
       <c r="B2" s="16">
         <v>42</v>
+      </c>
+      <c r="C2" s="17">
+        <v>15</v>
+      </c>
+      <c r="D2" s="17">
+        <v>80</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
@@ -2363,7 +2369,7 @@
   </sheetPr>
   <dimension ref="A1:BJ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="BB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Minor update to start up cost of Xpert
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="555" windowWidth="16275" windowHeight="6360" tabRatio="807"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1838,7 +1843,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1873,7 +1878,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2088,7 +2093,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2267,7 +2272,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="26">
-        <v>11575186.195826644</v>
+        <v>11575226.195826599</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Minor recalibration of Philippines
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -2094,7 +2094,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2121,7 +2121,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="16">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C2" s="17">
         <v>15</v>

</xml_diff>

<commit_message>
Recalibrate beta since ACF changes
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -2097,7 +2097,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2124,7 +2124,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="16">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="17">
         <v>15</v>

</xml_diff>

<commit_message>
Implement poverty reduction interventions
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="66">
   <si>
     <t>parameter</t>
   </si>
@@ -150,9 +150,6 @@
     <t>program_perc_xpertacf_indigenous</t>
   </si>
   <si>
-    <t>program_perc_xpertacf</t>
-  </si>
-  <si>
     <t>econ_unitcost_xpertacf</t>
   </si>
   <si>
@@ -217,9 +214,6 @@
   </si>
   <si>
     <t>program_prop_acf_detections_per_round</t>
-  </si>
-  <si>
-    <t>scenario_9</t>
   </si>
 </sst>
 </file>
@@ -2160,7 +2154,7 @@
     </row>
     <row r="5" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="19">
         <v>5</v>
@@ -2194,7 +2188,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="19">
         <v>2.5</v>
@@ -2202,7 +2196,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="19">
         <v>0.5</v>
@@ -2308,7 +2302,7 @@
     </row>
     <row r="20" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="25">
         <v>473</v>
@@ -2319,7 +2313,7 @@
     </row>
     <row r="21" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="25">
         <v>0</v>
@@ -2330,7 +2324,7 @@
     </row>
     <row r="22" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="25">
         <v>142024</v>
@@ -2341,7 +2335,7 @@
     </row>
     <row r="23" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" s="25">
         <v>3</v>
@@ -2352,7 +2346,7 @@
     </row>
     <row r="24" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="25">
         <v>0.9</v>
@@ -2387,13 +2381,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BK23"/>
+  <dimension ref="A1:BJ22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BB20" sqref="BB20"/>
+      <selection pane="bottomRight" activeCell="BE19" sqref="BE19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2420,11 +2414,11 @@
     <col min="55" max="56" width="14" style="7" customWidth="1"/>
     <col min="57" max="59" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="60" max="61" width="14.42578125" style="7" customWidth="1"/>
-    <col min="62" max="63" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="64" max="16384" width="9.140625" style="7"/>
+    <col min="62" max="62" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="63" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
@@ -2606,16 +2600,13 @@
         <v>17</v>
       </c>
       <c r="BI1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BJ1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="BK1" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:63" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:62" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -2633,11 +2624,8 @@
         <v>99</v>
       </c>
       <c r="BD2" s="27"/>
-      <c r="BK2" s="9">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -2663,9 +2651,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>4</v>
@@ -2682,11 +2670,8 @@
       <c r="BD4" s="7">
         <v>50</v>
       </c>
-      <c r="BK4" s="7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -2723,7 +2708,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -2756,7 +2741,7 @@
       <c r="AY6" s="8"/>
       <c r="AZ6" s="8"/>
     </row>
-    <row r="7" spans="1:63" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:62" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
@@ -2776,17 +2761,11 @@
       <c r="AY7" s="9">
         <v>2.8</v>
       </c>
-      <c r="BE7" s="9">
-        <v>99</v>
-      </c>
       <c r="BF7" s="27"/>
-      <c r="BK7" s="9">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
@@ -2806,19 +2785,15 @@
       <c r="BB8" s="7">
         <v>0</v>
       </c>
-      <c r="BF8" s="7">
+      <c r="BE8" s="13">
         <v>80</v>
       </c>
+      <c r="BF8" s="13"/>
       <c r="BG8" s="13"/>
-      <c r="BH8" s="13"/>
-      <c r="BI8" s="13"/>
-      <c r="BK8" s="7">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -2829,24 +2804,16 @@
       <c r="D9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="7">
-        <v>0</v>
-      </c>
       <c r="BB9" s="7">
         <v>0</v>
       </c>
-      <c r="BG9" s="13">
-        <v>80</v>
-      </c>
-      <c r="BH9" s="13"/>
-      <c r="BI9" s="13"/>
-    </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="BE9" s="13"/>
+      <c r="BF9" s="13"/>
+      <c r="BG9" s="13"/>
+    </row>
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>4</v>
@@ -2860,11 +2827,13 @@
       <c r="BB10" s="7">
         <v>0</v>
       </c>
+      <c r="BE10" s="13"/>
+      <c r="BF10" s="13">
+        <v>80</v>
+      </c>
       <c r="BG10" s="13"/>
-      <c r="BH10" s="13"/>
-      <c r="BI10" s="13"/>
-    </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>54</v>
       </c>
@@ -2880,15 +2849,15 @@
       <c r="BB11" s="7">
         <v>0</v>
       </c>
-      <c r="BG11" s="13"/>
-      <c r="BH11" s="13">
+      <c r="BE11" s="13"/>
+      <c r="BF11" s="13"/>
+      <c r="BG11" s="13">
         <v>80</v>
       </c>
-      <c r="BI11" s="13"/>
-    </row>
-    <row r="12" spans="1:63" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
@@ -2902,15 +2871,16 @@
       <c r="BB12" s="7">
         <v>0</v>
       </c>
+      <c r="BE12" s="13"/>
+      <c r="BF12" s="13"/>
       <c r="BG12" s="13"/>
-      <c r="BH12" s="13"/>
-      <c r="BI12" s="13">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="BH12" s="13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>4</v>
@@ -2921,25 +2891,163 @@
       <c r="D13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="BB13" s="7">
-        <v>0</v>
-      </c>
-      <c r="BG13" s="13"/>
-      <c r="BH13" s="13"/>
-      <c r="BI13" s="13"/>
-      <c r="BJ13" s="13">
-        <v>90</v>
-      </c>
-      <c r="BK13" s="7">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="E13" s="6">
+        <v>1</v>
+      </c>
+      <c r="F13" s="14">
+        <v>1</v>
+      </c>
+      <c r="G13" s="14">
+        <v>1.1289570744394</v>
+      </c>
+      <c r="H13" s="14">
+        <v>1.42215881727406</v>
+      </c>
+      <c r="I13" s="14">
+        <v>1.90118931222233</v>
+      </c>
+      <c r="J13" s="14">
+        <v>2.3081073919986701</v>
+      </c>
+      <c r="K13" s="14">
+        <v>2.4974653103104298</v>
+      </c>
+      <c r="L13" s="14">
+        <v>2.9115458645382701</v>
+      </c>
+      <c r="M13" s="14">
+        <v>3.90623450399154</v>
+      </c>
+      <c r="N13" s="14">
+        <v>4.1703507493909102</v>
+      </c>
+      <c r="O13" s="14">
+        <v>4.55399078719985</v>
+      </c>
+      <c r="P13" s="14">
+        <v>5.0047790229916798</v>
+      </c>
+      <c r="Q13" s="14">
+        <v>5.3718558386314896</v>
+      </c>
+      <c r="R13" s="14">
+        <v>6.3137212289735496</v>
+      </c>
+      <c r="S13" s="14">
+        <v>7.4628507238053698</v>
+      </c>
+      <c r="T13" s="14">
+        <v>8.4391855224587609</v>
+      </c>
+      <c r="U13" s="14">
+        <v>9.3018160392078606</v>
+      </c>
+      <c r="V13" s="14">
+        <v>10.2347283365258</v>
+      </c>
+      <c r="W13" s="14">
+        <v>15.386785740408699</v>
+      </c>
+      <c r="X13" s="14">
+        <v>18.9416113416321</v>
+      </c>
+      <c r="Y13" s="14">
+        <v>19.1590871369295</v>
+      </c>
+      <c r="Z13" s="14">
+        <v>19.938817427385899</v>
+      </c>
+      <c r="AA13" s="14">
+        <v>22.702351313969601</v>
+      </c>
+      <c r="AB13" s="14">
+        <v>25.481798063623799</v>
+      </c>
+      <c r="AC13" s="14">
+        <v>28.584806362378998</v>
+      </c>
+      <c r="AD13" s="14">
+        <v>34.090656984785603</v>
+      </c>
+      <c r="AE13" s="14">
+        <v>37.0398409405256</v>
+      </c>
+      <c r="AF13" s="14">
+        <v>39.527551867219898</v>
+      </c>
+      <c r="AG13" s="14">
+        <v>43.633070539419101</v>
+      </c>
+      <c r="AH13" s="14">
+        <v>46.6140802213001</v>
+      </c>
+      <c r="AI13" s="14">
+        <v>50.0989972337483</v>
+      </c>
+      <c r="AJ13" s="14">
+        <v>52.899661134163203</v>
+      </c>
+      <c r="AK13" s="14">
+        <v>57.784910096818798</v>
+      </c>
+      <c r="AL13" s="14">
+        <v>61.2167842323652</v>
+      </c>
+      <c r="AM13" s="14">
+        <v>63.651452282157699</v>
+      </c>
+      <c r="AN13" s="14">
+        <v>67.053941908713696</v>
+      </c>
+      <c r="AO13" s="14">
+        <v>68.8796680497925</v>
+      </c>
+      <c r="AP13" s="14">
+        <v>70.456431535269701</v>
+      </c>
+      <c r="AQ13" s="14">
+        <v>73.858921161825705</v>
+      </c>
+      <c r="AR13" s="14">
+        <v>78.6721991701245</v>
+      </c>
+      <c r="AS13" s="14">
+        <v>82.987551867219906</v>
+      </c>
+      <c r="AT13" s="14">
+        <v>85.394190871369304</v>
+      </c>
+      <c r="AU13" s="14">
+        <v>92.448132780083</v>
+      </c>
+      <c r="AV13" s="14">
+        <v>96.348547717842294</v>
+      </c>
+      <c r="AW13" s="14">
+        <v>100</v>
+      </c>
+      <c r="AX13" s="14">
+        <v>104.647302904564</v>
+      </c>
+      <c r="AY13" s="14">
+        <v>107.966804979253</v>
+      </c>
+      <c r="AZ13" s="14">
+        <v>111.203319502075</v>
+      </c>
+      <c r="BA13" s="14">
+        <v>115.767634854772</v>
+      </c>
+      <c r="BB13" s="14">
+        <v>117.42738589211601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
@@ -2947,158 +3055,26 @@
       <c r="D14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="6">
-        <v>1</v>
-      </c>
-      <c r="F14" s="14">
-        <v>1</v>
-      </c>
-      <c r="G14" s="14">
-        <v>1.1289570744394</v>
-      </c>
-      <c r="H14" s="14">
-        <v>1.42215881727406</v>
-      </c>
-      <c r="I14" s="14">
-        <v>1.90118931222233</v>
-      </c>
-      <c r="J14" s="14">
-        <v>2.3081073919986701</v>
-      </c>
-      <c r="K14" s="14">
-        <v>2.4974653103104298</v>
-      </c>
-      <c r="L14" s="14">
-        <v>2.9115458645382701</v>
-      </c>
-      <c r="M14" s="14">
-        <v>3.90623450399154</v>
-      </c>
-      <c r="N14" s="14">
-        <v>4.1703507493909102</v>
-      </c>
-      <c r="O14" s="14">
-        <v>4.55399078719985</v>
-      </c>
-      <c r="P14" s="14">
-        <v>5.0047790229916798</v>
-      </c>
-      <c r="Q14" s="14">
-        <v>5.3718558386314896</v>
-      </c>
-      <c r="R14" s="14">
-        <v>6.3137212289735496</v>
-      </c>
-      <c r="S14" s="14">
-        <v>7.4628507238053698</v>
-      </c>
-      <c r="T14" s="14">
-        <v>8.4391855224587609</v>
-      </c>
-      <c r="U14" s="14">
-        <v>9.3018160392078606</v>
-      </c>
-      <c r="V14" s="14">
-        <v>10.2347283365258</v>
-      </c>
-      <c r="W14" s="14">
-        <v>15.386785740408699</v>
-      </c>
-      <c r="X14" s="14">
-        <v>18.9416113416321</v>
-      </c>
-      <c r="Y14" s="14">
-        <v>19.1590871369295</v>
-      </c>
-      <c r="Z14" s="14">
-        <v>19.938817427385899</v>
-      </c>
-      <c r="AA14" s="14">
-        <v>22.702351313969601</v>
-      </c>
-      <c r="AB14" s="14">
-        <v>25.481798063623799</v>
-      </c>
-      <c r="AC14" s="14">
-        <v>28.584806362378998</v>
-      </c>
-      <c r="AD14" s="14">
-        <v>34.090656984785603</v>
-      </c>
-      <c r="AE14" s="14">
-        <v>37.0398409405256</v>
-      </c>
-      <c r="AF14" s="14">
-        <v>39.527551867219898</v>
-      </c>
-      <c r="AG14" s="14">
-        <v>43.633070539419101</v>
-      </c>
-      <c r="AH14" s="14">
-        <v>46.6140802213001</v>
-      </c>
-      <c r="AI14" s="14">
-        <v>50.0989972337483</v>
-      </c>
-      <c r="AJ14" s="14">
-        <v>52.899661134163203</v>
-      </c>
-      <c r="AK14" s="14">
-        <v>57.784910096818798</v>
-      </c>
-      <c r="AL14" s="14">
-        <v>61.2167842323652</v>
-      </c>
-      <c r="AM14" s="14">
-        <v>63.651452282157699</v>
-      </c>
-      <c r="AN14" s="14">
-        <v>67.053941908713696</v>
-      </c>
-      <c r="AO14" s="14">
-        <v>68.8796680497925</v>
-      </c>
-      <c r="AP14" s="14">
-        <v>70.456431535269701</v>
-      </c>
-      <c r="AQ14" s="14">
-        <v>73.858921161825705</v>
-      </c>
-      <c r="AR14" s="14">
-        <v>78.6721991701245</v>
-      </c>
-      <c r="AS14" s="14">
-        <v>82.987551867219906</v>
-      </c>
-      <c r="AT14" s="14">
-        <v>85.394190871369304</v>
-      </c>
-      <c r="AU14" s="14">
-        <v>92.448132780083</v>
-      </c>
-      <c r="AV14" s="14">
-        <v>96.348547717842294</v>
-      </c>
-      <c r="AW14" s="14">
-        <v>100</v>
-      </c>
-      <c r="AX14" s="14">
-        <v>104.647302904564</v>
-      </c>
-      <c r="AY14" s="14">
-        <v>107.966804979253</v>
-      </c>
-      <c r="AZ14" s="14">
-        <v>111.203319502075</v>
-      </c>
-      <c r="BA14" s="14">
-        <v>115.767634854772</v>
-      </c>
-      <c r="BB14" s="14">
-        <v>117.42738589211601</v>
-      </c>
-    </row>
-    <row r="15" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="AB14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="AP14" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AU14" s="7">
+        <v>5.2</v>
+      </c>
+      <c r="AZ14" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="BB14" s="7">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>57</v>
       </c>
@@ -3111,31 +3087,16 @@
       <c r="D15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB15" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK15" s="7">
-        <v>3.1</v>
-      </c>
-      <c r="AP15" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="AU15" s="7">
-        <v>5.2</v>
-      </c>
-      <c r="AZ15" s="7">
-        <v>5.4</v>
-      </c>
       <c r="BB15" s="7">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:63" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>58</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
@@ -3143,11 +3104,14 @@
       <c r="D16" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="AW16" s="7">
+        <v>0.112</v>
+      </c>
       <c r="BB16" s="7">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:54" x14ac:dyDescent="0.25">
+        <v>0.153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>59</v>
       </c>
@@ -3160,14 +3124,12 @@
       <c r="D17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AW17" s="7">
-        <v>0.112</v>
-      </c>
       <c r="BB17" s="7">
-        <v>0.153</v>
-      </c>
-    </row>
-    <row r="18" spans="1:54" x14ac:dyDescent="0.25">
+        <f>1/98 * 100</f>
+        <v>1.0204081632653061</v>
+      </c>
+    </row>
+    <row r="18" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>60</v>
       </c>
@@ -3181,11 +3143,15 @@
         <v>3</v>
       </c>
       <c r="BB18" s="7">
-        <f>1/98 * 100</f>
-        <v>1.0204081632653061</v>
-      </c>
-    </row>
-    <row r="19" spans="1:54" x14ac:dyDescent="0.25">
+        <f>4.5/98 * 100</f>
+        <v>4.591836734693878</v>
+      </c>
+      <c r="BI18" s="7">
+        <f>BB18/2</f>
+        <v>2.295918367346939</v>
+      </c>
+    </row>
+    <row r="19" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>61</v>
       </c>
@@ -3199,11 +3165,15 @@
         <v>3</v>
       </c>
       <c r="BB19" s="7">
-        <f>4.5/98 * 100</f>
-        <v>4.591836734693878</v>
-      </c>
-    </row>
-    <row r="20" spans="1:54" x14ac:dyDescent="0.25">
+        <f>10/98 * 100</f>
+        <v>10.204081632653061</v>
+      </c>
+      <c r="BJ19" s="7">
+        <f>BB19/2</f>
+        <v>5.1020408163265305</v>
+      </c>
+    </row>
+    <row r="20" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>62</v>
       </c>
@@ -3217,11 +3187,10 @@
         <v>3</v>
       </c>
       <c r="BB20" s="7">
-        <f>10/98 * 100</f>
-        <v>10.204081632653061</v>
-      </c>
-    </row>
-    <row r="21" spans="1:54" x14ac:dyDescent="0.25">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>63</v>
       </c>
@@ -3238,7 +3207,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>64</v>
       </c>
@@ -3251,47 +3220,30 @@
       <c r="D22" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="BB22" s="7">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="5">
-        <v>1</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F23" s="7">
+      <c r="F22" s="7">
         <v>0</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G22" s="7">
         <v>30</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I22" s="7">
         <v>50</v>
       </c>
-      <c r="S23" s="7">
+      <c r="S22" s="7">
         <v>50</v>
       </c>
-      <c r="AM23" s="7">
+      <c r="AM22" s="7">
         <v>50</v>
       </c>
-      <c r="AR23" s="7">
+      <c r="AR22" s="7">
         <v>53</v>
       </c>
-      <c r="AW23" s="7">
+      <c r="AW22" s="7">
         <v>55</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations xWindow="382" yWindow="552" count="4">
+  <dataValidations disablePrompts="1" xWindow="382" yWindow="552" count="4">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF7 BC7:BD7">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
@@ -3310,7 +3262,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" xWindow="382" yWindow="552" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>

</xml_diff>

<commit_message>
Correct starting population for the Philippines
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2102,8 +2102,8 @@
   </sheetPr>
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2179,7 +2179,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="21">
-        <v>30000000</v>
+        <v>25800000</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
@@ -2392,11 +2392,11 @@
   </sheetPr>
   <dimension ref="A1:BL23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="AU2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BJ14" sqref="BJ14"/>
+      <selection pane="bottomRight" activeCell="AW11" sqref="AW11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Remove unused interventions from Philippines sheet
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
   <si>
     <t>parameter</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>program_perc_xpertacf_prison</t>
-  </si>
-  <si>
-    <t>program_perc_xpertacf_indigenous</t>
   </si>
   <si>
     <t>econ_unitcost_xpertacf</t>
@@ -2102,8 +2099,8 @@
   </sheetPr>
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2163,7 +2160,7 @@
     </row>
     <row r="5" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="19">
         <v>5</v>
@@ -2197,7 +2194,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="19">
         <v>1.5</v>
@@ -2205,7 +2202,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" s="19">
         <f>1/3</f>
@@ -2312,7 +2309,7 @@
     </row>
     <row r="20" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="25">
         <v>473</v>
@@ -2323,7 +2320,7 @@
     </row>
     <row r="21" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="25">
         <v>0</v>
@@ -2334,7 +2331,7 @@
     </row>
     <row r="22" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" s="25">
         <v>142024</v>
@@ -2345,7 +2342,7 @@
     </row>
     <row r="23" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23" s="25">
         <v>3</v>
@@ -2356,7 +2353,7 @@
     </row>
     <row r="24" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24" s="25">
         <v>0.9</v>
@@ -2391,13 +2388,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BL23"/>
+  <dimension ref="A1:BL22"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="AU2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AW11" sqref="AW11"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2610,16 +2607,16 @@
         <v>17</v>
       </c>
       <c r="BI1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BJ1" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="BK1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BL1" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="BL1" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:64" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2669,7 +2666,7 @@
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>4</v>
@@ -2809,7 +2806,7 @@
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -2824,7 +2821,9 @@
         <v>0</v>
       </c>
       <c r="BE9" s="13"/>
-      <c r="BF9" s="13"/>
+      <c r="BF9" s="13">
+        <v>80</v>
+      </c>
       <c r="BG9" s="13"/>
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.25">
@@ -2844,14 +2843,14 @@
         <v>0</v>
       </c>
       <c r="BE10" s="13"/>
-      <c r="BF10" s="13">
+      <c r="BF10" s="13"/>
+      <c r="BG10" s="13">
         <v>80</v>
       </c>
-      <c r="BG10" s="13"/>
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>4</v>
@@ -2867,13 +2866,16 @@
       </c>
       <c r="BE11" s="13"/>
       <c r="BF11" s="13"/>
-      <c r="BG11" s="13">
-        <v>80</v>
-      </c>
+      <c r="BG11" s="13"/>
+      <c r="BH11" s="13">
+        <v>90</v>
+      </c>
+      <c r="BI11" s="13"/>
+      <c r="BJ11" s="13"/>
     </row>
     <row r="12" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
@@ -2890,15 +2892,17 @@
       <c r="BE12" s="13"/>
       <c r="BF12" s="13"/>
       <c r="BG12" s="13"/>
-      <c r="BH12" s="13">
-        <v>90</v>
-      </c>
-      <c r="BI12" s="13"/>
-      <c r="BJ12" s="13"/>
+      <c r="BH12" s="13"/>
+      <c r="BI12" s="13">
+        <v>50</v>
+      </c>
+      <c r="BJ12" s="13">
+        <v>100</v>
+      </c>
     </row>
     <row r="13" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>4</v>
@@ -2909,26 +2913,163 @@
       <c r="D13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="BB13" s="7">
-        <v>0</v>
-      </c>
-      <c r="BE13" s="13"/>
-      <c r="BF13" s="13"/>
-      <c r="BG13" s="13"/>
-      <c r="BH13" s="13"/>
-      <c r="BI13" s="13">
-        <v>50</v>
-      </c>
-      <c r="BJ13" s="13">
+      <c r="E13" s="6">
+        <v>1</v>
+      </c>
+      <c r="F13" s="14">
+        <v>1</v>
+      </c>
+      <c r="G13" s="14">
+        <v>1.1289570744394</v>
+      </c>
+      <c r="H13" s="14">
+        <v>1.42215881727406</v>
+      </c>
+      <c r="I13" s="14">
+        <v>1.90118931222233</v>
+      </c>
+      <c r="J13" s="14">
+        <v>2.3081073919986701</v>
+      </c>
+      <c r="K13" s="14">
+        <v>2.4974653103104298</v>
+      </c>
+      <c r="L13" s="14">
+        <v>2.9115458645382701</v>
+      </c>
+      <c r="M13" s="14">
+        <v>3.90623450399154</v>
+      </c>
+      <c r="N13" s="14">
+        <v>4.1703507493909102</v>
+      </c>
+      <c r="O13" s="14">
+        <v>4.55399078719985</v>
+      </c>
+      <c r="P13" s="14">
+        <v>5.0047790229916798</v>
+      </c>
+      <c r="Q13" s="14">
+        <v>5.3718558386314896</v>
+      </c>
+      <c r="R13" s="14">
+        <v>6.3137212289735496</v>
+      </c>
+      <c r="S13" s="14">
+        <v>7.4628507238053698</v>
+      </c>
+      <c r="T13" s="14">
+        <v>8.4391855224587609</v>
+      </c>
+      <c r="U13" s="14">
+        <v>9.3018160392078606</v>
+      </c>
+      <c r="V13" s="14">
+        <v>10.2347283365258</v>
+      </c>
+      <c r="W13" s="14">
+        <v>15.386785740408699</v>
+      </c>
+      <c r="X13" s="14">
+        <v>18.9416113416321</v>
+      </c>
+      <c r="Y13" s="14">
+        <v>19.1590871369295</v>
+      </c>
+      <c r="Z13" s="14">
+        <v>19.938817427385899</v>
+      </c>
+      <c r="AA13" s="14">
+        <v>22.702351313969601</v>
+      </c>
+      <c r="AB13" s="14">
+        <v>25.481798063623799</v>
+      </c>
+      <c r="AC13" s="14">
+        <v>28.584806362378998</v>
+      </c>
+      <c r="AD13" s="14">
+        <v>34.090656984785603</v>
+      </c>
+      <c r="AE13" s="14">
+        <v>37.0398409405256</v>
+      </c>
+      <c r="AF13" s="14">
+        <v>39.527551867219898</v>
+      </c>
+      <c r="AG13" s="14">
+        <v>43.633070539419101</v>
+      </c>
+      <c r="AH13" s="14">
+        <v>46.6140802213001</v>
+      </c>
+      <c r="AI13" s="14">
+        <v>50.0989972337483</v>
+      </c>
+      <c r="AJ13" s="14">
+        <v>52.899661134163203</v>
+      </c>
+      <c r="AK13" s="14">
+        <v>57.784910096818798</v>
+      </c>
+      <c r="AL13" s="14">
+        <v>61.2167842323652</v>
+      </c>
+      <c r="AM13" s="14">
+        <v>63.651452282157699</v>
+      </c>
+      <c r="AN13" s="14">
+        <v>67.053941908713696</v>
+      </c>
+      <c r="AO13" s="14">
+        <v>68.8796680497925</v>
+      </c>
+      <c r="AP13" s="14">
+        <v>70.456431535269701</v>
+      </c>
+      <c r="AQ13" s="14">
+        <v>73.858921161825705</v>
+      </c>
+      <c r="AR13" s="14">
+        <v>78.6721991701245</v>
+      </c>
+      <c r="AS13" s="14">
+        <v>82.987551867219906</v>
+      </c>
+      <c r="AT13" s="14">
+        <v>85.394190871369304</v>
+      </c>
+      <c r="AU13" s="14">
+        <v>92.448132780083</v>
+      </c>
+      <c r="AV13" s="14">
+        <v>96.348547717842294</v>
+      </c>
+      <c r="AW13" s="14">
         <v>100</v>
+      </c>
+      <c r="AX13" s="14">
+        <v>104.647302904564</v>
+      </c>
+      <c r="AY13" s="14">
+        <v>107.966804979253</v>
+      </c>
+      <c r="AZ13" s="14">
+        <v>111.203319502075</v>
+      </c>
+      <c r="BA13" s="14">
+        <v>115.767634854772</v>
+      </c>
+      <c r="BB13" s="14">
+        <v>117.42738589211601</v>
       </c>
     </row>
     <row r="14" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
@@ -2936,155 +3077,23 @@
       <c r="D14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="6">
-        <v>1</v>
-      </c>
-      <c r="F14" s="14">
-        <v>1</v>
-      </c>
-      <c r="G14" s="14">
-        <v>1.1289570744394</v>
-      </c>
-      <c r="H14" s="14">
-        <v>1.42215881727406</v>
-      </c>
-      <c r="I14" s="14">
-        <v>1.90118931222233</v>
-      </c>
-      <c r="J14" s="14">
-        <v>2.3081073919986701</v>
-      </c>
-      <c r="K14" s="14">
-        <v>2.4974653103104298</v>
-      </c>
-      <c r="L14" s="14">
-        <v>2.9115458645382701</v>
-      </c>
-      <c r="M14" s="14">
-        <v>3.90623450399154</v>
-      </c>
-      <c r="N14" s="14">
-        <v>4.1703507493909102</v>
-      </c>
-      <c r="O14" s="14">
-        <v>4.55399078719985</v>
-      </c>
-      <c r="P14" s="14">
-        <v>5.0047790229916798</v>
-      </c>
-      <c r="Q14" s="14">
-        <v>5.3718558386314896</v>
-      </c>
-      <c r="R14" s="14">
-        <v>6.3137212289735496</v>
-      </c>
-      <c r="S14" s="14">
-        <v>7.4628507238053698</v>
-      </c>
-      <c r="T14" s="14">
-        <v>8.4391855224587609</v>
-      </c>
-      <c r="U14" s="14">
-        <v>9.3018160392078606</v>
-      </c>
-      <c r="V14" s="14">
-        <v>10.2347283365258</v>
-      </c>
-      <c r="W14" s="14">
-        <v>15.386785740408699</v>
-      </c>
-      <c r="X14" s="14">
-        <v>18.9416113416321</v>
-      </c>
-      <c r="Y14" s="14">
-        <v>19.1590871369295</v>
-      </c>
-      <c r="Z14" s="14">
-        <v>19.938817427385899</v>
-      </c>
-      <c r="AA14" s="14">
-        <v>22.702351313969601</v>
-      </c>
-      <c r="AB14" s="14">
-        <v>25.481798063623799</v>
-      </c>
-      <c r="AC14" s="14">
-        <v>28.584806362378998</v>
-      </c>
-      <c r="AD14" s="14">
-        <v>34.090656984785603</v>
-      </c>
-      <c r="AE14" s="14">
-        <v>37.0398409405256</v>
-      </c>
-      <c r="AF14" s="14">
-        <v>39.527551867219898</v>
-      </c>
-      <c r="AG14" s="14">
-        <v>43.633070539419101</v>
-      </c>
-      <c r="AH14" s="14">
-        <v>46.6140802213001</v>
-      </c>
-      <c r="AI14" s="14">
-        <v>50.0989972337483</v>
-      </c>
-      <c r="AJ14" s="14">
-        <v>52.899661134163203</v>
-      </c>
-      <c r="AK14" s="14">
-        <v>57.784910096818798</v>
-      </c>
-      <c r="AL14" s="14">
-        <v>61.2167842323652</v>
-      </c>
-      <c r="AM14" s="14">
-        <v>63.651452282157699</v>
-      </c>
-      <c r="AN14" s="14">
-        <v>67.053941908713696</v>
-      </c>
-      <c r="AO14" s="14">
-        <v>68.8796680497925</v>
-      </c>
-      <c r="AP14" s="14">
-        <v>70.456431535269701</v>
-      </c>
-      <c r="AQ14" s="14">
-        <v>73.858921161825705</v>
-      </c>
-      <c r="AR14" s="14">
-        <v>78.6721991701245</v>
-      </c>
-      <c r="AS14" s="14">
-        <v>82.987551867219906</v>
-      </c>
-      <c r="AT14" s="14">
-        <v>85.394190871369304</v>
-      </c>
-      <c r="AU14" s="14">
-        <v>92.448132780083</v>
-      </c>
-      <c r="AV14" s="14">
-        <v>96.348547717842294</v>
-      </c>
-      <c r="AW14" s="14">
-        <v>100</v>
-      </c>
-      <c r="AX14" s="14">
-        <v>104.647302904564</v>
-      </c>
-      <c r="AY14" s="14">
-        <v>107.966804979253</v>
-      </c>
-      <c r="AZ14" s="14">
-        <v>111.203319502075</v>
-      </c>
-      <c r="BA14" s="14">
-        <v>115.767634854772</v>
-      </c>
-      <c r="BB14" s="14">
-        <v>117.42738589211601</v>
+      <c r="AB14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="AP14" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AU14" s="7">
+        <v>5.2</v>
+      </c>
+      <c r="AZ14" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="BB14" s="7">
+        <v>5.9</v>
       </c>
     </row>
     <row r="15" spans="1:64" x14ac:dyDescent="0.25">
@@ -3100,23 +3109,8 @@
       <c r="D15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB15" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK15" s="7">
-        <v>3.1</v>
-      </c>
-      <c r="AP15" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="AU15" s="7">
-        <v>5.2</v>
-      </c>
-      <c r="AZ15" s="7">
-        <v>5.4</v>
-      </c>
       <c r="BB15" s="7">
-        <v>5.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16" spans="1:64" x14ac:dyDescent="0.25">
@@ -3124,7 +3118,7 @@
         <v>57</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
@@ -3132,8 +3126,11 @@
       <c r="D16" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="AW16" s="7">
+        <v>0.112</v>
+      </c>
       <c r="BB16" s="7">
-        <v>0.1</v>
+        <v>0.153</v>
       </c>
     </row>
     <row r="17" spans="1:64" x14ac:dyDescent="0.25">
@@ -3149,11 +3146,9 @@
       <c r="D17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AW17" s="7">
-        <v>0.112</v>
-      </c>
       <c r="BB17" s="7">
-        <v>0.153</v>
+        <f>1/98 * 100</f>
+        <v>1.0204081632653061</v>
       </c>
     </row>
     <row r="18" spans="1:64" x14ac:dyDescent="0.25">
@@ -3170,8 +3165,12 @@
         <v>3</v>
       </c>
       <c r="BB18" s="7">
-        <f>1/98 * 100</f>
-        <v>1.0204081632653061</v>
+        <f>4.5/98 * 100</f>
+        <v>4.591836734693878</v>
+      </c>
+      <c r="BK18" s="7">
+        <f>BB18/2</f>
+        <v>2.295918367346939</v>
       </c>
     </row>
     <row r="19" spans="1:64" x14ac:dyDescent="0.25">
@@ -3188,12 +3187,12 @@
         <v>3</v>
       </c>
       <c r="BB19" s="7">
-        <f>4.5/98 * 100</f>
-        <v>4.591836734693878</v>
-      </c>
-      <c r="BK19" s="7">
+        <f>10/98 * 100</f>
+        <v>10.204081632653061</v>
+      </c>
+      <c r="BL19" s="7">
         <f>BB19/2</f>
-        <v>2.295918367346939</v>
+        <v>5.1020408163265305</v>
       </c>
     </row>
     <row r="20" spans="1:64" x14ac:dyDescent="0.25">
@@ -3210,12 +3209,7 @@
         <v>3</v>
       </c>
       <c r="BB20" s="7">
-        <f>10/98 * 100</f>
-        <v>10.204081632653061</v>
-      </c>
-      <c r="BL20" s="7">
-        <f>BB20/2</f>
-        <v>5.1020408163265305</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="21" spans="1:64" x14ac:dyDescent="0.25">
@@ -3248,42 +3242,25 @@
       <c r="D22" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="BB22" s="7">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="5">
-        <v>1</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F23" s="7">
+      <c r="F22" s="7">
         <v>0</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G22" s="7">
         <v>30</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I22" s="7">
         <v>50</v>
       </c>
-      <c r="S23" s="7">
+      <c r="S22" s="7">
         <v>50</v>
       </c>
-      <c r="AM23" s="7">
+      <c r="AM22" s="7">
         <v>50</v>
       </c>
-      <c r="AR23" s="7">
+      <c r="AR22" s="7">
         <v>53</v>
       </c>
-      <c r="AW23" s="7">
+      <c r="AW22" s="7">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor changes to perc_treatment_death
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1865,7 +1870,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1900,7 +1905,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2409,7 +2414,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="AJ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AX6" sqref="AX6"/>
+      <selection pane="bottomRight" activeCell="AT8" sqref="AT8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2762,33 +2767,15 @@
       <c r="AQ6" s="8"/>
       <c r="AR6" s="9"/>
       <c r="AS6" s="8"/>
-      <c r="AT6" s="9">
-        <v>2</v>
-      </c>
-      <c r="AU6" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="AV6" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="AW6" s="9">
-        <v>1</v>
-      </c>
-      <c r="AX6" s="9">
-        <v>1</v>
-      </c>
-      <c r="AY6" s="9">
-        <v>1</v>
-      </c>
-      <c r="AZ6" s="9">
-        <v>1</v>
-      </c>
-      <c r="BA6" s="9">
-        <v>1</v>
-      </c>
-      <c r="BB6" s="9">
-        <v>1</v>
-      </c>
+      <c r="AT6" s="9"/>
+      <c r="AU6" s="9"/>
+      <c r="AV6" s="9"/>
+      <c r="AW6" s="9"/>
+      <c r="AX6" s="9"/>
+      <c r="AY6" s="9"/>
+      <c r="AZ6" s="9"/>
+      <c r="BA6" s="9"/>
+      <c r="BB6" s="9"/>
     </row>
     <row r="7" spans="1:65" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">

</xml_diff>

<commit_message>
Revise scenarios for analysis
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="78">
   <si>
     <t>parameter</t>
   </si>
@@ -240,6 +240,21 @@
   </si>
   <si>
     <t>program_perc_ipt_age0to5</t>
+  </si>
+  <si>
+    <t>scenario_12</t>
+  </si>
+  <si>
+    <t>scenario_13</t>
+  </si>
+  <si>
+    <t>scenario_14</t>
+  </si>
+  <si>
+    <t>scenario_16</t>
+  </si>
+  <si>
+    <t>scenario_15</t>
   </si>
 </sst>
 </file>
@@ -2120,7 +2135,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2289,7 +2304,7 @@
         <v>41</v>
       </c>
       <c r="B15" s="25">
-        <v>30.26</v>
+        <v>26.24</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
@@ -2408,13 +2423,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BM26"/>
+  <dimension ref="A1:BR26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AJ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AT2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AT8" sqref="AT8"/>
+      <selection pane="bottomRight" activeCell="BP3" sqref="BP3:BP26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2442,10 +2457,13 @@
     <col min="57" max="59" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="60" max="64" width="14.42578125" style="7" customWidth="1"/>
     <col min="65" max="65" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="66" max="16384" width="9.140625" style="7"/>
+    <col min="66" max="66" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="15" style="7" bestFit="1" customWidth="1"/>
+    <col min="69" max="70" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="71" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
@@ -2641,8 +2659,23 @@
       <c r="BM1" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:65" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BN1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="BP1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="BR1" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:70" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -2658,8 +2691,11 @@
       <c r="E2" s="1"/>
       <c r="BC2" s="27"/>
       <c r="BD2" s="27"/>
-    </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BN2" s="27">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -2684,8 +2720,9 @@
       <c r="AW3" s="7">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BP3" s="13"/>
+    </row>
+    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>49</v>
       </c>
@@ -2701,11 +2738,14 @@
       <c r="BB4" s="7">
         <v>0</v>
       </c>
-      <c r="BD4" s="7">
+      <c r="BC4" s="13">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BP4" s="13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -2741,8 +2781,9 @@
       <c r="AZ5" s="8">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BP5" s="13"/>
+    </row>
+    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -2776,8 +2817,9 @@
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
       <c r="BB6" s="9"/>
-    </row>
-    <row r="7" spans="1:65" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BP6" s="13"/>
+    </row>
+    <row r="7" spans="1:70" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
@@ -2797,9 +2839,15 @@
       <c r="AY7" s="9">
         <v>2.8</v>
       </c>
+      <c r="BD7" s="27">
+        <v>99</v>
+      </c>
       <c r="BF7" s="27"/>
-    </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BP7" s="27">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
@@ -2821,14 +2869,15 @@
       <c r="BB8" s="7">
         <v>0</v>
       </c>
-      <c r="BE8" s="13">
-        <v>80</v>
-      </c>
+      <c r="BE8" s="13"/>
       <c r="BF8" s="13"/>
       <c r="BG8" s="13"/>
-      <c r="BH8" s="13"/>
-    </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BH8" s="13">
+        <v>80</v>
+      </c>
+      <c r="BP8" s="13"/>
+    </row>
+    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>52</v>
       </c>
@@ -2845,13 +2894,15 @@
         <v>0</v>
       </c>
       <c r="BE9" s="13"/>
-      <c r="BF9" s="13">
-        <v>80</v>
-      </c>
+      <c r="BF9" s="13"/>
       <c r="BG9" s="13"/>
       <c r="BH9" s="13"/>
-    </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BI9" s="7">
+        <v>80</v>
+      </c>
+      <c r="BP9" s="13"/>
+    </row>
+    <row r="10" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>53</v>
       </c>
@@ -2869,12 +2920,14 @@
       </c>
       <c r="BE10" s="13"/>
       <c r="BF10" s="13"/>
-      <c r="BG10" s="13">
+      <c r="BG10" s="13"/>
+      <c r="BH10" s="13"/>
+      <c r="BJ10" s="7">
         <v>80</v>
       </c>
-      <c r="BH10" s="13"/>
-    </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BP10" s="13"/>
+    </row>
+    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>70</v>
       </c>
@@ -2890,16 +2943,19 @@
       <c r="BB11" s="7">
         <v>0</v>
       </c>
-      <c r="BE11" s="13"/>
+      <c r="BE11" s="13">
+        <v>80</v>
+      </c>
       <c r="BF11" s="13"/>
       <c r="BG11" s="13"/>
-      <c r="BH11" s="13">
-        <v>80</v>
-      </c>
+      <c r="BH11" s="13"/>
       <c r="BI11" s="13"/>
       <c r="BJ11" s="13"/>
-    </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BP11" s="13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>71</v>
       </c>
@@ -2916,15 +2972,18 @@
         <v>0</v>
       </c>
       <c r="BE12" s="13"/>
-      <c r="BF12" s="13"/>
+      <c r="BF12" s="13">
+        <v>80</v>
+      </c>
       <c r="BG12" s="13"/>
       <c r="BH12" s="13"/>
-      <c r="BI12" s="13">
+      <c r="BI12" s="13"/>
+      <c r="BJ12" s="13"/>
+      <c r="BP12" s="13">
         <v>80</v>
       </c>
-      <c r="BJ12" s="13"/>
-    </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>69</v>
       </c>
@@ -2942,14 +3001,17 @@
       </c>
       <c r="BE13" s="13"/>
       <c r="BF13" s="13"/>
-      <c r="BG13" s="13"/>
+      <c r="BG13" s="13">
+        <v>80</v>
+      </c>
       <c r="BH13" s="13"/>
       <c r="BI13" s="13"/>
-      <c r="BJ13" s="13">
+      <c r="BJ13" s="13"/>
+      <c r="BP13" s="13">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
@@ -2969,13 +3031,17 @@
       <c r="BF14" s="13"/>
       <c r="BG14" s="13"/>
       <c r="BH14" s="13"/>
-      <c r="BK14" s="13">
-        <v>90</v>
-      </c>
+      <c r="BK14" s="13"/>
       <c r="BL14" s="13"/>
       <c r="BM14" s="13"/>
-    </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BO14" s="13">
+        <v>90</v>
+      </c>
+      <c r="BP14" s="13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>72</v>
       </c>
@@ -2992,20 +3058,22 @@
         <v>0</v>
       </c>
       <c r="BB15" s="7">
-        <v>0</v>
-      </c>
-      <c r="BC15" s="7">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="BE15" s="13"/>
       <c r="BF15" s="13"/>
       <c r="BG15" s="13"/>
       <c r="BH15" s="13"/>
-      <c r="BK15" s="13"/>
+      <c r="BK15" s="13">
+        <v>90</v>
+      </c>
       <c r="BL15" s="13"/>
       <c r="BM15" s="13"/>
-    </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BP15" s="13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>65</v>
       </c>
@@ -3030,10 +3098,13 @@
         <v>50</v>
       </c>
       <c r="BM16" s="13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="BP16" s="13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
@@ -3196,8 +3267,9 @@
       <c r="BB17" s="14">
         <v>117.42738589211601</v>
       </c>
-    </row>
-    <row r="18" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BP17" s="13"/>
+    </row>
+    <row r="18" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>55</v>
       </c>
@@ -3228,8 +3300,9 @@
       <c r="BB18" s="7">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="19" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BP18" s="13"/>
+    </row>
+    <row r="19" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
@@ -3245,8 +3318,9 @@
       <c r="BB19" s="7">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="20" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BP19" s="13"/>
+    </row>
+    <row r="20" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>57</v>
       </c>
@@ -3265,8 +3339,9 @@
       <c r="BB20" s="7">
         <v>0.153</v>
       </c>
-    </row>
-    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BP20" s="13"/>
+    </row>
+    <row r="21" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>58</v>
       </c>
@@ -3283,8 +3358,9 @@
         <f>1/98 * 100</f>
         <v>1.0204081632653061</v>
       </c>
-    </row>
-    <row r="22" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BP21" s="13"/>
+    </row>
+    <row r="22" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>59</v>
       </c>
@@ -3301,12 +3377,13 @@
         <f>4.5/98 * 100</f>
         <v>4.591836734693878</v>
       </c>
-      <c r="BL22" s="7">
+      <c r="BP22" s="13"/>
+      <c r="BQ22" s="7">
         <f>BB22/2</f>
         <v>2.295918367346939</v>
       </c>
     </row>
-    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>60</v>
       </c>
@@ -3323,12 +3400,13 @@
         <f>10/98 * 100</f>
         <v>10.204081632653061</v>
       </c>
-      <c r="BM23" s="7">
+      <c r="BP23" s="13"/>
+      <c r="BR23" s="7">
         <f>BB23/2</f>
         <v>5.1020408163265305</v>
       </c>
     </row>
-    <row r="24" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>61</v>
       </c>
@@ -3344,8 +3422,9 @@
       <c r="BB24" s="7">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BP24" s="13"/>
+    </row>
+    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>62</v>
       </c>
@@ -3361,8 +3440,9 @@
       <c r="BB25" s="7">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="26" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="BP25" s="13"/>
+    </row>
+    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>63</v>
       </c>
@@ -3402,9 +3482,10 @@
       <c r="BB26" s="7">
         <v>62</v>
       </c>
+      <c r="BP26" s="13"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="382" yWindow="552" count="4">
+  <dataValidations disablePrompts="1" xWindow="382" yWindow="552" count="4">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF7 BC7:BD7">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
@@ -3423,7 +3504,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" xWindow="382" yWindow="552" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>

</xml_diff>

<commit_message>
Add IPT in adults
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="612" windowWidth="16272" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="75">
   <si>
     <t>parameter</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>program_perc_ipt_age5to15</t>
+  </si>
+  <si>
+    <t>program_perc_ipt_age15up</t>
   </si>
 </sst>
 </file>
@@ -2126,18 +2129,18 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="23" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="20"/>
-    <col min="6" max="6" width="13.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="20"/>
+    <col min="1" max="1" width="51.5546875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="23" customWidth="1"/>
+    <col min="3" max="5" width="9.109375" style="20"/>
+    <col min="6" max="6" width="13.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2145,7 +2148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
@@ -2161,7 +2164,7 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>11</v>
       </c>
@@ -2171,7 +2174,7 @@
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>30</v>
       </c>
@@ -2181,7 +2184,7 @@
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
     </row>
-    <row r="5" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>43</v>
       </c>
@@ -2194,7 +2197,7 @@
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
     </row>
-    <row r="6" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>13</v>
       </c>
@@ -2204,7 +2207,7 @@
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>28</v>
       </c>
@@ -2215,7 +2218,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>49</v>
       </c>
@@ -2223,7 +2226,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>59</v>
       </c>
@@ -2232,7 +2235,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
         <v>32</v>
       </c>
@@ -2243,7 +2246,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>33</v>
       </c>
@@ -2254,7 +2257,7 @@
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>34</v>
       </c>
@@ -2265,7 +2268,7 @@
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>35</v>
       </c>
@@ -2276,7 +2279,7 @@
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>36</v>
       </c>
@@ -2287,7 +2290,7 @@
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -2298,7 +2301,7 @@
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
@@ -2306,7 +2309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
@@ -2314,7 +2317,7 @@
         <v>11575186.195826644</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>39</v>
       </c>
@@ -2322,7 +2325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
@@ -2356,47 +2359,47 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BR27"/>
+  <dimension ref="A1:BR28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="BF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BN18" sqref="BN18"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="73.88671875" style="4" customWidth="1"/>
     <col min="2" max="2" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11" style="5" customWidth="1"/>
     <col min="5" max="5" width="11" style="6" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="18" width="7.42578125" style="7" customWidth="1"/>
-    <col min="19" max="24" width="7.28515625" style="7" customWidth="1"/>
-    <col min="25" max="26" width="7.42578125" style="7" customWidth="1"/>
-    <col min="27" max="28" width="7.140625" style="7" customWidth="1"/>
-    <col min="29" max="29" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="33" width="7.42578125" style="7" customWidth="1"/>
-    <col min="34" max="34" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="38" width="7.42578125" style="7" customWidth="1"/>
-    <col min="39" max="39" width="7.5703125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="18" width="7.44140625" style="7" customWidth="1"/>
+    <col min="19" max="24" width="7.33203125" style="7" customWidth="1"/>
+    <col min="25" max="26" width="7.44140625" style="7" customWidth="1"/>
+    <col min="27" max="28" width="7.109375" style="7" customWidth="1"/>
+    <col min="29" max="29" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="33" width="7.44140625" style="7" customWidth="1"/>
+    <col min="34" max="34" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="35" max="38" width="7.44140625" style="7" customWidth="1"/>
+    <col min="39" max="39" width="7.5546875" style="7" customWidth="1"/>
     <col min="40" max="50" width="7" style="7" customWidth="1"/>
-    <col min="51" max="52" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="7.85546875" style="7" customWidth="1"/>
+    <col min="51" max="52" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="7.88671875" style="7" customWidth="1"/>
     <col min="55" max="56" width="14" style="7" customWidth="1"/>
-    <col min="57" max="59" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="60" max="64" width="14.42578125" style="7" customWidth="1"/>
-    <col min="65" max="65" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="57" max="59" width="14.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="60" max="64" width="14.44140625" style="7" customWidth="1"/>
+    <col min="65" max="65" width="14.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="15.44140625" style="7" bestFit="1" customWidth="1"/>
     <col min="67" max="68" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="69" max="70" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="71" max="16384" width="9.140625" style="7"/>
+    <col min="69" max="70" width="15.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="71" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
@@ -2608,7 +2611,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:70" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:70" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -2629,7 +2632,7 @@
       </c>
       <c r="BN2" s="27"/>
     </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -2656,7 +2659,7 @@
       </c>
       <c r="BP3" s="13"/>
     </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
@@ -2679,7 +2682,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -2717,7 +2720,7 @@
       </c>
       <c r="BM5" s="13"/>
     </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -2753,7 +2756,7 @@
       <c r="BB6" s="9"/>
       <c r="BM6" s="13"/>
     </row>
-    <row r="7" spans="1:70" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:70" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
@@ -2781,7 +2784,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
@@ -2809,7 +2812,7 @@
       <c r="BH8" s="13"/>
       <c r="BM8" s="13"/>
     </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>47</v>
       </c>
@@ -2831,7 +2834,7 @@
       <c r="BH9" s="13"/>
       <c r="BM9" s="13"/>
     </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>48</v>
       </c>
@@ -2853,7 +2856,7 @@
       <c r="BH10" s="13"/>
       <c r="BM10" s="13"/>
     </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>65</v>
       </c>
@@ -2881,7 +2884,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>66</v>
       </c>
@@ -2909,7 +2912,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>64</v>
       </c>
@@ -2937,7 +2940,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
@@ -2966,7 +2969,7 @@
       </c>
       <c r="BO14" s="13"/>
     </row>
-    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>67</v>
       </c>
@@ -2996,8 +2999,14 @@
       <c r="BM15" s="13">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BO15" s="7">
+        <v>90</v>
+      </c>
+      <c r="BP15" s="7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>73</v>
       </c>
@@ -3025,10 +3034,16 @@
       <c r="BM16" s="13">
         <v>90</v>
       </c>
-    </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BO16" s="7">
+        <v>90</v>
+      </c>
+      <c r="BP16" s="7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>4</v>
@@ -3042,22 +3057,13 @@
       <c r="BB17" s="7">
         <v>0</v>
       </c>
-      <c r="BE17" s="13"/>
-      <c r="BF17" s="13"/>
-      <c r="BG17" s="13"/>
-      <c r="BH17" s="13"/>
-      <c r="BJ17" s="13">
-        <v>80</v>
-      </c>
-      <c r="BK17" s="13"/>
-      <c r="BM17" s="13">
-        <v>80</v>
-      </c>
-      <c r="BN17" s="13"/>
-    </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BO17" s="7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>4</v>
@@ -3068,164 +3074,28 @@
       <c r="D18" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="6">
-        <v>1</v>
-      </c>
-      <c r="F18" s="14">
-        <v>1</v>
-      </c>
-      <c r="G18" s="14">
-        <v>1.1289570744394</v>
-      </c>
-      <c r="H18" s="14">
-        <v>1.42215881727406</v>
-      </c>
-      <c r="I18" s="14">
-        <v>1.90118931222233</v>
-      </c>
-      <c r="J18" s="14">
-        <v>2.3081073919986701</v>
-      </c>
-      <c r="K18" s="14">
-        <v>2.4974653103104298</v>
-      </c>
-      <c r="L18" s="14">
-        <v>2.9115458645382701</v>
-      </c>
-      <c r="M18" s="14">
-        <v>3.90623450399154</v>
-      </c>
-      <c r="N18" s="14">
-        <v>4.1703507493909102</v>
-      </c>
-      <c r="O18" s="14">
-        <v>4.55399078719985</v>
-      </c>
-      <c r="P18" s="14">
-        <v>5.0047790229916798</v>
-      </c>
-      <c r="Q18" s="14">
-        <v>5.3718558386314896</v>
-      </c>
-      <c r="R18" s="14">
-        <v>6.3137212289735496</v>
-      </c>
-      <c r="S18" s="14">
-        <v>7.4628507238053698</v>
-      </c>
-      <c r="T18" s="14">
-        <v>8.4391855224587609</v>
-      </c>
-      <c r="U18" s="14">
-        <v>9.3018160392078606</v>
-      </c>
-      <c r="V18" s="14">
-        <v>10.2347283365258</v>
-      </c>
-      <c r="W18" s="14">
-        <v>15.386785740408699</v>
-      </c>
-      <c r="X18" s="14">
-        <v>18.9416113416321</v>
-      </c>
-      <c r="Y18" s="14">
-        <v>19.1590871369295</v>
-      </c>
-      <c r="Z18" s="14">
-        <v>19.938817427385899</v>
-      </c>
-      <c r="AA18" s="14">
-        <v>22.702351313969601</v>
-      </c>
-      <c r="AB18" s="14">
-        <v>25.481798063623799</v>
-      </c>
-      <c r="AC18" s="14">
-        <v>28.584806362378998</v>
-      </c>
-      <c r="AD18" s="14">
-        <v>34.090656984785603</v>
-      </c>
-      <c r="AE18" s="14">
-        <v>37.0398409405256</v>
-      </c>
-      <c r="AF18" s="14">
-        <v>39.527551867219898</v>
-      </c>
-      <c r="AG18" s="14">
-        <v>43.633070539419101</v>
-      </c>
-      <c r="AH18" s="14">
-        <v>46.6140802213001</v>
-      </c>
-      <c r="AI18" s="14">
-        <v>50.0989972337483</v>
-      </c>
-      <c r="AJ18" s="14">
-        <v>52.899661134163203</v>
-      </c>
-      <c r="AK18" s="14">
-        <v>57.784910096818798</v>
-      </c>
-      <c r="AL18" s="14">
-        <v>61.2167842323652</v>
-      </c>
-      <c r="AM18" s="14">
-        <v>63.651452282157699</v>
-      </c>
-      <c r="AN18" s="14">
-        <v>67.053941908713696</v>
-      </c>
-      <c r="AO18" s="14">
-        <v>68.8796680497925</v>
-      </c>
-      <c r="AP18" s="14">
-        <v>70.456431535269701</v>
-      </c>
-      <c r="AQ18" s="14">
-        <v>73.858921161825705</v>
-      </c>
-      <c r="AR18" s="14">
-        <v>78.6721991701245</v>
-      </c>
-      <c r="AS18" s="14">
-        <v>82.987551867219906</v>
-      </c>
-      <c r="AT18" s="14">
-        <v>85.394190871369304</v>
-      </c>
-      <c r="AU18" s="14">
-        <v>92.448132780083</v>
-      </c>
-      <c r="AV18" s="14">
-        <v>96.348547717842294</v>
-      </c>
-      <c r="AW18" s="14">
-        <v>100</v>
-      </c>
-      <c r="AX18" s="14">
-        <v>104.647302904564</v>
-      </c>
-      <c r="AY18" s="14">
-        <v>107.966804979253</v>
-      </c>
-      <c r="AZ18" s="14">
-        <v>111.203319502075</v>
-      </c>
-      <c r="BA18" s="14">
-        <v>115.767634854772</v>
-      </c>
-      <c r="BB18" s="14">
-        <v>117.42738589211601</v>
-      </c>
-      <c r="BP18" s="13"/>
-    </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BB18" s="7">
+        <v>0</v>
+      </c>
+      <c r="BE18" s="13"/>
+      <c r="BF18" s="13"/>
+      <c r="BG18" s="13"/>
+      <c r="BH18" s="13"/>
+      <c r="BJ18" s="13">
+        <v>80</v>
+      </c>
+      <c r="BK18" s="13"/>
+      <c r="BM18" s="13">
+        <v>80</v>
+      </c>
+      <c r="BN18" s="13"/>
+    </row>
+    <row r="19" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
@@ -3233,29 +3103,161 @@
       <c r="D19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB19" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK19" s="7">
-        <v>3.1</v>
-      </c>
-      <c r="AP19" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="AU19" s="7">
-        <v>5.2</v>
-      </c>
-      <c r="AZ19" s="7">
-        <v>5.4</v>
-      </c>
-      <c r="BB19" s="7">
-        <v>5.9</v>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+      <c r="F19" s="14">
+        <v>1</v>
+      </c>
+      <c r="G19" s="14">
+        <v>1.1289570744394</v>
+      </c>
+      <c r="H19" s="14">
+        <v>1.42215881727406</v>
+      </c>
+      <c r="I19" s="14">
+        <v>1.90118931222233</v>
+      </c>
+      <c r="J19" s="14">
+        <v>2.3081073919986701</v>
+      </c>
+      <c r="K19" s="14">
+        <v>2.4974653103104298</v>
+      </c>
+      <c r="L19" s="14">
+        <v>2.9115458645382701</v>
+      </c>
+      <c r="M19" s="14">
+        <v>3.90623450399154</v>
+      </c>
+      <c r="N19" s="14">
+        <v>4.1703507493909102</v>
+      </c>
+      <c r="O19" s="14">
+        <v>4.55399078719985</v>
+      </c>
+      <c r="P19" s="14">
+        <v>5.0047790229916798</v>
+      </c>
+      <c r="Q19" s="14">
+        <v>5.3718558386314896</v>
+      </c>
+      <c r="R19" s="14">
+        <v>6.3137212289735496</v>
+      </c>
+      <c r="S19" s="14">
+        <v>7.4628507238053698</v>
+      </c>
+      <c r="T19" s="14">
+        <v>8.4391855224587609</v>
+      </c>
+      <c r="U19" s="14">
+        <v>9.3018160392078606</v>
+      </c>
+      <c r="V19" s="14">
+        <v>10.2347283365258</v>
+      </c>
+      <c r="W19" s="14">
+        <v>15.386785740408699</v>
+      </c>
+      <c r="X19" s="14">
+        <v>18.9416113416321</v>
+      </c>
+      <c r="Y19" s="14">
+        <v>19.1590871369295</v>
+      </c>
+      <c r="Z19" s="14">
+        <v>19.938817427385899</v>
+      </c>
+      <c r="AA19" s="14">
+        <v>22.702351313969601</v>
+      </c>
+      <c r="AB19" s="14">
+        <v>25.481798063623799</v>
+      </c>
+      <c r="AC19" s="14">
+        <v>28.584806362378998</v>
+      </c>
+      <c r="AD19" s="14">
+        <v>34.090656984785603</v>
+      </c>
+      <c r="AE19" s="14">
+        <v>37.0398409405256</v>
+      </c>
+      <c r="AF19" s="14">
+        <v>39.527551867219898</v>
+      </c>
+      <c r="AG19" s="14">
+        <v>43.633070539419101</v>
+      </c>
+      <c r="AH19" s="14">
+        <v>46.6140802213001</v>
+      </c>
+      <c r="AI19" s="14">
+        <v>50.0989972337483</v>
+      </c>
+      <c r="AJ19" s="14">
+        <v>52.899661134163203</v>
+      </c>
+      <c r="AK19" s="14">
+        <v>57.784910096818798</v>
+      </c>
+      <c r="AL19" s="14">
+        <v>61.2167842323652</v>
+      </c>
+      <c r="AM19" s="14">
+        <v>63.651452282157699</v>
+      </c>
+      <c r="AN19" s="14">
+        <v>67.053941908713696</v>
+      </c>
+      <c r="AO19" s="14">
+        <v>68.8796680497925</v>
+      </c>
+      <c r="AP19" s="14">
+        <v>70.456431535269701</v>
+      </c>
+      <c r="AQ19" s="14">
+        <v>73.858921161825705</v>
+      </c>
+      <c r="AR19" s="14">
+        <v>78.6721991701245</v>
+      </c>
+      <c r="AS19" s="14">
+        <v>82.987551867219906</v>
+      </c>
+      <c r="AT19" s="14">
+        <v>85.394190871369304</v>
+      </c>
+      <c r="AU19" s="14">
+        <v>92.448132780083</v>
+      </c>
+      <c r="AV19" s="14">
+        <v>96.348547717842294</v>
+      </c>
+      <c r="AW19" s="14">
+        <v>100</v>
+      </c>
+      <c r="AX19" s="14">
+        <v>104.647302904564</v>
+      </c>
+      <c r="AY19" s="14">
+        <v>107.966804979253</v>
+      </c>
+      <c r="AZ19" s="14">
+        <v>111.203319502075</v>
+      </c>
+      <c r="BA19" s="14">
+        <v>115.767634854772</v>
+      </c>
+      <c r="BB19" s="14">
+        <v>117.42738589211601</v>
       </c>
       <c r="BP19" s="13"/>
     </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>3</v>
@@ -3266,17 +3268,32 @@
       <c r="D20" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="AB20" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="AP20" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AU20" s="7">
+        <v>5.2</v>
+      </c>
+      <c r="AZ20" s="7">
+        <v>5.4</v>
+      </c>
       <c r="BB20" s="7">
-        <v>0.1</v>
+        <v>5.9</v>
       </c>
       <c r="BP20" s="13"/>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" s="5">
         <v>1</v>
@@ -3284,17 +3301,14 @@
       <c r="D21" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AW21" s="7">
-        <v>0.112</v>
-      </c>
       <c r="BB21" s="7">
-        <v>0.153</v>
+        <v>0.1</v>
       </c>
       <c r="BP21" s="13"/>
     </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>4</v>
@@ -3305,85 +3319,88 @@
       <c r="D22" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="AW22" s="7">
+        <v>0.112</v>
+      </c>
       <c r="BB22" s="7">
+        <v>0.153</v>
+      </c>
+      <c r="BP22" s="13"/>
+    </row>
+    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BB23" s="7">
         <f>1/98 * 100</f>
         <v>1.0204081632653061</v>
       </c>
-      <c r="BP22" s="13"/>
-    </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="BP23" s="13"/>
+    </row>
+    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C24" s="5">
         <v>1</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D24" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="BB23" s="7">
+      <c r="BB24" s="7">
         <f>4.5/98 * 100</f>
         <v>4.591836734693878</v>
       </c>
-      <c r="BN23" s="13">
+      <c r="BN24" s="13">
         <v>2.2999999999999998</v>
       </c>
-      <c r="BP23" s="13"/>
-      <c r="BQ23" s="7">
-        <f>BB23/2</f>
+      <c r="BP24" s="13"/>
+      <c r="BQ24" s="7">
+        <f>BB24/2</f>
         <v>2.295918367346939</v>
       </c>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C25" s="5">
         <v>1</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="BB24" s="7">
+      <c r="BB25" s="7">
         <f>10/98 * 100</f>
         <v>10.204081632653061</v>
       </c>
-      <c r="BN24" s="13">
+      <c r="BN25" s="13">
         <v>5.0999999999999996</v>
       </c>
-      <c r="BP24" s="13"/>
-      <c r="BR24" s="7">
-        <f>BB24/2</f>
+      <c r="BP25" s="13"/>
+      <c r="BR25" s="7">
+        <f>BB25/2</f>
         <v>5.1020408163265305</v>
       </c>
     </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    <row r="26" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="5">
-        <v>1</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="BB25" s="7">
-        <v>0.4</v>
-      </c>
-      <c r="BP25" s="13"/>
-    </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>4</v>
@@ -3399,9 +3416,9 @@
       </c>
       <c r="BP26" s="13"/>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>4</v>
@@ -3412,34 +3429,52 @@
       <c r="D27" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="7">
+      <c r="BB27" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="BP27" s="13"/>
+    </row>
+    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="5">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="7">
         <v>0</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G28" s="7">
         <v>30</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I28" s="7">
         <v>50</v>
       </c>
-      <c r="S27" s="7">
+      <c r="S28" s="7">
         <v>50</v>
       </c>
-      <c r="AM27" s="7">
+      <c r="AM28" s="7">
         <v>50</v>
       </c>
-      <c r="AR27" s="7">
+      <c r="AR28" s="7">
         <v>53</v>
       </c>
-      <c r="AW27" s="7">
+      <c r="AW28" s="7">
         <v>55</v>
       </c>
-      <c r="AZ27" s="7">
+      <c r="AZ28" s="7">
         <v>60</v>
       </c>
-      <c r="BB27" s="7">
+      <c r="BB28" s="7">
         <v>62</v>
       </c>
-      <c r="BP27" s="13"/>
+      <c r="BP28" s="13"/>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="4">
@@ -3452,7 +3487,7 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C28 C30:C1048576">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3472,7 +3507,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>D2:D28 D30:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3491,9 +3526,9 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3507,7 +3542,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3518,7 +3553,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Simplify Philippines input sheet
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="74">
   <si>
     <t>parameter</t>
   </si>
@@ -220,12 +220,6 @@
   </si>
   <si>
     <t>scenario_14</t>
-  </si>
-  <si>
-    <t>scenario_16</t>
-  </si>
-  <si>
-    <t>scenario_15</t>
   </si>
   <si>
     <t>program_perc_ipt_age5to15</t>
@@ -340,7 +334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,12 +350,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB9DAED"/>
         <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -1196,14 +1184,13 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1235,56 +1222,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2266,13 +2246,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="23" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="20"/>
-    <col min="6" max="6" width="13.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="20"/>
+    <col min="1" max="1" width="51.5703125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="22" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="19"/>
+    <col min="6" max="6" width="13.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2283,182 +2263,182 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="15">
         <v>9</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="18">
         <v>0.44</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+    </row>
+    <row r="4" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="18">
         <v>0.4</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-    </row>
-    <row r="5" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <v>5</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="16">
         <v>15</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-    </row>
-    <row r="6" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>25800000</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="22">
         <v>4.5999999999999996</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="18">
         <v>1.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="18">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="28">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="34">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="34">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" s="34">
+      <c r="B12" s="28">
         <v>3.8</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="24">
         <v>21</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="24">
         <v>0</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="24">
         <v>265450</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="24">
         <v>3</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17" s="24">
         <v>1</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="24">
         <v>26.24</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2466,15 +2446,15 @@
       <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="26">
+      <c r="B20" s="25">
         <v>11575186.195826644</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="13">
         <v>3</v>
       </c>
     </row>
@@ -2482,22 +2462,22 @@
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="33"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="27"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
+      <c r="B24" s="19"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="20"/>
+      <c r="B25" s="19"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -2525,13 +2505,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BQ28"/>
+  <dimension ref="A1:AH28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2539,298 +2519,185 @@
     <col min="1" max="1" width="73.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" style="5" customWidth="1"/>
     <col min="3" max="3" width="11" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11" style="6" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="17" width="7.42578125" style="7" customWidth="1"/>
-    <col min="18" max="23" width="7.28515625" style="7" customWidth="1"/>
-    <col min="24" max="25" width="7.42578125" style="7" customWidth="1"/>
-    <col min="26" max="27" width="7.140625" style="7" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="32" width="7.42578125" style="7" customWidth="1"/>
-    <col min="33" max="33" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="37" width="7.42578125" style="7" customWidth="1"/>
-    <col min="38" max="38" width="7.5703125" style="7" customWidth="1"/>
-    <col min="39" max="49" width="7" style="7" customWidth="1"/>
-    <col min="50" max="51" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="52" max="53" width="7.85546875" style="7" customWidth="1"/>
-    <col min="54" max="55" width="14" style="7" customWidth="1"/>
-    <col min="56" max="58" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="59" max="63" width="14.42578125" style="7" customWidth="1"/>
-    <col min="64" max="64" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="66" max="67" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="68" max="69" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="70" max="16384" width="9.140625" style="7"/>
+    <col min="4" max="4" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="7.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="6" customWidth="1"/>
+    <col min="9" max="10" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" style="6" customWidth="1"/>
+    <col min="13" max="16" width="7" style="6" customWidth="1"/>
+    <col min="17" max="18" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="7.85546875" style="6" customWidth="1"/>
+    <col min="21" max="22" width="14" style="6" customWidth="1"/>
+    <col min="23" max="25" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="26" max="30" width="14.42578125" style="6" customWidth="1"/>
+    <col min="31" max="31" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="15" style="6" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="2">
-        <v>1920</v>
+        <v>1950</v>
       </c>
       <c r="E1" s="2">
-        <v>1950</v>
+        <v>1960</v>
       </c>
       <c r="F1" s="2">
-        <v>1960</v>
+        <v>1970</v>
       </c>
       <c r="G1" s="2">
-        <v>1965</v>
+        <v>1980</v>
       </c>
       <c r="H1" s="2">
-        <v>1970</v>
+        <v>1989</v>
       </c>
       <c r="I1" s="2">
-        <v>1971</v>
+        <v>1990</v>
       </c>
       <c r="J1" s="2">
-        <v>1972</v>
+        <v>1995</v>
       </c>
       <c r="K1" s="2">
-        <v>1973</v>
+        <v>1998</v>
       </c>
       <c r="L1" s="2">
-        <v>1974</v>
+        <v>2000</v>
       </c>
       <c r="M1" s="2">
-        <v>1975</v>
+        <v>2003</v>
       </c>
       <c r="N1" s="2">
-        <v>1976</v>
+        <v>2005</v>
       </c>
       <c r="O1" s="2">
-        <v>1977</v>
+        <v>2008</v>
       </c>
       <c r="P1" s="2">
-        <v>1978</v>
+        <v>2010</v>
       </c>
       <c r="Q1" s="2">
-        <v>1979</v>
+        <v>2012</v>
       </c>
       <c r="R1" s="2">
-        <v>1980</v>
+        <v>2013</v>
       </c>
       <c r="S1" s="2">
-        <v>1981</v>
+        <v>2014</v>
       </c>
       <c r="T1" s="2">
-        <v>1982</v>
-      </c>
-      <c r="U1" s="2">
-        <v>1983</v>
-      </c>
-      <c r="V1" s="2">
-        <v>1984</v>
-      </c>
-      <c r="W1" s="2">
-        <v>1985</v>
-      </c>
-      <c r="X1" s="2">
-        <v>1986</v>
-      </c>
-      <c r="Y1" s="2">
-        <v>1987</v>
-      </c>
-      <c r="Z1" s="2">
-        <v>1988</v>
-      </c>
-      <c r="AA1" s="2">
-        <v>1989</v>
-      </c>
-      <c r="AB1" s="2">
-        <v>1990</v>
-      </c>
-      <c r="AC1" s="2">
-        <v>1991</v>
-      </c>
-      <c r="AD1" s="2">
-        <v>1992</v>
-      </c>
-      <c r="AE1" s="2">
-        <v>1993</v>
-      </c>
-      <c r="AF1" s="2">
-        <v>1994</v>
-      </c>
-      <c r="AG1" s="2">
-        <v>1995</v>
-      </c>
-      <c r="AH1" s="2">
-        <v>1996</v>
-      </c>
-      <c r="AI1" s="2">
-        <v>1997</v>
-      </c>
-      <c r="AJ1" s="2">
-        <v>1998</v>
-      </c>
-      <c r="AK1" s="2">
-        <v>1999</v>
-      </c>
-      <c r="AL1" s="2">
-        <v>2000</v>
-      </c>
-      <c r="AM1" s="2">
-        <v>2001</v>
-      </c>
-      <c r="AN1" s="2">
-        <v>2002</v>
-      </c>
-      <c r="AO1" s="2">
-        <v>2003</v>
-      </c>
-      <c r="AP1" s="2">
-        <v>2004</v>
-      </c>
-      <c r="AQ1" s="2">
-        <v>2005</v>
-      </c>
-      <c r="AR1" s="2">
-        <v>2006</v>
-      </c>
-      <c r="AS1" s="2">
-        <v>2007</v>
-      </c>
-      <c r="AT1" s="2">
-        <v>2008</v>
-      </c>
-      <c r="AU1" s="2">
-        <v>2009</v>
-      </c>
-      <c r="AV1" s="2">
-        <v>2010</v>
-      </c>
-      <c r="AW1" s="2">
-        <v>2011</v>
-      </c>
-      <c r="AX1" s="2">
-        <v>2012</v>
-      </c>
-      <c r="AY1" s="2">
-        <v>2013</v>
-      </c>
-      <c r="AZ1" s="2">
-        <v>2014</v>
-      </c>
-      <c r="BA1" s="2">
         <v>2015</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="BP1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="BQ1" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <v>0.1</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="BB2" s="27"/>
-      <c r="BC2" s="27"/>
-      <c r="BK2" s="27"/>
-      <c r="BM2" s="27"/>
-      <c r="BO2" s="47"/>
-    </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AF2" s="26"/>
+      <c r="AH2" s="41"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7">
+      <c r="D3" s="6">
         <v>5</v>
       </c>
-      <c r="AL3" s="7">
+      <c r="L3" s="6">
         <v>10</v>
       </c>
-      <c r="AQ3" s="7">
+      <c r="N3" s="6">
         <v>15</v>
       </c>
-      <c r="AV3" s="7">
+      <c r="P3" s="6">
         <v>30</v>
       </c>
-      <c r="BO3" s="48"/>
-    </row>
-    <row r="4" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="AH3" s="42"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BA4" s="7">
+      <c r="T4" s="6">
         <v>0</v>
       </c>
-      <c r="BB4" s="35">
+      <c r="U4" s="29">
         <v>80</v>
       </c>
-      <c r="BL4" s="13"/>
-      <c r="BO4" s="48">
+      <c r="AE4" s="12"/>
+      <c r="AH4" s="42">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
@@ -2840,33 +2707,23 @@
       <c r="C5" s="5">
         <v>0.2</v>
       </c>
-      <c r="AG5" s="8"/>
-      <c r="AH5" s="8"/>
-      <c r="AI5" s="8"/>
-      <c r="AJ5" s="8"/>
-      <c r="AK5" s="8"/>
-      <c r="AL5" s="8"/>
-      <c r="AM5" s="8"/>
-      <c r="AN5" s="8"/>
-      <c r="AO5" s="8"/>
-      <c r="AP5" s="8"/>
-      <c r="AQ5" s="8"/>
-      <c r="AR5" s="8"/>
-      <c r="AS5" s="8"/>
-      <c r="AT5" s="8"/>
-      <c r="AU5" s="8"/>
-      <c r="AV5" s="8"/>
-      <c r="AW5" s="8"/>
-      <c r="AX5" s="8">
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7">
         <v>93</v>
       </c>
-      <c r="AY5" s="8">
+      <c r="R5" s="7">
         <v>85</v>
       </c>
-      <c r="BL5" s="13"/>
-      <c r="BO5" s="48"/>
-    </row>
-    <row r="6" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="AE5" s="12"/>
+      <c r="AH5" s="42"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -2876,665 +2733,544 @@
       <c r="C6" s="5">
         <v>0.2</v>
       </c>
-      <c r="AG6" s="9"/>
-      <c r="AH6" s="8"/>
-      <c r="AI6" s="8"/>
-      <c r="AJ6" s="8"/>
-      <c r="AK6" s="8"/>
-      <c r="AL6" s="9"/>
-      <c r="AM6" s="8"/>
-      <c r="AN6" s="8"/>
-      <c r="AO6" s="8"/>
-      <c r="AP6" s="8"/>
-      <c r="AQ6" s="9"/>
-      <c r="AR6" s="17"/>
-      <c r="AS6" s="9"/>
-      <c r="AT6" s="9"/>
-      <c r="AU6" s="9"/>
-      <c r="AV6" s="9"/>
-      <c r="AW6" s="9"/>
-      <c r="AX6" s="9"/>
-      <c r="AY6" s="9"/>
-      <c r="AZ6" s="9"/>
-      <c r="BA6" s="9"/>
-      <c r="BL6" s="13"/>
-      <c r="BO6" s="48"/>
-    </row>
-    <row r="7" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="8"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="AE6" s="12"/>
+      <c r="AH6" s="42"/>
+    </row>
+    <row r="7" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="1"/>
-      <c r="AV7" s="9">
+      <c r="C7" s="11"/>
+      <c r="P7" s="8">
         <v>0</v>
       </c>
-      <c r="AX7" s="9">
+      <c r="Q7" s="8">
         <v>2.8</v>
       </c>
-      <c r="BC7" s="37">
+      <c r="V7" s="31">
         <v>99</v>
       </c>
-      <c r="BE7" s="27"/>
-      <c r="BL7" s="27"/>
-      <c r="BO7" s="47">
+      <c r="X7" s="26"/>
+      <c r="AE7" s="26"/>
+      <c r="AH7" s="41">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="7">
+      <c r="T8" s="6">
         <v>0</v>
       </c>
-      <c r="AD8" s="7">
-        <v>0</v>
-      </c>
-      <c r="BA8" s="7">
-        <v>0</v>
-      </c>
-      <c r="BD8" s="13"/>
-      <c r="BE8" s="13"/>
-      <c r="BF8" s="13"/>
-      <c r="BG8" s="13"/>
-      <c r="BL8" s="13"/>
-      <c r="BO8" s="48"/>
-    </row>
-    <row r="9" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+      <c r="AE8" s="12"/>
+      <c r="AH8" s="42"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BA9" s="7">
+      <c r="T9" s="6">
         <v>0</v>
       </c>
-      <c r="BD9" s="13"/>
-      <c r="BE9" s="13"/>
-      <c r="BF9" s="13"/>
-      <c r="BG9" s="13"/>
-      <c r="BL9" s="13"/>
-      <c r="BO9" s="48"/>
-    </row>
-    <row r="10" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="12"/>
+      <c r="AE9" s="12"/>
+      <c r="AH9" s="42"/>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BA10" s="7">
+      <c r="T10" s="6">
         <v>0</v>
       </c>
-      <c r="BD10" s="13"/>
-      <c r="BE10" s="13"/>
-      <c r="BF10" s="13"/>
-      <c r="BG10" s="13"/>
-      <c r="BL10" s="13"/>
-      <c r="BO10" s="48"/>
-    </row>
-    <row r="11" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="12"/>
+      <c r="AE10" s="12"/>
+      <c r="AH10" s="42"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BA11" s="7">
+      <c r="T11" s="6">
         <v>0</v>
       </c>
-      <c r="BD11" s="36">
+      <c r="W11" s="30">
         <v>99</v>
       </c>
-      <c r="BE11" s="13"/>
-      <c r="BF11" s="13"/>
-      <c r="BG11" s="13"/>
-      <c r="BH11" s="39">
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="33">
         <v>99</v>
       </c>
-      <c r="BI11" s="40">
+      <c r="AB11" s="34">
         <v>99</v>
       </c>
-      <c r="BL11" s="13"/>
-      <c r="BO11" s="48">
+      <c r="AE11" s="12"/>
+      <c r="AH11" s="42">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>63</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BA12" s="7">
+      <c r="T12" s="6">
         <v>0</v>
       </c>
-      <c r="BD12" s="13"/>
-      <c r="BE12" s="36">
+      <c r="W12" s="12"/>
+      <c r="X12" s="30">
         <v>80</v>
       </c>
-      <c r="BF12" s="13"/>
-      <c r="BG12" s="13"/>
-      <c r="BH12" s="39">
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="33">
         <v>80</v>
       </c>
-      <c r="BI12" s="40">
+      <c r="AB12" s="34">
         <v>80</v>
       </c>
-      <c r="BL12" s="13"/>
-      <c r="BO12" s="48">
+      <c r="AE12" s="12"/>
+      <c r="AH12" s="42">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BA13" s="7">
+      <c r="T13" s="6">
         <v>0</v>
       </c>
-      <c r="BD13" s="13"/>
-      <c r="BE13" s="13"/>
-      <c r="BF13" s="36">
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="30">
         <v>70</v>
       </c>
-      <c r="BG13" s="13"/>
-      <c r="BH13" s="39">
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="33">
         <v>70</v>
       </c>
-      <c r="BI13" s="40">
+      <c r="AB13" s="34">
         <v>70</v>
       </c>
-      <c r="BL13" s="13"/>
-      <c r="BO13" s="48">
+      <c r="AE13" s="12"/>
+      <c r="AH13" s="42">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BA14" s="7">
+      <c r="T14" s="6">
         <v>0</v>
       </c>
-      <c r="BD14" s="13"/>
-      <c r="BE14" s="13"/>
-      <c r="BF14" s="13"/>
-      <c r="BG14" s="13"/>
-      <c r="BI14" s="41"/>
-      <c r="BJ14" s="43">
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
+      <c r="Z14" s="12"/>
+      <c r="AB14" s="35"/>
+      <c r="AC14" s="37">
         <v>90</v>
       </c>
-      <c r="BK14" s="13"/>
-      <c r="BL14" s="13"/>
-      <c r="BN14" s="13"/>
-      <c r="BO14" s="48">
+      <c r="AD14" s="12"/>
+      <c r="AE14" s="12"/>
+      <c r="AG14" s="12"/>
+      <c r="AH14" s="42">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>64</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AV15" s="7">
+      <c r="P15" s="6">
         <v>0</v>
       </c>
-      <c r="BA15" s="7">
+      <c r="T15" s="6">
         <v>14</v>
       </c>
-      <c r="BB15" s="13"/>
-      <c r="BD15" s="13"/>
-      <c r="BE15" s="13"/>
-      <c r="BF15" s="13"/>
-      <c r="BG15" s="13"/>
-      <c r="BI15" s="41"/>
-      <c r="BJ15" s="13"/>
-      <c r="BK15" s="44">
+      <c r="U15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="12"/>
+      <c r="AB15" s="35"/>
+      <c r="AC15" s="12"/>
+      <c r="AD15" s="38">
         <v>90</v>
       </c>
-      <c r="BL15" s="13"/>
-      <c r="BO15" s="48">
+      <c r="AE15" s="12"/>
+      <c r="AH15" s="42">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BA16" s="7">
+      <c r="T16" s="6">
         <v>0</v>
       </c>
-      <c r="BD16" s="13"/>
-      <c r="BE16" s="13"/>
-      <c r="BF16" s="13"/>
-      <c r="BG16" s="13"/>
-      <c r="BH16" s="13"/>
-      <c r="BI16" s="40"/>
-      <c r="BJ16" s="13"/>
-      <c r="BK16" s="13"/>
-      <c r="BL16" s="13"/>
-      <c r="BO16" s="48"/>
-    </row>
-    <row r="17" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="12"/>
+      <c r="AA16" s="12"/>
+      <c r="AB16" s="34"/>
+      <c r="AC16" s="12"/>
+      <c r="AD16" s="12"/>
+      <c r="AE16" s="12"/>
+      <c r="AH16" s="42"/>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BA17" s="7">
+      <c r="T17" s="6">
         <v>0</v>
       </c>
-      <c r="BI17" s="41"/>
-      <c r="BK17" s="13"/>
-      <c r="BL17" s="45">
+      <c r="AB17" s="35"/>
+      <c r="AD17" s="12"/>
+      <c r="AE17" s="39">
         <v>90</v>
       </c>
-      <c r="BO17" s="48">
+      <c r="AH17" s="42">
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BA18" s="7">
+      <c r="T18" s="6">
         <v>0</v>
       </c>
-      <c r="BD18" s="13"/>
-      <c r="BE18" s="13"/>
-      <c r="BF18" s="13"/>
-      <c r="BG18" s="13"/>
-      <c r="BI18" s="41"/>
-      <c r="BJ18" s="13"/>
-      <c r="BL18" s="13"/>
-      <c r="BM18" s="13"/>
-      <c r="BN18" s="46">
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="12"/>
+      <c r="AB18" s="35"/>
+      <c r="AC18" s="12"/>
+      <c r="AE18" s="12"/>
+      <c r="AF18" s="12"/>
+      <c r="AG18" s="40">
         <v>50</v>
       </c>
-      <c r="BO18" s="48">
+      <c r="AH18" s="42">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="1"/>
-      <c r="BA19" s="7">
+      <c r="C19" s="11"/>
+      <c r="T19" s="6">
         <v>0</v>
       </c>
-      <c r="BB19" s="27"/>
-      <c r="BC19" s="27"/>
-      <c r="BE19" s="27"/>
-      <c r="BG19" s="38">
+      <c r="U19" s="26"/>
+      <c r="V19" s="26"/>
+      <c r="X19" s="26"/>
+      <c r="Z19" s="32">
         <v>90</v>
       </c>
-      <c r="BH19" s="27"/>
-      <c r="BI19" s="42">
+      <c r="AA19" s="26"/>
+      <c r="AB19" s="36">
         <v>90</v>
       </c>
-      <c r="BL19" s="27"/>
-      <c r="BO19" s="47">
+      <c r="AE19" s="26"/>
+      <c r="AH19" s="41">
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="13">
         <v>1</v>
       </c>
-      <c r="E20" s="14">
-        <v>1</v>
-      </c>
-      <c r="F20" s="14">
+      <c r="E20" s="13">
         <v>1.1289570744394</v>
       </c>
-      <c r="G20" s="14">
-        <v>1.42215881727406</v>
-      </c>
-      <c r="H20" s="14">
+      <c r="F20" s="13">
         <v>1.90118931222233</v>
       </c>
-      <c r="I20" s="14">
-        <v>2.3081073919986701</v>
-      </c>
-      <c r="J20" s="14">
-        <v>2.4974653103104298</v>
-      </c>
-      <c r="K20" s="14">
-        <v>2.9115458645382701</v>
-      </c>
-      <c r="L20" s="14">
-        <v>3.90623450399154</v>
-      </c>
-      <c r="M20" s="14">
-        <v>4.1703507493909102</v>
-      </c>
-      <c r="N20" s="14">
-        <v>4.55399078719985</v>
-      </c>
-      <c r="O20" s="14">
-        <v>5.0047790229916798</v>
-      </c>
-      <c r="P20" s="14">
-        <v>5.3718558386314896</v>
-      </c>
-      <c r="Q20" s="14">
-        <v>6.3137212289735496</v>
-      </c>
-      <c r="R20" s="14">
+      <c r="G20" s="13">
         <v>7.4628507238053698</v>
       </c>
-      <c r="S20" s="14">
-        <v>8.4391855224587609</v>
-      </c>
-      <c r="T20" s="14">
-        <v>9.3018160392078606</v>
-      </c>
-      <c r="U20" s="14">
-        <v>10.2347283365258</v>
-      </c>
-      <c r="V20" s="14">
-        <v>15.386785740408699</v>
-      </c>
-      <c r="W20" s="14">
-        <v>18.9416113416321</v>
-      </c>
-      <c r="X20" s="14">
-        <v>19.1590871369295</v>
-      </c>
-      <c r="Y20" s="14">
-        <v>19.938817427385899</v>
-      </c>
-      <c r="Z20" s="14">
-        <v>22.702351313969601</v>
-      </c>
-      <c r="AA20" s="14">
+      <c r="H20" s="13">
         <v>25.481798063623799</v>
       </c>
-      <c r="AB20" s="14">
+      <c r="I20" s="13">
         <v>28.584806362378998</v>
       </c>
-      <c r="AC20" s="14">
-        <v>34.090656984785603</v>
-      </c>
-      <c r="AD20" s="14">
-        <v>37.0398409405256</v>
-      </c>
-      <c r="AE20" s="14">
-        <v>39.527551867219898</v>
-      </c>
-      <c r="AF20" s="14">
-        <v>43.633070539419101</v>
-      </c>
-      <c r="AG20" s="14">
+      <c r="J20" s="13">
         <v>46.6140802213001</v>
       </c>
-      <c r="AH20" s="14">
-        <v>50.0989972337483</v>
-      </c>
-      <c r="AI20" s="14">
-        <v>52.899661134163203</v>
-      </c>
-      <c r="AJ20" s="14">
+      <c r="K20" s="13">
         <v>57.784910096818798</v>
       </c>
-      <c r="AK20" s="14">
-        <v>61.2167842323652</v>
-      </c>
-      <c r="AL20" s="14">
+      <c r="L20" s="13">
         <v>63.651452282157699</v>
       </c>
-      <c r="AM20" s="14">
-        <v>67.053941908713696</v>
-      </c>
-      <c r="AN20" s="14">
-        <v>68.8796680497925</v>
-      </c>
-      <c r="AO20" s="14">
+      <c r="M20" s="13">
         <v>70.456431535269701</v>
       </c>
-      <c r="AP20" s="14">
-        <v>73.858921161825705</v>
-      </c>
-      <c r="AQ20" s="14">
+      <c r="N20" s="13">
         <v>78.6721991701245</v>
       </c>
-      <c r="AR20" s="14">
-        <v>82.987551867219906</v>
-      </c>
-      <c r="AS20" s="14">
-        <v>85.394190871369304</v>
-      </c>
-      <c r="AT20" s="14">
+      <c r="O20" s="13">
         <v>92.448132780083</v>
       </c>
-      <c r="AU20" s="14">
-        <v>96.348547717842294</v>
-      </c>
-      <c r="AV20" s="14">
+      <c r="P20" s="13">
         <v>100</v>
       </c>
-      <c r="AW20" s="14">
-        <v>104.647302904564</v>
-      </c>
-      <c r="AX20" s="14">
+      <c r="Q20" s="13">
         <v>107.966804979253</v>
       </c>
-      <c r="AY20" s="14">
+      <c r="R20" s="13">
         <v>111.203319502075</v>
       </c>
-      <c r="AZ20" s="14">
+      <c r="S20" s="13">
         <v>115.767634854772</v>
       </c>
-      <c r="BA20" s="14">
+      <c r="T20" s="13">
         <v>117.42738589211601</v>
       </c>
-      <c r="BO20" s="13"/>
-    </row>
-    <row r="21" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="AH20" s="12"/>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AA21" s="7">
+      <c r="H21" s="6">
         <v>1</v>
       </c>
-      <c r="AJ21" s="7">
+      <c r="K21" s="6">
         <v>3.1</v>
       </c>
-      <c r="AO21" s="7">
+      <c r="M21" s="6">
         <v>4.4000000000000004</v>
       </c>
-      <c r="AT21" s="7">
+      <c r="O21" s="6">
         <v>5.2</v>
       </c>
-      <c r="AY21" s="7">
+      <c r="R21" s="6">
         <v>5.4</v>
       </c>
-      <c r="BA21" s="7">
+      <c r="T21" s="6">
         <v>5.9</v>
       </c>
-      <c r="BO21" s="13"/>
-    </row>
-    <row r="22" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="AH21" s="12"/>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB22" s="7">
+      <c r="I22" s="6">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="AG22" s="7">
+      <c r="J22" s="6">
         <v>2.3E-3</v>
       </c>
-      <c r="AL22" s="7">
+      <c r="L22" s="6">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="AQ22" s="7">
+      <c r="N22" s="6">
         <v>1.24E-2</v>
       </c>
-      <c r="AV22" s="7">
+      <c r="P22" s="6">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="AY22" s="7">
+      <c r="R22" s="6">
         <v>5.6300000000000003E-2</v>
       </c>
-      <c r="AZ22" s="7">
+      <c r="S22" s="6">
         <v>6.6799999999999998E-2</v>
       </c>
-      <c r="BA22" s="7">
+      <c r="T22" s="6">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="BO22" s="13"/>
-    </row>
-    <row r="23" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="AH22" s="12"/>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>51</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AV23" s="7">
+      <c r="P23" s="6">
         <v>0.112</v>
       </c>
-      <c r="BA23" s="7">
+      <c r="T23" s="6">
         <v>0.153</v>
       </c>
-      <c r="BO23" s="13"/>
-    </row>
-    <row r="24" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="AH23" s="12"/>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BA24" s="7">
+      <c r="T24" s="6">
         <v>14</v>
       </c>
-      <c r="BO24" s="13"/>
-    </row>
-    <row r="25" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="AH24" s="12"/>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BA25" s="7">
+      <c r="T25" s="6">
         <v>21</v>
       </c>
-      <c r="BM25" s="49">
+      <c r="AF25" s="43">
         <v>10.5</v>
       </c>
-      <c r="BO25" s="13"/>
-    </row>
-    <row r="26" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="AH25" s="12"/>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BA26" s="7">
+      <c r="T26" s="6">
         <v>21</v>
       </c>
-      <c r="BM26" s="49">
+      <c r="AF26" s="43">
         <v>10.5</v>
       </c>
-      <c r="BO26" s="13"/>
-    </row>
-    <row r="27" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="AH26" s="12"/>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="7">
+      <c r="D27" s="6">
         <v>0</v>
       </c>
-      <c r="F27" s="7">
+      <c r="E27" s="6">
         <v>30</v>
       </c>
-      <c r="H27" s="7">
+      <c r="F27" s="6">
         <v>50</v>
       </c>
-      <c r="R27" s="7">
+      <c r="G27" s="6">
         <v>50</v>
       </c>
-      <c r="AL27" s="7">
+      <c r="L27" s="6">
         <v>50</v>
       </c>
-      <c r="AQ27" s="7">
+      <c r="N27" s="6">
         <v>53</v>
       </c>
-      <c r="AV27" s="7">
+      <c r="P27" s="6">
         <v>55</v>
       </c>
-      <c r="AY27" s="7">
+      <c r="R27" s="6">
         <v>60</v>
       </c>
-      <c r="BA27" s="7">
+      <c r="T27" s="6">
         <v>62</v>
       </c>
-      <c r="BO27" s="13"/>
-    </row>
-    <row r="28" spans="1:67" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="30"/>
-      <c r="BE28" s="32"/>
-      <c r="BF28" s="32"/>
-      <c r="BG28" s="32"/>
-      <c r="BH28" s="32"/>
-      <c r="BI28" s="32"/>
-      <c r="BJ28" s="32"/>
-      <c r="BK28" s="32"/>
-      <c r="BL28" s="32"/>
-      <c r="BM28" s="32"/>
-      <c r="BN28" s="32"/>
-      <c r="BO28" s="32"/>
+      <c r="AH27" s="12"/>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="X28" s="12"/>
+      <c r="Y28" s="12"/>
+      <c r="Z28" s="12"/>
+      <c r="AA28" s="12"/>
+      <c r="AB28" s="12"/>
+      <c r="AC28" s="12"/>
+      <c r="AD28" s="12"/>
+      <c r="AE28" s="12"/>
+      <c r="AF28" s="12"/>
+      <c r="AG28" s="12"/>
+      <c r="AH28" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Make time to treatment constant
Haven't been varying it in any models so far, so rate of transition from diagnosis to treatment commencement might as well be calculated from constant parameters.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_philippines.xlsx
+++ b/autumn/xls/data_philippines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2234,8 +2234,8 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2501,7 +2501,7 @@
   </sheetPr>
   <dimension ref="A1:AH28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>